<commit_message>
add MoCo - w/o distributed yet
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C14883EF-DB1D-D04D-8324-F4277D9B62F2}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{581029E3-E53B-6344-AD94-A6AF2F78E2E5}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="2420" windowWidth="30240" windowHeight="8640" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-31860" yWindow="6480" windowWidth="35060" windowHeight="17360" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,9 +484,10 @@
     <col min="7" max="7" width="16.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="3"/>
+    <col min="10" max="10" width="15.33203125" style="3" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="35" width="10.83203125" style="8"/>
+    <col min="12" max="12" width="21" style="8" customWidth="1"/>
+    <col min="13" max="35" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -741,6 +742,9 @@
       <c r="E6" s="3">
         <v>128</v>
       </c>
+      <c r="F6" s="3">
+        <v>16</v>
+      </c>
       <c r="G6" s="3" t="b">
         <v>0</v>
       </c>
@@ -749,6 +753,15 @@
       </c>
       <c r="I6" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.66279999999999994</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.58640000000000003</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.59770000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add output record into checkpoints
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{581029E3-E53B-6344-AD94-A6AF2F78E2E5}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50EF0A9B-9C54-A347-AED7-FDB3D3D0D630}"/>
   <bookViews>
-    <workbookView xWindow="-31860" yWindow="6480" windowWidth="35060" windowHeight="17360" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="0" yWindow="2420" windowWidth="30240" windowHeight="8640" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
+    <sheet name="MoCo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -77,6 +78,15 @@
   </si>
   <si>
     <t>Biased_sampling</t>
+  </si>
+  <si>
+    <t>MoCo</t>
+  </si>
+  <si>
+    <t>Number of GPUs</t>
+  </si>
+  <si>
+    <t>the loss flucuates a lot, but stay at a low value for a long time, let's say the best is iter 6 for now</t>
   </si>
 </sst>
 </file>
@@ -133,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -155,6 +165,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,4 +783,125 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
+  <dimension ref="A1:AI3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="29" style="10" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="19" style="10" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="17.5" style="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>8544579</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10">
+        <v>64</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>8548727</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="10">
+        <v>64</v>
+      </c>
+      <c r="F3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove softmax before cross entropy
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -1014,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add validation while training.
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E61E4C30-D4FB-664C-A499-3B23E9D040FE}"/>
+  <xr:revisionPtr revIDLastSave="382" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3DE84AD-5A62-944B-A4F2-3368ED5BFE72}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="760" windowWidth="25540" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="3040" yWindow="760" windowWidth="25540" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -147,7 +147,31 @@
     <t>converge to trivial solution</t>
   </si>
   <si>
-    <t>increase memsize to 12800</t>
+    <t>increase memsize to 12800, did not converge</t>
+  </si>
+  <si>
+    <t>to see if the MoCo loss still converge (was worried I changed something accidentally)</t>
+  </si>
+  <si>
+    <t>training loss keep fluctuating…</t>
+  </si>
+  <si>
+    <t>update loss</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>training without augmentation</t>
+  </si>
+  <si>
+    <t>loss decreases then flutuate, but still decreasing</t>
+  </si>
+  <si>
+    <t>0.03 might be better</t>
+  </si>
+  <si>
+    <t>havn't converge, should increase the number of epoch</t>
   </si>
 </sst>
 </file>
@@ -163,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +197,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,10 +260,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,7 +586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView zoomScale="157" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="157" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -849,10 +885,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView zoomScale="180" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="180" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,8 +900,8 @@
     <col min="5" max="5" width="17.6640625" style="10" customWidth="1"/>
     <col min="6" max="6" width="29" style="10" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="16" customWidth="1"/>
     <col min="10" max="10" width="19" style="10" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" style="10" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="10" customWidth="1"/>
@@ -893,10 +929,10 @@
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -922,106 +958,123 @@
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+    <row r="2" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
         <v>8544579</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="12">
         <v>0.03</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="10">
+      <c r="D2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="12">
         <v>64</v>
       </c>
-      <c r="F2" s="10">
-        <v>1</v>
-      </c>
-      <c r="G2" s="10">
+      <c r="F2" s="12">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12">
         <v>50</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="I2" s="15"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
         <v>8548727</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="12">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12">
         <v>64</v>
       </c>
-      <c r="F3" s="10">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10">
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
         <v>8618521</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="12">
         <v>0.03</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="10">
-        <v>128</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="D4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="12">
+        <v>128</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12">
         <v>50</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="I4" s="15"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
         <v>8630046</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="12">
         <v>0.03</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="10">
-        <v>128</v>
-      </c>
-      <c r="F5" s="10">
-        <v>1</v>
-      </c>
-      <c r="G5" s="10">
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="12">
+        <v>128</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12">
         <v>100</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="15" t="s">
         <v>19</v>
       </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
@@ -1045,7 +1098,7 @@
       <c r="G6" s="10">
         <v>100</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1094,12 +1147,301 @@
       <c r="G8" s="10">
         <v>100</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="16" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>8704666</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="10">
+        <v>128</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>8714665</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="12">
+        <v>128</v>
+      </c>
+      <c r="F10" s="12">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12">
+        <v>100</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+    </row>
+    <row r="11" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>8714947</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="12">
+        <v>128</v>
+      </c>
+      <c r="F11" s="12">
+        <v>1</v>
+      </c>
+      <c r="G11" s="12">
+        <v>100</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>8715114</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="10">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="10">
+        <v>128</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>8719970</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="10">
+        <v>30</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="10">
+        <v>128</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
+      </c>
+      <c r="G13" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>8725293</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="10">
+        <v>128</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
+      </c>
+      <c r="G14" s="10">
+        <v>100</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>8727149</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="10">
+        <v>128</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="10">
+        <v>100</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>8733913</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="10">
+        <v>128</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
+      </c>
+      <c r="G16" s="10">
+        <v>100</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>8735495</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="10">
+        <v>128</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
+      </c>
+      <c r="G17" s="10">
+        <v>100</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>8736656</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>128</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="10">
+        <v>100</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>8741212</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="10">
+        <v>128</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
+      </c>
+      <c r="G19" s="10">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1107,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="181" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,8 +1554,8 @@
       <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1240,10 +1582,10 @@
       <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>0.6</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>0.42</v>
       </c>
       <c r="L3" t="s">

</xml_diff>

<commit_message>
remove color jitter from MoCoLabelDataset as it is too difficult for MoCo to learn from.
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="382" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3DE84AD-5A62-944B-A4F2-3368ED5BFE72}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAFCBF59-3CBF-D246-99DD-333B856C32CE}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="760" windowWidth="25540" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="4080" yWindow="2460" windowWidth="25540" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="79">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -172,6 +172,108 @@
   </si>
   <si>
     <t>havn't converge, should increase the number of epoch</t>
+  </si>
+  <si>
+    <t>not sure when to stop</t>
+  </si>
+  <si>
+    <t>need to add validation when training</t>
+  </si>
+  <si>
+    <t>failed because of GPU RAM issues</t>
+  </si>
+  <si>
+    <t>reduce the batch size for validation and lets see</t>
+  </si>
+  <si>
+    <t>lowest validation 70</t>
+  </si>
+  <si>
+    <t>8751286_70</t>
+  </si>
+  <si>
+    <t>moving very slowly, increase lr</t>
+  </si>
+  <si>
+    <t>the learned features are garbage based on the classification performance</t>
+  </si>
+  <si>
+    <t>should put some augmentation back</t>
+  </si>
+  <si>
+    <t>converge to a trivial solution</t>
+  </si>
+  <si>
+    <t>put back everything</t>
+  </si>
+  <si>
+    <t>put back everything but Gaussian blur</t>
+  </si>
+  <si>
+    <t>same as above</t>
+  </si>
+  <si>
+    <t>put back everything but Gaussian blur or colar gitter</t>
+  </si>
+  <si>
+    <t>put back everything but Gaussian blur or grey scale</t>
+  </si>
+  <si>
+    <t>put back everything but Gaussian blur or grey scale or colar gitter</t>
+  </si>
+  <si>
+    <t>put back everything but grey scale or color jitter</t>
+  </si>
+  <si>
+    <t>8763825_160</t>
+  </si>
+  <si>
+    <t>8763825_290</t>
+  </si>
+  <si>
+    <t>garbage</t>
+  </si>
+  <si>
+    <t>fixed vali</t>
+  </si>
+  <si>
+    <t>that’s because no aug is applied to vali</t>
+  </si>
+  <si>
+    <t>add aug to vali</t>
+  </si>
+  <si>
+    <t>forget to add normalization to aug dataset</t>
+  </si>
+  <si>
+    <t>add normalization to aug, use non-aug vali</t>
+  </si>
+  <si>
+    <t>didn’t converge</t>
+  </si>
+  <si>
+    <t>should increase ne</t>
+  </si>
+  <si>
+    <t>put back everything but color jitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incrase ne to 500 </t>
+  </si>
+  <si>
+    <t>increase ne to 100</t>
+  </si>
+  <si>
+    <t>lr too large</t>
+  </si>
+  <si>
+    <t>increase lr to 0.3</t>
+  </si>
+  <si>
+    <t>try earlier models</t>
+  </si>
+  <si>
+    <t>may be try higher # of epoch for training LabelMoCo</t>
   </si>
 </sst>
 </file>
@@ -234,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,6 +372,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -885,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI19"/>
+  <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView zoomScale="180" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,7 +1470,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>8735495</v>
       </c>
@@ -1390,7 +1496,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>8736656</v>
       </c>
@@ -1416,7 +1522,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>8741212</v>
       </c>
@@ -1436,7 +1542,288 @@
         <v>1</v>
       </c>
       <c r="G19" s="10">
-        <v>100</v>
+        <v>300</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="10">
+        <v>128</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
+      </c>
+      <c r="G20" s="10">
+        <v>300</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>8751286</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="10">
+        <v>128</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1</v>
+      </c>
+      <c r="G21" s="10">
+        <v>300</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>8760687</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="10">
+        <v>128</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
+      </c>
+      <c r="G22" s="10">
+        <v>300</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>8761020</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="10">
+        <v>128</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
+      </c>
+      <c r="G23" s="10">
+        <v>300</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>8763825</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="10">
+        <v>128</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="10">
+        <v>300</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>8763833</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="10">
+        <v>128</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
+      </c>
+      <c r="G25" s="10">
+        <v>300</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>8763845</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="10">
+        <v>128</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
+      </c>
+      <c r="G26" s="10">
+        <v>300</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>8764388</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="10">
+        <v>128</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
+      </c>
+      <c r="G27" s="10">
+        <v>300</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>8775747</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="10">
+        <v>128</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+      <c r="G28" s="10">
+        <v>300</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>8776341</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="10">
+        <v>128</v>
+      </c>
+      <c r="F29" s="10">
+        <v>1</v>
+      </c>
+      <c r="G29" s="10">
+        <v>300</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1447,15 +1834,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AI21"/>
   <sheetViews>
-    <sheetView zoomScale="181" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="181" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
@@ -1734,6 +2121,431 @@
         <v>33</v>
       </c>
     </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8757293</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>128</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8757377</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>128</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8773343</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8773369</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>0.3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>128</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>8773429</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>128</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8773428</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>0.3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>128</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>8773794</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>0.3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" t="s">
+        <v>70</v>
+      </c>
+      <c r="O15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8773772</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>0.3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>128</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N16" t="s">
+        <v>70</v>
+      </c>
+      <c r="O16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8775647</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>128</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8775648</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>0.3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>128</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>8775782</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>0.03</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19">
+        <v>28</v>
+      </c>
+      <c r="K19" s="18">
+        <v>0.64810000000000001</v>
+      </c>
+      <c r="L19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8775783</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>0.03</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>128</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20">
+        <v>46</v>
+      </c>
+      <c r="K20" s="18">
+        <v>0.64690000000000003</v>
+      </c>
+      <c r="L20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8776347</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>0.03</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>128</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add .item() in metric calculation
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="559" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AED4CAB-3987-B542-8C82-02164ECF862D}"/>
+  <xr:revisionPtr revIDLastSave="576" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CF465E6-5C8E-4844-A49F-8BA36EBC620C}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="1080" windowWidth="25540" windowHeight="14220" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="5580" yWindow="6480" windowWidth="25540" windowHeight="14220" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="80">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -339,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,6 +379,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="157" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -987,63 +994,231 @@
         <v>0.59770000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
         <v>8777104</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="19">
         <v>1E-3</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="3">
-        <v>128</v>
-      </c>
-      <c r="F7" s="3">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3" t="b">
+      <c r="D7" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="19">
+        <v>128</v>
+      </c>
+      <c r="F7" s="19">
+        <v>5</v>
+      </c>
+      <c r="G7" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3" t="b">
+      <c r="H7" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20">
+        <v>0.65490000000000004</v>
+      </c>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
+      <c r="AC7" s="21"/>
+      <c r="AD7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AF7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AH7" s="21"/>
+      <c r="AI7" s="21"/>
+    </row>
+    <row r="8" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
         <v>8777107</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="19">
         <v>1E-3</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3">
-        <v>128</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="D8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="19">
+        <v>128</v>
+      </c>
+      <c r="F8" s="19">
         <v>38</v>
       </c>
-      <c r="G8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3" t="b">
+      <c r="G8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="19" t="b">
         <v>0</v>
       </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20">
+        <v>0.59240000000000004</v>
+      </c>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+      <c r="AF8" s="21"/>
+      <c r="AG8" s="21"/>
+      <c r="AH8" s="21"/>
+      <c r="AI8" s="21"/>
+    </row>
+    <row r="9" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="19">
+        <v>8780600</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="19">
+        <v>128</v>
+      </c>
+      <c r="F9" s="19">
+        <v>3</v>
+      </c>
+      <c r="G9" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="20">
+        <v>0.63429999999999997</v>
+      </c>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="21"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="21"/>
+      <c r="AD9" s="21"/>
+      <c r="AE9" s="21"/>
+      <c r="AF9" s="21"/>
+      <c r="AG9" s="21"/>
+      <c r="AH9" s="21"/>
+      <c r="AI9" s="21"/>
+    </row>
+    <row r="10" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
+        <v>8782406</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="19">
+        <v>128</v>
+      </c>
+      <c r="F10" s="19">
+        <v>3</v>
+      </c>
+      <c r="G10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+      <c r="AF10" s="21"/>
+      <c r="AG10" s="21"/>
+      <c r="AH10" s="21"/>
+      <c r="AI10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1897,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI21"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="181" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="H10" zoomScale="181" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2603,6 +2778,9 @@
       <c r="H21" t="s">
         <v>29</v>
       </c>
+      <c r="I21">
+        <v>24</v>
+      </c>
       <c r="L21" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
add batchnormalization in MoCoClfV2
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="615" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EA6E9CD-CA50-8E4D-A08A-2F73580758B9}"/>
+  <xr:revisionPtr revIDLastSave="616" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4794B04D-66CF-CA46-B3EE-DFD2B1320960}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="6480" windowWidth="25540" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -2129,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="181" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="181" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>8783948</v>
+        <v>8784007</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
add side feature to res50_fc
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="650" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDC660C7-8074-BC47-92B9-AD4A00810978}"/>
+  <xr:revisionPtr revIDLastSave="673" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44F2EBDF-B497-F14B-941D-3C64737FA5C1}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="1320" windowWidth="43080" windowHeight="14220" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="91">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>too slow, increase lr</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-16-16(with speed and n lanes)-4</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-16-16(with road type and cyc infras)-4</t>
   </si>
 </sst>
 </file>
@@ -727,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
-  <dimension ref="A1:AI16"/>
+  <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="157" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1439,6 +1445,122 @@
       </c>
       <c r="I16" s="19" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>8836387</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="19">
+        <v>128</v>
+      </c>
+      <c r="F17" s="19">
+        <v>3</v>
+      </c>
+      <c r="G17" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>8836388</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="19">
+        <v>128</v>
+      </c>
+      <c r="F18" s="19">
+        <v>3</v>
+      </c>
+      <c r="G18" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>8836393</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19">
+        <v>128</v>
+      </c>
+      <c r="F19" s="19">
+        <v>3</v>
+      </c>
+      <c r="G19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>8836394</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="19">
+        <v>128</v>
+      </c>
+      <c r="F20" s="19">
+        <v>3</v>
+      </c>
+      <c r="G20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="19" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add side feature to MoCo_clf
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="673" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44F2EBDF-B497-F14B-941D-3C64737FA5C1}"/>
+  <xr:revisionPtr revIDLastSave="689" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BE7FEC6-64AC-5A41-AF1F-441B82C719CB}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1320" windowWidth="43080" windowHeight="14220" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="4560" yWindow="1320" windowWidth="43080" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="93">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -310,13 +310,19 @@
   </si>
   <si>
     <t>Res50-noFC-100-16-16(with road type and cyc infras)-4</t>
+  </si>
+  <si>
+    <t>MoCoClfV2Fea + n lanes + speed</t>
+  </si>
+  <si>
+    <t>MoCoClfV2Fea + road type + cyc infras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -324,8 +330,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +355,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -372,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,6 +438,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="157" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="157" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1572,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI32"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView zoomScale="180" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2488,10 +2508,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI24"/>
+  <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="181" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="181" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3290,6 +3310,110 @@
         <v>29</v>
       </c>
     </row>
+    <row r="25" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
+        <v>8836483</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="13">
+        <v>128</v>
+      </c>
+      <c r="F25" s="13">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13">
+        <v>100</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
+        <v>8836482</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="13">
+        <v>128</v>
+      </c>
+      <c r="F26" s="13">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13">
+        <v>100</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13">
+        <v>8836484</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="13">
+        <v>128</v>
+      </c>
+      <c r="F27" s="13">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13">
+        <v>100</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22">
+        <v>8836485</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="13">
+        <v>128</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1</v>
+      </c>
+      <c r="G28" s="13">
+        <v>100</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add exp and rec weighting options
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="853" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{581E67FF-F113-334A-BB20-1919789F0043}"/>
+  <xr:revisionPtr revIDLastSave="896" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA92C975-7A49-3F4D-99D2-816D08F15B41}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1320" windowWidth="43080" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="4560" yWindow="1320" windowWidth="43080" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="100">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Res50-noFC-100-4</t>
   </si>
   <si>
-    <t>OrdLabelMoCo (alpha=2)</t>
-  </si>
-  <si>
     <t>8775747_480</t>
   </si>
   <si>
@@ -325,6 +322,21 @@
   </si>
   <si>
     <t>MoCoCLfV2</t>
+  </si>
+  <si>
+    <t>OrdLabelMoCo (alpha=1, exp)</t>
+  </si>
+  <si>
+    <t>lost track</t>
+  </si>
+  <si>
+    <t>8782858_480</t>
+  </si>
+  <si>
+    <t>OrdLabelMoCo (alpha=2, ratio)</t>
+  </si>
+  <si>
+    <t>wrong spec, descarded</t>
   </si>
 </sst>
 </file>
@@ -784,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="157" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A7" zoomScale="157" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,7 +1321,7 @@
         <v>8834025</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="19">
         <v>1E-3</v>
@@ -1338,7 +1350,7 @@
         <v>0.56310000000000004</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
@@ -1346,7 +1358,7 @@
         <v>8834107</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="19">
         <v>1E-3</v>
@@ -1372,10 +1384,10 @@
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
       <c r="M12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
@@ -1383,7 +1395,7 @@
         <v>8834107</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="19">
         <v>0.01</v>
@@ -1414,7 +1426,7 @@
         <v>8835249</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="19">
         <v>0.01</v>
@@ -1443,7 +1455,7 @@
         <v>8835250</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="19">
         <v>0.01</v>
@@ -1472,7 +1484,7 @@
         <v>8835261</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="19">
         <v>0.01</v>
@@ -1501,7 +1513,7 @@
         <v>8836387</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C17" s="19">
         <v>0.01</v>
@@ -1533,7 +1545,7 @@
         <v>8836388</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="19">
         <v>0.01</v>
@@ -1560,7 +1572,7 @@
         <v>0.79600000000000004</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
@@ -1568,7 +1580,7 @@
         <v>8836393</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="19">
         <v>0.01</v>
@@ -1592,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.2">
@@ -1600,7 +1612,7 @@
         <v>8836394</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="19">
         <v>0.01</v>
@@ -1629,7 +1641,7 @@
         <v>8837237</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="24">
         <v>0.01</v>
@@ -1684,7 +1696,7 @@
         <v>8837239</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="24">
         <v>0.01</v>
@@ -1741,16 +1753,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI32"/>
+  <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="180" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="10" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" style="10" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="10" customWidth="1"/>
@@ -2581,7 +2593,7 @@
         <v>8782858</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C30" s="10">
         <v>0.3</v>
@@ -2599,7 +2611,7 @@
         <v>500</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -2607,7 +2619,7 @@
         <v>8783455</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C31" s="10">
         <v>0.03</v>
@@ -2625,7 +2637,7 @@
         <v>500</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -2633,7 +2645,7 @@
         <v>8786623</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C32" s="10">
         <v>3</v>
@@ -2648,6 +2660,107 @@
         <v>1</v>
       </c>
       <c r="G32" s="10">
+        <v>500</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>8850812</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="10">
+        <v>128</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
+      </c>
+      <c r="G33" s="10">
+        <v>500</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
+        <v>8850814</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="10">
+        <v>3</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="10">
+        <v>128</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
+      </c>
+      <c r="G34" s="10">
+        <v>500</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>8852324</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="10">
+        <v>128</v>
+      </c>
+      <c r="F35" s="10">
+        <v>1</v>
+      </c>
+      <c r="G35" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>8852325</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="10">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="10">
+        <v>128</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
+      </c>
+      <c r="G36" s="10">
         <v>500</v>
       </c>
     </row>
@@ -2659,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="181" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A25" zoomScale="181" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3401,7 +3514,7 @@
         <v>100</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I22">
         <v>4</v>
@@ -3415,7 +3528,7 @@
         <v>8784006</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23">
         <v>0.03</v>
@@ -3441,7 +3554,7 @@
         <v>8784007</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24">
         <v>0.03</v>
@@ -3467,7 +3580,7 @@
         <v>8836483</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="13">
         <v>0.03</v>
@@ -3494,7 +3607,7 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -3502,7 +3615,7 @@
         <v>8836482</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="13">
         <v>0.03</v>
@@ -3534,7 +3647,7 @@
         <v>8836484</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="13">
         <v>0.03</v>
@@ -3566,7 +3679,7 @@
         <v>8836485</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="13">
         <v>0.03</v>
@@ -3598,7 +3711,7 @@
         <v>8837319</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" s="26">
         <v>0.03</v>
@@ -3630,7 +3743,7 @@
         <v>8837321</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="26">
         <v>0.03</v>
@@ -3662,7 +3775,7 @@
         <v>8837322</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="26">
         <v>0.03</v>
@@ -3694,7 +3807,7 @@
         <v>8837323</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="26">
         <v>0.03</v>
@@ -3721,12 +3834,12 @@
         <v>0.70130000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27">
         <v>8838183</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="27">
         <v>0.01</v>
@@ -3747,12 +3860,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <v>8838185</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="27">
         <v>0.01</v>
@@ -3771,6 +3884,93 @@
       </c>
       <c r="H34" s="27" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="26">
+        <v>8851279</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="26">
+        <v>128</v>
+      </c>
+      <c r="F35" s="26">
+        <v>1</v>
+      </c>
+      <c r="G35" s="26">
+        <v>200</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" s="26">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="26">
+        <v>8851280</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="26">
+        <v>128</v>
+      </c>
+      <c r="F36" s="26">
+        <v>1</v>
+      </c>
+      <c r="G36" s="26">
+        <v>200</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I36" s="26">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="26">
+        <v>8851281</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D37" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="26">
+        <v>128</v>
+      </c>
+      <c r="F37" s="26">
+        <v>1</v>
+      </c>
+      <c r="G37" s="26">
+        <v>200</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="I37" s="26">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add output dimension option to models so that we can use it for arttribute prediction
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="896" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA92C975-7A49-3F4D-99D2-816D08F15B41}"/>
+  <xr:revisionPtr revIDLastSave="958" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C478F84-2444-3543-A01C-5986EC36A434}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1320" windowWidth="43080" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-38860" yWindow="6820" windowWidth="43080" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="103">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>wrong spec, descarded</t>
+  </si>
+  <si>
+    <t>OrdLabelMoCo (alpha=2, ratio, start from 8782858_480)</t>
+  </si>
+  <si>
+    <t>8852525_580</t>
+  </si>
+  <si>
+    <t>8852525_640</t>
   </si>
 </sst>
 </file>
@@ -1753,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI36"/>
+  <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A27" zoomScale="180" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2764,6 +2773,29 @@
         <v>500</v>
       </c>
     </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
+        <v>8852525</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="10">
+        <v>3</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="10">
+        <v>128</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1</v>
+      </c>
+      <c r="G37" s="10">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2772,10 +2804,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI37"/>
+  <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="181" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="181" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3834,7 +3866,7 @@
         <v>0.70130000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="27">
         <v>8838183</v>
       </c>
@@ -3860,7 +3892,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <v>8838185</v>
       </c>
@@ -3886,7 +3918,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="26">
         <v>8851279</v>
       </c>
@@ -3914,8 +3946,11 @@
       <c r="I35" s="26">
         <v>84</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K35" s="18">
+        <v>0.69669999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="26">
         <v>8851280</v>
       </c>
@@ -3943,8 +3978,11 @@
       <c r="I36" s="26">
         <v>184</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K36" s="28">
+        <v>0.80059999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="26">
         <v>8851281</v>
       </c>
@@ -3972,6 +4010,117 @@
       <c r="I37" s="26">
         <v>194</v>
       </c>
+      <c r="K37" s="28">
+        <v>0.63029999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="26">
+        <v>8855877</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="26">
+        <v>128</v>
+      </c>
+      <c r="F38" s="26">
+        <v>1</v>
+      </c>
+      <c r="G38" s="26">
+        <v>200</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="I38" s="26"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="26">
+        <v>8855878</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="26">
+        <v>128</v>
+      </c>
+      <c r="F39" s="26">
+        <v>1</v>
+      </c>
+      <c r="G39" s="26">
+        <v>200</v>
+      </c>
+      <c r="H39" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I39" s="26"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="26">
+        <v>8855876</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="26">
+        <v>128</v>
+      </c>
+      <c r="F40" s="26">
+        <v>1</v>
+      </c>
+      <c r="G40" s="26">
+        <v>200</v>
+      </c>
+      <c r="H40" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="I40" s="26"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="26">
+        <v>8855875</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="26">
+        <v>128</v>
+      </c>
+      <c r="F41" s="26">
+        <v>1</v>
+      </c>
+      <c r="G41" s="26">
+        <v>200</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I41" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add label option to the streetview dataset so that it can output speed label and optentially others as well.
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="958" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C478F84-2444-3543-A01C-5986EC36A434}"/>
+  <xr:revisionPtr revIDLastSave="1012" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51DD0092-C676-4E4F-8646-727B628E2272}"/>
   <bookViews>
-    <workbookView xWindow="-38860" yWindow="6820" windowWidth="43080" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-38860" yWindow="6820" windowWidth="43080" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
-    <sheet name="MoCo" sheetId="2" r:id="rId2"/>
-    <sheet name="MoCoClf" sheetId="3" r:id="rId3"/>
+    <sheet name="Res50FC_speed" sheetId="4" r:id="rId2"/>
+    <sheet name="MoCo" sheetId="2" r:id="rId3"/>
+    <sheet name="MoCoClf" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="106">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -346,6 +347,15 @@
   </si>
   <si>
     <t>8852525_640</t>
+  </si>
+  <si>
+    <t>Res50FC (for speed)</t>
+  </si>
+  <si>
+    <t>fluctuating validation loss</t>
+  </si>
+  <si>
+    <t>better but still fluctuating</t>
   </si>
 </sst>
 </file>
@@ -803,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
-  <dimension ref="A1:AI22"/>
+  <dimension ref="A1:AI24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="157" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A10" zoomScale="157" workbookViewId="0">
+      <selection activeCell="B20" sqref="A1:N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1755,17 +1765,248 @@
       <c r="AH22" s="25"/>
       <c r="AI22" s="25"/>
     </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>8857319</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="19">
+        <v>128</v>
+      </c>
+      <c r="G23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>8857317</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="19">
+        <v>128</v>
+      </c>
+      <c r="G24" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>8857317</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="19">
+        <v>128</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8857726</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1E-3</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="19">
+        <v>128</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>8857843</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="19">
+        <v>1E-4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="19">
+        <v>128</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8858089</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="19">
+        <v>128</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="180" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A25" zoomScale="180" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2802,12 +3043,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="181" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView topLeftCell="A32" zoomScale="181" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4039,7 +4280,12 @@
       <c r="H38" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I38" s="26"/>
+      <c r="I38" s="26">
+        <v>54</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="26">
@@ -4066,7 +4312,12 @@
       <c r="H39" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I39" s="26"/>
+      <c r="I39" s="26">
+        <v>99</v>
+      </c>
+      <c r="K39" s="28">
+        <v>0.58150000000000002</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="26">
@@ -4093,7 +4344,12 @@
       <c r="H40" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I40" s="26"/>
+      <c r="I40" s="26">
+        <v>119</v>
+      </c>
+      <c r="K40" s="18">
+        <v>0.80079999999999996</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="26">
@@ -4120,7 +4376,12 @@
       <c r="H41" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="I41" s="26"/>
+      <c r="I41" s="26">
+        <v>124</v>
+      </c>
+      <c r="K41" s="18">
+        <v>0.79479999999999995</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add label option to MoCoClf
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1012" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51DD0092-C676-4E4F-8646-727B628E2272}"/>
+  <xr:revisionPtr revIDLastSave="1020" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8055573-1401-A348-9905-F7EFB0642563}"/>
   <bookViews>
     <workbookView xWindow="-38860" yWindow="6820" windowWidth="43080" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="106">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -416,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -439,11 +439,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -499,6 +510,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1824,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1994,6 +2012,32 @@
       </c>
       <c r="I5" s="7" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>8858108</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="29">
+        <v>128</v>
+      </c>
+      <c r="G6" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="31" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3047,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI41"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="181" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A23" zoomScale="181" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add startpoint to all trainers
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1069" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BA9C5E-21AB-4249-BAAD-C6EF30F2C2F2}"/>
+  <xr:revisionPtr revIDLastSave="1075" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47A2CDBF-D43D-884F-B5B2-35BC7831538F}"/>
   <bookViews>
     <workbookView xWindow="5740" yWindow="1380" windowWidth="43080" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="114">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>failed but we can see this already raeach 250 at 50 epochs</t>
+  </si>
+  <si>
+    <t>8763825_290 start from8858108_59</t>
   </si>
 </sst>
 </file>
@@ -1876,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2173,6 +2176,32 @@
       </c>
       <c r="M8" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="35">
+        <v>8859036</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="29">
+        <v>128</v>
+      </c>
+      <c r="G9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="31" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update acc calculations for Classification problems
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1075" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47A2CDBF-D43D-884F-B5B2-35BC7831538F}"/>
+  <xr:revisionPtr revIDLastSave="1107" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{581215EF-C1A2-9549-87EC-10DBEC513B64}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="1380" windowWidth="43080" windowHeight="14220" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-40480" yWindow="6140" windowWidth="43080" windowHeight="14220" activeTab="3" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
-    <sheet name="Res50FC_speed" sheetId="4" r:id="rId2"/>
-    <sheet name="MoCo" sheetId="2" r:id="rId3"/>
-    <sheet name="MoCoClf" sheetId="3" r:id="rId4"/>
+    <sheet name="speed_actual" sheetId="4" r:id="rId2"/>
+    <sheet name="cyc_infras" sheetId="5" r:id="rId3"/>
+    <sheet name="n_lanes_onehot" sheetId="7" r:id="rId4"/>
+    <sheet name="road_type" sheetId="6" r:id="rId5"/>
+    <sheet name="MoCo" sheetId="2" r:id="rId6"/>
+    <sheet name="MoCoClf" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="114">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -478,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,6 +557,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1881,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="214" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2210,6 +2216,272 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD73061-4BAF-F54E-8EFF-64837B56220A}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" zoomScale="255" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="35">
+        <v>8859060</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="29">
+        <v>128</v>
+      </c>
+      <c r="G2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E3C5AA-20D1-7C41-8293-23B50C3B1A81}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="287" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="35">
+        <v>8859128</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="29">
+        <v>128</v>
+      </c>
+      <c r="F2" s="37">
+        <v>84</v>
+      </c>
+      <c r="G2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99EA194-F5BA-0349-B29E-B82D48F8A802}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" zoomScale="318" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="35">
+        <v>8859127</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="29">
+        <v>128</v>
+      </c>
+      <c r="G2" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI38"/>
   <sheetViews>
@@ -3274,7 +3546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI41"/>
   <sheetViews>

</xml_diff>

<commit_message>
update test for all attri predictions
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1107" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{581215EF-C1A2-9549-87EC-10DBEC513B64}"/>
+  <xr:revisionPtr revIDLastSave="1129" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{949799A4-A0FA-E54E-9696-9727CEE7BF1D}"/>
   <bookViews>
-    <workbookView xWindow="-40480" yWindow="6140" windowWidth="43080" windowHeight="14220" activeTab="3" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-46880" yWindow="9380" windowWidth="43080" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="118">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -383,6 +383,18 @@
   </si>
   <si>
     <t>8763825_290 start from8858108_59</t>
+  </si>
+  <si>
+    <t>haven't converge yet but showing good results</t>
+  </si>
+  <si>
+    <t>8763825_290 start from8859036_99</t>
+  </si>
+  <si>
+    <t>8763825_290 start from 8859128_84</t>
+  </si>
+  <si>
+    <t>8763825_290 start from 8859127_99</t>
   </si>
 </sst>
 </file>
@@ -1885,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView zoomScale="214" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2200,6 +2212,9 @@
       <c r="E9" s="29">
         <v>128</v>
       </c>
+      <c r="F9" s="37">
+        <v>99</v>
+      </c>
       <c r="G9" s="30" t="b">
         <v>0</v>
       </c>
@@ -2207,6 +2222,41 @@
         <v>1</v>
       </c>
       <c r="I9" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="35">
+        <v>235.17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="35">
+        <v>8860382</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="29">
+        <v>128</v>
+      </c>
+      <c r="F10" s="37">
+        <v>99</v>
+      </c>
+      <c r="G10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2219,8 +2269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD73061-4BAF-F54E-8EFF-64837B56220A}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="255" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="255" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2283,6 +2333,9 @@
       <c r="E2" s="29">
         <v>128</v>
       </c>
+      <c r="F2" s="37">
+        <v>89</v>
+      </c>
       <c r="G2" s="30" t="b">
         <v>0</v>
       </c>
@@ -2306,10 +2359,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E3C5AA-20D1-7C41-8293-23B50C3B1A81}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="287" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="287" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2391,6 +2444,35 @@
         <v>92</v>
       </c>
     </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="35">
+        <v>8860385</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="29">
+        <v>128</v>
+      </c>
+      <c r="F3" s="37">
+        <v>84</v>
+      </c>
+      <c r="G3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="31" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2398,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99EA194-F5BA-0349-B29E-B82D48F8A802}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="318" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView zoomScale="318" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2460,6 +2542,9 @@
       <c r="E2" s="29">
         <v>128</v>
       </c>
+      <c r="F2" s="37">
+        <v>99</v>
+      </c>
       <c r="G2" s="30" t="b">
         <v>0</v>
       </c>
@@ -2474,6 +2559,35 @@
       <c r="L2" s="35"/>
       <c r="M2" s="36" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8860384</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="29">
+        <v>128</v>
+      </c>
+      <c r="F3" s="37">
+        <v>99</v>
+      </c>
+      <c r="G3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="31" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add biased sampling for cyc_infras pred
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1129" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{949799A4-A0FA-E54E-9696-9727CEE7BF1D}"/>
+  <xr:revisionPtr revIDLastSave="1136" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB2B215A-BF71-4F47-8E0A-A263511E8704}"/>
   <bookViews>
     <workbookView xWindow="-46880" yWindow="9380" windowWidth="43080" windowHeight="14220" activeTab="2" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="120">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>8763825_290 start from 8859127_99</t>
+  </si>
+  <si>
+    <t>prediction everything to be 0</t>
+  </si>
+  <si>
+    <t>add over sampling</t>
   </si>
 </sst>
 </file>
@@ -2267,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD73061-4BAF-F54E-8EFF-64837B56220A}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="255" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2349,7 +2355,44 @@
       <c r="K2" s="35"/>
       <c r="L2" s="35"/>
       <c r="M2" s="36" t="s">
-        <v>92</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8860416</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="29">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="29">
+        <v>128</v>
+      </c>
+      <c r="G3" s="37">
+        <v>89</v>
+      </c>
+      <c r="H3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add random seed control
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1302" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC9ED273-6834-6F47-9102-736026FBC684}"/>
+  <xr:revisionPtr revIDLastSave="1305" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11986375-40F1-0F4F-B461-5DC6BD181B8C}"/>
   <bookViews>
     <workbookView xWindow="-47820" yWindow="-160" windowWidth="43080" windowHeight="14220" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="129">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>wired</t>
+  </si>
+  <si>
+    <t>need to check later, loss is wired</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="157" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2078,7 +2081,9 @@
       <c r="L27" s="40">
         <v>0.81730000000000003</v>
       </c>
-      <c r="M27" s="33"/>
+      <c r="M27" s="33" t="s">
+        <v>128</v>
+      </c>
       <c r="N27" s="33"/>
       <c r="O27" s="33"/>
       <c r="P27" s="33"/>
@@ -2135,7 +2140,9 @@
       <c r="L28" s="40">
         <v>0.78920000000000001</v>
       </c>
-      <c r="M28" s="33"/>
+      <c r="M28" s="33" t="s">
+        <v>128</v>
+      </c>
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
       <c r="P28" s="33"/>

</xml_diff>

<commit_message>
add mask former module
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1692" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{754E8215-B969-FD40-823C-F63367AC80C0}"/>
+  <xr:revisionPtr revIDLastSave="1795" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD771E5B-0715-CF47-A0B1-B2D59145C660}"/>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="9420" windowWidth="43080" windowHeight="14220" activeTab="5" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="5680" yWindow="1680" windowWidth="43080" windowHeight="19860" activeTab="7" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="MoCo" sheetId="2" r:id="rId7"/>
     <sheet name="MoCoClf" sheetId="3" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="177">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -519,6 +519,60 @@
   </si>
   <si>
     <t>consider increasing # of epochs if have time</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, start from 8899274_49)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, start from 8899123_49)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, start from 8897747_49)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, start from 8900561_99)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, start from 8900562_99)</t>
+  </si>
+  <si>
+    <t>increase the number of epochs</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, satrt from 8899275_49)</t>
+  </si>
+  <si>
+    <t>encounter random error from the cluster, terminated at epoch 680</t>
+  </si>
+  <si>
+    <t>Ord MoCo (start from 8899242_680)</t>
+  </si>
+  <si>
+    <t>8897030_980</t>
+  </si>
+  <si>
+    <t>8897030_760</t>
+  </si>
+  <si>
+    <t>severe overfitting</t>
+  </si>
+  <si>
+    <t>8897030_500</t>
+  </si>
+  <si>
+    <t>8897030_600</t>
+  </si>
+  <si>
+    <t>8878104_220</t>
+  </si>
+  <si>
+    <t>8878104_240</t>
+  </si>
+  <si>
+    <t>8878104_260</t>
+  </si>
+  <si>
+    <t>8878104_280</t>
   </si>
 </sst>
 </file>
@@ -548,7 +602,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +654,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -664,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -793,6 +859,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2872,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="214" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A4" zoomScale="214" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3261,9 +3379,38 @@
       <c r="I11" s="57" t="b">
         <v>1</v>
       </c>
+      <c r="M11" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B12"/>
+      <c r="A12" s="28">
+        <v>8903282</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="52">
+        <v>1E-4</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="53">
+        <v>128</v>
+      </c>
+      <c r="F12" s="54">
+        <v>99</v>
+      </c>
+      <c r="G12" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="57" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3399,10 +3546,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E3C5AA-20D1-7C41-8293-23B50C3B1A81}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView zoomScale="287" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="225" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3449,102 +3596,119 @@
       </c>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="28">
+    <row r="2" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="58">
         <v>8859128</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="60">
         <v>0.01</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="23">
-        <v>128</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="D2" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="60">
+        <v>128</v>
+      </c>
+      <c r="F2" s="59">
         <v>84</v>
       </c>
-      <c r="G2" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="31">
+      <c r="G2" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="62">
         <v>0.74560000000000004</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="61" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="28">
+    <row r="3" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="58">
         <v>8860385</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="60">
         <v>0.01</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="23">
-        <v>128</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="D3" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="60">
+        <v>128</v>
+      </c>
+      <c r="F3" s="59">
         <v>84</v>
       </c>
-      <c r="G3" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="25" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="G3" s="60" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="60" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="61" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="44" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="44">
         <v>8899274</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="64">
         <v>1E-4</v>
       </c>
-      <c r="D4" s="53" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="53">
-        <v>128</v>
-      </c>
-      <c r="F4" s="54">
+      <c r="D4" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="65">
+        <v>128</v>
+      </c>
+      <c r="F4" s="66">
         <v>99</v>
       </c>
-      <c r="G4" s="55" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="56" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="57" t="b">
-        <v>1</v>
+      <c r="G4" s="67" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="68" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="69" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" s="61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8900559</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5">
+        <v>79</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0.78680000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -3554,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99EA194-F5BA-0349-B29E-B82D48F8A802}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="230" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView zoomScale="230" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3772,9 +3936,75 @@
       <c r="I6" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="12">
+        <v>0.86380000000000001</v>
+      </c>
       <c r="M6" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>8900562</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="23">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23">
+        <v>128</v>
+      </c>
+      <c r="F7" s="8">
+        <v>42</v>
+      </c>
+      <c r="G7" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="39">
+        <v>8901570</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="77">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="77">
+        <v>128</v>
+      </c>
+      <c r="F8" s="39">
+        <v>193</v>
+      </c>
+      <c r="G8" s="77" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="77" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="78" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="47">
+        <v>0.86699999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3784,16 +4014,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5B8BFC-BD6E-0747-8364-88A4C94E808C}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="231" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView zoomScale="231" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -3852,7 +4082,7 @@
         <v>128</v>
       </c>
       <c r="F2" s="54">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="G2" s="55" t="b">
         <v>0</v>
@@ -3862,9 +4092,76 @@
       </c>
       <c r="I2" s="57" t="b">
         <v>1</v>
+      </c>
+      <c r="L2" s="12">
+        <v>0.85660000000000003</v>
       </c>
       <c r="M2" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8900561</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="52">
+        <v>1E-4</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="53">
+        <v>128</v>
+      </c>
+      <c r="F3" s="54">
+        <v>46</v>
+      </c>
+      <c r="G3" s="55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="56" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34">
+        <v>8901571</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="71">
+        <v>1E-4</v>
+      </c>
+      <c r="D4" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="72">
+        <v>128</v>
+      </c>
+      <c r="F4" s="73">
+        <v>174</v>
+      </c>
+      <c r="G4" s="74" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="75" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="76" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="47">
+        <v>0.86040000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -3876,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI49"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A32" zoomScale="180" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5076,17 +5373,32 @@
         <v>1</v>
       </c>
       <c r="G44" s="39"/>
+      <c r="I44" s="34" t="s">
+        <v>166</v>
+      </c>
       <c r="J44" s="39"/>
       <c r="K44" s="39"/>
       <c r="L44" s="39"/>
     </row>
     <row r="45" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
+      <c r="A45" s="39">
+        <v>8905233</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="39">
+        <v>128</v>
+      </c>
+      <c r="F45" s="39">
+        <v>1</v>
+      </c>
       <c r="G45" s="39"/>
       <c r="J45" s="39"/>
       <c r="K45" s="39"/>
@@ -5148,10 +5460,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI65"/>
+  <dimension ref="A1:AI75"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="181" workbookViewId="0">
-      <selection activeCell="L65" sqref="L65"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="181" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7212,6 +7524,284 @@
         <v>153</v>
       </c>
     </row>
+    <row r="66" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="9">
+        <v>8908438</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="9">
+        <v>128</v>
+      </c>
+      <c r="F66" s="9">
+        <v>1</v>
+      </c>
+      <c r="G66" s="9">
+        <v>200</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I66" s="9">
+        <v>39</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9">
+        <v>8908439</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="9">
+        <v>128</v>
+      </c>
+      <c r="F67" s="9">
+        <v>1</v>
+      </c>
+      <c r="G67" s="9">
+        <v>200</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="L67" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="79">
+        <v>8908441</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="9">
+        <v>128</v>
+      </c>
+      <c r="F68" s="9">
+        <v>1</v>
+      </c>
+      <c r="G68" s="9">
+        <v>200</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="I68" s="9">
+        <v>17</v>
+      </c>
+      <c r="L68" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="9">
+        <v>8908440</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="9">
+        <v>128</v>
+      </c>
+      <c r="F69" s="9">
+        <v>1</v>
+      </c>
+      <c r="G69" s="9">
+        <v>200</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A70" s="9">
+        <v>8910616</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="9">
+        <v>128</v>
+      </c>
+      <c r="F70" s="9">
+        <v>1</v>
+      </c>
+      <c r="G70" s="9">
+        <v>200</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A71" s="9">
+        <v>8910618</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" s="9">
+        <v>128</v>
+      </c>
+      <c r="F71" s="9">
+        <v>1</v>
+      </c>
+      <c r="G71" s="9">
+        <v>200</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A72" s="9">
+        <v>8910792</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="9">
+        <v>128</v>
+      </c>
+      <c r="F72" s="9">
+        <v>1</v>
+      </c>
+      <c r="G72" s="9">
+        <v>200</v>
+      </c>
+      <c r="H72" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A73" s="9">
+        <v>8910797</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="9">
+        <v>128</v>
+      </c>
+      <c r="F73" s="9">
+        <v>1</v>
+      </c>
+      <c r="G73" s="9">
+        <v>200</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A74" s="9">
+        <v>8910798</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" s="9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" s="9">
+        <v>128</v>
+      </c>
+      <c r="F74" s="9">
+        <v>1</v>
+      </c>
+      <c r="G74" s="9">
+        <v>200</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A75" s="9">
+        <v>8910799</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D75" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="16">
+        <v>128</v>
+      </c>
+      <c r="F75" s="16">
+        <v>1</v>
+      </c>
+      <c r="G75" s="16">
+        <v>200</v>
+      </c>
+      <c r="H75" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add scenario features to side feature
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1879" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C84178-736E-4E4A-BAE4-DBA203A55479}"/>
+  <xr:revisionPtr revIDLastSave="1896" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A18B8FFB-C449-744F-9EAD-327D00870F91}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="1780" windowWidth="43080" windowHeight="19860" activeTab="1" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="4760" yWindow="1780" windowWidth="43080" windowHeight="19860" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="182">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -581,6 +581,15 @@
   </si>
   <si>
     <t>correct speed categories!</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 + sce1</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 + sce2</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 + sce3</t>
   </si>
 </sst>
 </file>
@@ -1235,10 +1244,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
-  <dimension ref="A1:AI38"/>
+  <dimension ref="A1:AI40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="157" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2955,15 +2964,31 @@
       <c r="AI37" s="33"/>
     </row>
     <row r="38" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
+      <c r="A38" s="32">
+        <v>8917437</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="C38" s="32">
+        <v>1E-4</v>
+      </c>
+      <c r="D38" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="32">
+        <v>128</v>
+      </c>
       <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
+      <c r="G38" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="32" t="b">
+        <v>0</v>
+      </c>
       <c r="J38" s="32"/>
       <c r="K38" s="32"/>
       <c r="L38" s="32"/>
@@ -2990,6 +3015,60 @@
       <c r="AG38" s="33"/>
       <c r="AH38" s="33"/>
       <c r="AI38" s="33"/>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A39" s="32">
+        <v>8917438</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C39" s="32">
+        <v>1E-4</v>
+      </c>
+      <c r="D39" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="32">
+        <v>128</v>
+      </c>
+      <c r="F39" s="32"/>
+      <c r="G39" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A40" s="32">
+        <v>8917439</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" s="32">
+        <v>1E-4</v>
+      </c>
+      <c r="D40" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="32">
+        <v>128</v>
+      </c>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="32" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5509,8 +5588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView zoomScale="214" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5994,6 +6073,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add color jittering to MoCo dataset
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bolin/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1896" documentId="8_{617594CE-D88A-2B4E-9C6E-F89E3E464D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A18B8FFB-C449-744F-9EAD-327D00870F91}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E899C16-016F-FE4E-BA9D-45FDFDB903F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="1780" windowWidth="43080" windowHeight="19860" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="9520" yWindow="820" windowWidth="20720" windowHeight="9040" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="180">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -68,12 +68,6 @@
   </si>
   <si>
     <t>best_epoch_id (starting from 0)</t>
-  </si>
-  <si>
-    <t>train_accuracy</t>
-  </si>
-  <si>
-    <t>vali_accuracy</t>
   </si>
   <si>
     <t>frozen</t>
@@ -747,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -927,9 +921,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,28 +1235,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
-  <dimension ref="A1:AI40"/>
+  <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="157" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23" style="3" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" style="3"/>
     <col min="6" max="6" width="11.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="21" style="3" customWidth="1"/>
-    <col min="13" max="35" width="10.83203125" style="5"/>
+    <col min="7" max="7" width="10.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21" style="3" customWidth="1"/>
+    <col min="11" max="33" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1285,23 +1274,19 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -1323,10 +1308,8 @@
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>8504035</v>
       </c>
@@ -1355,16 +1338,10 @@
         <v>0</v>
       </c>
       <c r="J2" s="4">
-        <v>0.69369999999999998</v>
-      </c>
-      <c r="K2" s="4">
-        <v>0.6421</v>
-      </c>
-      <c r="L2" s="4">
         <v>0.63780000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>8520205</v>
       </c>
@@ -1393,16 +1370,10 @@
         <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>0.72389999999999999</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.6341</v>
-      </c>
-      <c r="L3" s="4">
         <v>0.62860000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>8520206</v>
       </c>
@@ -1431,16 +1402,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="4">
-        <v>0.6784</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0.65210000000000001</v>
-      </c>
-      <c r="L4" s="4">
         <v>0.65759999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>8524094</v>
       </c>
@@ -1469,16 +1434,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="4">
-        <v>0.69950000000000001</v>
-      </c>
-      <c r="K5" s="4">
-        <v>0.64870000000000005</v>
-      </c>
-      <c r="L5" s="4">
         <v>0.65280000000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>8531513</v>
       </c>
@@ -1507,21 +1466,15 @@
         <v>1</v>
       </c>
       <c r="J6" s="4">
-        <v>0.66279999999999994</v>
-      </c>
-      <c r="K6" s="4">
-        <v>0.58640000000000003</v>
-      </c>
-      <c r="L6" s="4">
         <v>0.59770000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>8777104</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="13">
         <v>1E-3</v>
@@ -1544,11 +1497,11 @@
       <c r="I7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14">
+      <c r="J7" s="14">
         <v>0.65490000000000004</v>
       </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
@@ -1570,15 +1523,13 @@
       <c r="AE7" s="15"/>
       <c r="AF7" s="15"/>
       <c r="AG7" s="15"/>
-      <c r="AH7" s="15"/>
-      <c r="AI7" s="15"/>
-    </row>
-    <row r="8" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>8777107</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="13">
         <v>1E-3</v>
@@ -1601,11 +1552,11 @@
       <c r="I8" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14">
+      <c r="J8" s="14">
         <v>0.59240000000000004</v>
       </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
@@ -1627,15 +1578,13 @@
       <c r="AE8" s="15"/>
       <c r="AF8" s="15"/>
       <c r="AG8" s="15"/>
-      <c r="AH8" s="15"/>
-      <c r="AI8" s="15"/>
-    </row>
-    <row r="9" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>8780600</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="13">
         <v>1E-3</v>
@@ -1658,11 +1607,11 @@
       <c r="I9" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14">
+      <c r="J9" s="14">
         <v>0.63429999999999997</v>
       </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
@@ -1684,15 +1633,13 @@
       <c r="AE9" s="15"/>
       <c r="AF9" s="15"/>
       <c r="AG9" s="15"/>
-      <c r="AH9" s="15"/>
-      <c r="AI9" s="15"/>
-    </row>
-    <row r="10" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>8782406</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="13">
         <v>1E-3</v>
@@ -1715,11 +1662,11 @@
       <c r="I10" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14">
+      <c r="J10" s="14">
         <v>0.56310000000000004</v>
       </c>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
@@ -1741,15 +1688,13 @@
       <c r="AE10" s="15"/>
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
-      <c r="AH10" s="15"/>
-      <c r="AI10" s="15"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>8834025</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="13">
         <v>1E-3</v>
@@ -1772,21 +1717,19 @@
       <c r="I11" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14">
+      <c r="J11" s="14">
         <v>0.56310000000000004</v>
       </c>
-      <c r="M11" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="K11" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>8834107</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" s="13">
         <v>1E-3</v>
@@ -1809,21 +1752,19 @@
       <c r="I12" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="M12" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="K12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>8834107</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" s="13">
         <v>0.01</v>
@@ -1846,15 +1787,13 @@
       <c r="I13" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>8835249</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="13">
         <v>0.01</v>
@@ -1878,12 +1817,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>8835250</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C15" s="13">
         <v>0.01</v>
@@ -1907,12 +1846,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>8835261</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="13">
         <v>0.01</v>
@@ -1936,12 +1875,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>8836387</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="13">
         <v>0.01</v>
@@ -1964,16 +1903,16 @@
       <c r="I17" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="L17" s="4">
+      <c r="J17" s="4">
         <v>0.78239999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>8836388</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C18" s="13">
         <v>0.01</v>
@@ -1996,19 +1935,19 @@
       <c r="I18" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="L18" s="4">
+      <c r="J18" s="4">
         <v>0.79600000000000004</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="K18" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>8836393</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C19" s="13">
         <v>0.01</v>
@@ -2031,16 +1970,16 @@
       <c r="I19" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="M19" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="K19" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>8836394</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C20" s="13">
         <v>0.01</v>
@@ -2064,12 +2003,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>8837237</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C21" s="18">
         <v>0.01</v>
@@ -2093,8 +2032,8 @@
         <v>0</v>
       </c>
       <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
@@ -2116,15 +2055,13 @@
       <c r="AE21" s="19"/>
       <c r="AF21" s="19"/>
       <c r="AG21" s="19"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="19"/>
-    </row>
-    <row r="22" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:33" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>8837239</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" s="18">
         <v>0.01</v>
@@ -2148,8 +2085,8 @@
         <v>0</v>
       </c>
       <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
@@ -2171,15 +2108,13 @@
       <c r="AE22" s="19"/>
       <c r="AF22" s="19"/>
       <c r="AG22" s="19"/>
-      <c r="AH22" s="19"/>
-      <c r="AI22" s="19"/>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>8857319</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="13">
         <v>0.01</v>
@@ -2200,12 +2135,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>8857317</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="13">
         <v>0.01</v>
@@ -2226,12 +2161,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32">
         <v>8886900</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="32">
         <v>1E-3</v>
@@ -2254,15 +2189,15 @@
       <c r="I25" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="40">
+      <c r="J25" s="40">
         <v>0.66200000000000003</v>
       </c>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33" t="s">
+        <v>121</v>
+      </c>
       <c r="M25" s="33"/>
-      <c r="N25" s="33" t="s">
-        <v>123</v>
-      </c>
+      <c r="N25" s="33"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
@@ -2282,15 +2217,13 @@
       <c r="AE25" s="33"/>
       <c r="AF25" s="33"/>
       <c r="AG25" s="33"/>
-      <c r="AH25" s="33"/>
-      <c r="AI25" s="33"/>
-    </row>
-    <row r="26" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
         <v>8886891</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" s="41">
         <v>0.01</v>
@@ -2314,11 +2247,11 @@
         <v>0</v>
       </c>
       <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="43" t="s">
-        <v>139</v>
-      </c>
+      <c r="K26" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
       <c r="N26" s="43"/>
       <c r="O26" s="43"/>
       <c r="P26" s="43"/>
@@ -2339,15 +2272,13 @@
       <c r="AE26" s="43"/>
       <c r="AF26" s="43"/>
       <c r="AG26" s="43"/>
-      <c r="AH26" s="43"/>
-      <c r="AI26" s="43"/>
-    </row>
-    <row r="27" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32">
         <v>8886880</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="32">
         <v>0.01</v>
@@ -2370,14 +2301,14 @@
       <c r="I27" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="40">
+      <c r="J27" s="40">
         <v>0.81730000000000003</v>
       </c>
-      <c r="M27" s="33" t="s">
-        <v>126</v>
-      </c>
+      <c r="K27" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
       <c r="N27" s="33"/>
       <c r="O27" s="33"/>
       <c r="P27" s="33"/>
@@ -2398,15 +2329,13 @@
       <c r="AE27" s="33"/>
       <c r="AF27" s="33"/>
       <c r="AG27" s="33"/>
-      <c r="AH27" s="33"/>
-      <c r="AI27" s="33"/>
-    </row>
-    <row r="28" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32">
         <v>8886881</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C28" s="32">
         <v>0.01</v>
@@ -2429,14 +2358,14 @@
       <c r="I28" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="40">
+      <c r="J28" s="40">
         <v>0.78920000000000001</v>
       </c>
-      <c r="M28" s="33" t="s">
-        <v>126</v>
-      </c>
+      <c r="K28" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
       <c r="N28" s="33"/>
       <c r="O28" s="33"/>
       <c r="P28" s="33"/>
@@ -2457,15 +2386,13 @@
       <c r="AE28" s="33"/>
       <c r="AF28" s="33"/>
       <c r="AG28" s="33"/>
-      <c r="AH28" s="33"/>
-      <c r="AI28" s="33"/>
-    </row>
-    <row r="29" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="41">
         <v>8886884</v>
       </c>
       <c r="B29" s="41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="41">
         <v>0.01</v>
@@ -2488,12 +2415,12 @@
       <c r="I29" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="43" t="s">
-        <v>129</v>
-      </c>
+      <c r="J29" s="42"/>
+      <c r="K29" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
       <c r="N29" s="43"/>
       <c r="O29" s="43"/>
       <c r="P29" s="43"/>
@@ -2514,15 +2441,13 @@
       <c r="AE29" s="43"/>
       <c r="AF29" s="43"/>
       <c r="AG29" s="43"/>
-      <c r="AH29" s="43"/>
-      <c r="AI29" s="43"/>
-    </row>
-    <row r="30" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="41">
         <v>8886885</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C30" s="41">
         <v>0.01</v>
@@ -2545,12 +2470,12 @@
       <c r="I30" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="43" t="s">
-        <v>129</v>
-      </c>
+      <c r="J30" s="42"/>
+      <c r="K30" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
       <c r="N30" s="43"/>
       <c r="O30" s="43"/>
       <c r="P30" s="43"/>
@@ -2571,15 +2496,13 @@
       <c r="AE30" s="43"/>
       <c r="AF30" s="43"/>
       <c r="AG30" s="43"/>
-      <c r="AH30" s="43"/>
-      <c r="AI30" s="43"/>
-    </row>
-    <row r="31" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="41">
         <v>8889925</v>
       </c>
       <c r="B31" s="41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C31" s="41">
         <v>0.1</v>
@@ -2601,11 +2524,11 @@
         <v>0</v>
       </c>
       <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="43" t="s">
-        <v>127</v>
-      </c>
+      <c r="K31" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
       <c r="N31" s="43"/>
       <c r="O31" s="43"/>
       <c r="P31" s="43"/>
@@ -2626,15 +2549,13 @@
       <c r="AE31" s="43"/>
       <c r="AF31" s="43"/>
       <c r="AG31" s="43"/>
-      <c r="AH31" s="43"/>
-      <c r="AI31" s="43"/>
-    </row>
-    <row r="32" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="41">
         <v>8889924</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C32" s="41">
         <v>0.1</v>
@@ -2656,11 +2577,11 @@
         <v>0</v>
       </c>
       <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="43" t="s">
-        <v>128</v>
-      </c>
+      <c r="K32" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
       <c r="N32" s="43"/>
       <c r="O32" s="43"/>
       <c r="P32" s="43"/>
@@ -2681,15 +2602,13 @@
       <c r="AE32" s="43"/>
       <c r="AF32" s="43"/>
       <c r="AG32" s="43"/>
-      <c r="AH32" s="43"/>
-      <c r="AI32" s="43"/>
-    </row>
-    <row r="33" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="41">
         <v>8890178</v>
       </c>
       <c r="B33" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="41">
         <v>3.0000000000000001E-3</v>
@@ -2711,11 +2630,11 @@
         <v>0</v>
       </c>
       <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="43" t="s">
-        <v>138</v>
-      </c>
+      <c r="K33" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
       <c r="N33" s="43"/>
       <c r="O33" s="43"/>
       <c r="P33" s="43"/>
@@ -2736,15 +2655,13 @@
       <c r="AE33" s="43"/>
       <c r="AF33" s="43"/>
       <c r="AG33" s="43"/>
-      <c r="AH33" s="43"/>
-      <c r="AI33" s="43"/>
-    </row>
-    <row r="34" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="32">
         <v>8890095</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C34" s="32">
         <v>3.0000000000000001E-3</v>
@@ -2767,11 +2684,11 @@
       <c r="I34" s="32" t="b">
         <v>0</v>
       </c>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="40">
+      <c r="J34" s="40">
         <v>0.68869999999999998</v>
       </c>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
       <c r="M34" s="33"/>
       <c r="N34" s="33"/>
       <c r="O34" s="33"/>
@@ -2793,15 +2710,13 @@
       <c r="AE34" s="33"/>
       <c r="AF34" s="33"/>
       <c r="AG34" s="33"/>
-      <c r="AH34" s="33"/>
-      <c r="AI34" s="33"/>
-    </row>
-    <row r="35" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32">
         <v>8890096</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C35" s="32">
         <v>3.0000000000000001E-3</v>
@@ -2825,11 +2740,11 @@
         <v>0</v>
       </c>
       <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="33" t="s">
-        <v>142</v>
-      </c>
+      <c r="K35" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
       <c r="N35" s="33"/>
       <c r="O35" s="33"/>
       <c r="P35" s="33"/>
@@ -2850,15 +2765,13 @@
       <c r="AE35" s="33"/>
       <c r="AF35" s="33"/>
       <c r="AG35" s="33"/>
-      <c r="AH35" s="33"/>
-      <c r="AI35" s="33"/>
-    </row>
-    <row r="36" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="41">
         <v>8891440</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36" s="41">
         <v>0.1</v>
@@ -2880,11 +2793,11 @@
         <v>0</v>
       </c>
       <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="43" t="s">
-        <v>137</v>
-      </c>
+      <c r="K36" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
       <c r="N36" s="43"/>
       <c r="O36" s="43"/>
       <c r="P36" s="43"/>
@@ -2905,15 +2818,13 @@
       <c r="AE36" s="43"/>
       <c r="AF36" s="43"/>
       <c r="AG36" s="43"/>
-      <c r="AH36" s="43"/>
-      <c r="AI36" s="43"/>
-    </row>
-    <row r="37" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32">
         <v>8891507</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C37" s="32">
         <v>0.03</v>
@@ -2935,11 +2846,11 @@
         <v>0</v>
       </c>
       <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="33" t="s">
-        <v>142</v>
-      </c>
+      <c r="K37" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
       <c r="N37" s="33"/>
       <c r="O37" s="33"/>
       <c r="P37" s="33"/>
@@ -2960,115 +2871,328 @@
       <c r="AE37" s="33"/>
       <c r="AF37" s="33"/>
       <c r="AG37" s="33"/>
-      <c r="AH37" s="33"/>
-      <c r="AI37" s="33"/>
-    </row>
-    <row r="38" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="32">
-        <v>8917437</v>
-      </c>
-      <c r="B38" s="32" t="s">
+    </row>
+    <row r="38" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="13">
+        <v>8917457</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C38" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="13">
+        <v>128</v>
+      </c>
+      <c r="F38" s="13">
+        <v>2</v>
+      </c>
+      <c r="G38" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="14">
+        <v>0.65180000000000005</v>
+      </c>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
+      <c r="S38" s="15"/>
+      <c r="T38" s="15"/>
+      <c r="U38" s="15"/>
+      <c r="V38" s="15"/>
+      <c r="W38" s="15"/>
+      <c r="X38" s="15"/>
+      <c r="Y38" s="15"/>
+      <c r="Z38" s="15"/>
+      <c r="AA38" s="15"/>
+      <c r="AB38" s="15"/>
+      <c r="AC38" s="15"/>
+      <c r="AD38" s="15"/>
+      <c r="AE38" s="15"/>
+      <c r="AF38" s="15"/>
+      <c r="AG38" s="15"/>
+    </row>
+    <row r="39" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <v>8919722</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="13">
+        <v>128</v>
+      </c>
+      <c r="F39" s="13">
+        <v>9</v>
+      </c>
+      <c r="G39" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" s="13"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="15"/>
+      <c r="Q39" s="15"/>
+      <c r="R39" s="15"/>
+      <c r="S39" s="15"/>
+      <c r="T39" s="15"/>
+      <c r="U39" s="15"/>
+      <c r="V39" s="15"/>
+      <c r="W39" s="15"/>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="15"/>
+      <c r="Z39" s="15"/>
+      <c r="AA39" s="15"/>
+      <c r="AB39" s="15"/>
+      <c r="AC39" s="15"/>
+      <c r="AD39" s="15"/>
+      <c r="AE39" s="15"/>
+      <c r="AF39" s="15"/>
+      <c r="AG39" s="15"/>
+    </row>
+    <row r="40" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
+        <v>8917459</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C38" s="32">
+      <c r="C40" s="13">
         <v>1E-4</v>
       </c>
-      <c r="D38" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="32">
-        <v>128</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H38" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="33"/>
-      <c r="N38" s="33"/>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
-      <c r="R38" s="33"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
-      <c r="U38" s="33"/>
-      <c r="V38" s="33"/>
-      <c r="W38" s="33"/>
-      <c r="X38" s="33"/>
-      <c r="Y38" s="33"/>
-      <c r="Z38" s="33"/>
-      <c r="AA38" s="33"/>
-      <c r="AB38" s="33"/>
-      <c r="AC38" s="33"/>
-      <c r="AD38" s="33"/>
-      <c r="AE38" s="33"/>
-      <c r="AF38" s="33"/>
-      <c r="AG38" s="33"/>
-      <c r="AH38" s="33"/>
-      <c r="AI38" s="33"/>
-    </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A39" s="32">
-        <v>8917438</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="C39" s="32">
-        <v>1E-4</v>
-      </c>
-      <c r="D39" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="32">
-        <v>128</v>
-      </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39" s="32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A40" s="32">
-        <v>8917439</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="C40" s="32">
-        <v>1E-4</v>
-      </c>
-      <c r="D40" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="32">
-        <v>128</v>
-      </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="32" t="b">
-        <v>0</v>
-      </c>
+      <c r="D40" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="13">
+        <v>128</v>
+      </c>
+      <c r="F40" s="13">
+        <v>10</v>
+      </c>
+      <c r="G40" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" s="14">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+      <c r="O40" s="15"/>
+      <c r="P40" s="15"/>
+      <c r="Q40" s="15"/>
+      <c r="R40" s="15"/>
+      <c r="S40" s="15"/>
+      <c r="T40" s="15"/>
+      <c r="U40" s="15"/>
+      <c r="V40" s="15"/>
+      <c r="W40" s="15"/>
+      <c r="X40" s="15"/>
+      <c r="Y40" s="15"/>
+      <c r="Z40" s="15"/>
+      <c r="AA40" s="15"/>
+      <c r="AB40" s="15"/>
+      <c r="AC40" s="15"/>
+      <c r="AD40" s="15"/>
+      <c r="AE40" s="15"/>
+      <c r="AF40" s="15"/>
+      <c r="AG40" s="15"/>
+    </row>
+    <row r="41" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13">
+        <v>8918581</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="13">
+        <v>128</v>
+      </c>
+      <c r="F41" s="13">
+        <v>32</v>
+      </c>
+      <c r="G41" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" s="13"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
+      <c r="S41" s="15"/>
+      <c r="T41" s="15"/>
+      <c r="U41" s="15"/>
+      <c r="V41" s="15"/>
+      <c r="W41" s="15"/>
+      <c r="X41" s="15"/>
+      <c r="Y41" s="15"/>
+      <c r="Z41" s="15"/>
+      <c r="AA41" s="15"/>
+      <c r="AB41" s="15"/>
+      <c r="AC41" s="15"/>
+      <c r="AD41" s="15"/>
+      <c r="AE41" s="15"/>
+      <c r="AF41" s="15"/>
+      <c r="AG41" s="15"/>
+    </row>
+    <row r="42" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="13">
+        <v>8919721</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="13">
+        <v>128</v>
+      </c>
+      <c r="F42" s="13">
+        <v>29</v>
+      </c>
+      <c r="G42" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+      <c r="V42" s="15"/>
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+      <c r="Z42" s="15"/>
+      <c r="AA42" s="15"/>
+      <c r="AB42" s="15"/>
+      <c r="AC42" s="15"/>
+      <c r="AD42" s="15"/>
+      <c r="AE42" s="15"/>
+      <c r="AF42" s="15"/>
+      <c r="AG42" s="15"/>
+    </row>
+    <row r="43" spans="1:33" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="13">
+        <v>8918583</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="13">
+        <v>128</v>
+      </c>
+      <c r="F43" s="13">
+        <v>19</v>
+      </c>
+      <c r="G43" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
+      <c r="S43" s="15"/>
+      <c r="T43" s="15"/>
+      <c r="U43" s="15"/>
+      <c r="V43" s="15"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
+      <c r="Z43" s="15"/>
+      <c r="AA43" s="15"/>
+      <c r="AB43" s="15"/>
+      <c r="AC43" s="15"/>
+      <c r="AD43" s="15"/>
+      <c r="AE43" s="15"/>
+      <c r="AF43" s="15"/>
+      <c r="AG43" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3113,25 +3237,25 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -3162,7 +3286,7 @@
         <v>8637608</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>2.9999999999999997E-4</v>
@@ -3180,10 +3304,10 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -3193,7 +3317,7 @@
         <v>8639430</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>3.0000000000000001E-3</v>
@@ -3211,7 +3335,7 @@
         <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J3" s="7">
         <v>0.6</v>
@@ -3220,7 +3344,7 @@
         <v>0.42</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
@@ -3228,7 +3352,7 @@
         <v>8641783</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>3.0000000000000001E-3</v>
@@ -3246,10 +3370,10 @@
         <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
@@ -3257,7 +3381,7 @@
         <v>8641803</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>3.0000000000000001E-3</v>
@@ -3275,10 +3399,10 @@
         <v>50</v>
       </c>
       <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
         <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.2">
@@ -3286,7 +3410,7 @@
         <v>8641912</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>3.0000000000000001E-3</v>
@@ -3304,10 +3428,10 @@
         <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
@@ -3315,7 +3439,7 @@
         <v>8642199</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>2.9999999999999997E-4</v>
@@ -3333,10 +3457,10 @@
         <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.2">
@@ -3344,7 +3468,7 @@
         <v>8642862</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>2.9999999999999997E-4</v>
@@ -3362,7 +3486,7 @@
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
@@ -3370,7 +3494,7 @@
         <v>8757293</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>3.0000000000000001E-3</v>
@@ -3388,10 +3512,10 @@
         <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.2">
@@ -3399,7 +3523,7 @@
         <v>8757377</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>0.3</v>
@@ -3417,10 +3541,10 @@
         <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.2">
@@ -3428,7 +3552,7 @@
         <v>8773343</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>0.3</v>
@@ -3446,13 +3570,13 @@
         <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
@@ -3460,7 +3584,7 @@
         <v>8773369</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>0.3</v>
@@ -3478,13 +3602,13 @@
         <v>30</v>
       </c>
       <c r="H12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" t="s">
         <v>63</v>
       </c>
-      <c r="L12" t="s">
-        <v>65</v>
-      </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
@@ -3492,7 +3616,7 @@
         <v>8773429</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>0.3</v>
@@ -3510,13 +3634,13 @@
         <v>30</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
@@ -3524,7 +3648,7 @@
         <v>8773428</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>0.3</v>
@@ -3542,13 +3666,13 @@
         <v>30</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
@@ -3556,7 +3680,7 @@
         <v>8773794</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>0.3</v>
@@ -3574,19 +3698,19 @@
         <v>30</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K15" s="7">
         <v>0.64</v>
       </c>
       <c r="L15" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" t="s">
         <v>69</v>
-      </c>
-      <c r="N15" t="s">
-        <v>70</v>
-      </c>
-      <c r="O15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
@@ -3594,7 +3718,7 @@
         <v>8773772</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>0.3</v>
@@ -3612,19 +3736,19 @@
         <v>30</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K16" s="7">
         <v>0.64</v>
       </c>
       <c r="L16" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" t="s">
         <v>69</v>
-      </c>
-      <c r="N16" t="s">
-        <v>70</v>
-      </c>
-      <c r="O16" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -3632,7 +3756,7 @@
         <v>8775647</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>0.3</v>
@@ -3650,13 +3774,13 @@
         <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -3664,7 +3788,7 @@
         <v>8775648</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>0.3</v>
@@ -3682,13 +3806,13 @@
         <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -3696,7 +3820,7 @@
         <v>8775782</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>0.03</v>
@@ -3714,7 +3838,7 @@
         <v>100</v>
       </c>
       <c r="H19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I19">
         <v>28</v>
@@ -3723,7 +3847,7 @@
         <v>0.64810000000000001</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -3731,7 +3855,7 @@
         <v>8775783</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>0.03</v>
@@ -3749,7 +3873,7 @@
         <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I20">
         <v>46</v>
@@ -3758,7 +3882,7 @@
         <v>0.64690000000000003</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -3766,7 +3890,7 @@
         <v>8776347</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>0.03</v>
@@ -3784,7 +3908,7 @@
         <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I21">
         <v>24</v>
@@ -3793,7 +3917,7 @@
         <v>0.6331</v>
       </c>
       <c r="L21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -3801,7 +3925,7 @@
         <v>8782883</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>0.03</v>
@@ -3819,7 +3943,7 @@
         <v>100</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I22">
         <v>4</v>
@@ -3833,7 +3957,7 @@
         <v>8784006</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23">
         <v>0.03</v>
@@ -3851,7 +3975,7 @@
         <v>100</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -3859,7 +3983,7 @@
         <v>8784007</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C24">
         <v>0.03</v>
@@ -3877,7 +4001,7 @@
         <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3885,7 +4009,7 @@
         <v>8836483</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="9">
         <v>0.03</v>
@@ -3903,7 +4027,7 @@
         <v>100</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I25" s="9">
         <v>94</v>
@@ -3912,7 +4036,7 @@
         <v>0.80400000000000005</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3920,7 +4044,7 @@
         <v>8836482</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C26" s="9">
         <v>0.03</v>
@@ -3938,7 +4062,7 @@
         <v>100</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I26" s="9">
         <v>99</v>
@@ -3952,7 +4076,7 @@
         <v>8836484</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C27" s="9">
         <v>0.03</v>
@@ -3970,7 +4094,7 @@
         <v>100</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I27" s="9">
         <v>89</v>
@@ -3984,7 +4108,7 @@
         <v>8836485</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" s="9">
         <v>0.03</v>
@@ -4002,7 +4126,7 @@
         <v>100</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I28" s="9">
         <v>99</v>
@@ -4016,7 +4140,7 @@
         <v>8837319</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="20">
         <v>0.03</v>
@@ -4034,7 +4158,7 @@
         <v>100</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I29" s="20">
         <v>114</v>
@@ -4048,7 +4172,7 @@
         <v>8837321</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C30" s="20">
         <v>0.03</v>
@@ -4066,7 +4190,7 @@
         <v>100</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I30" s="20">
         <v>59</v>
@@ -4080,7 +4204,7 @@
         <v>8837322</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C31" s="20">
         <v>0.03</v>
@@ -4098,7 +4222,7 @@
         <v>100</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I31" s="20">
         <v>59</v>
@@ -4112,7 +4236,7 @@
         <v>8837323</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C32" s="20">
         <v>0.03</v>
@@ -4130,7 +4254,7 @@
         <v>100</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I32" s="20">
         <v>114</v>
@@ -4144,7 +4268,7 @@
         <v>8838183</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C33" s="21">
         <v>0.01</v>
@@ -4162,7 +4286,7 @@
         <v>200</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -4170,7 +4294,7 @@
         <v>8838185</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="21">
         <v>0.01</v>
@@ -4188,7 +4312,7 @@
         <v>200</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -4196,7 +4320,7 @@
         <v>8851279</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" s="20">
         <v>0.01</v>
@@ -4214,7 +4338,7 @@
         <v>200</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I35" s="20">
         <v>84</v>
@@ -4228,7 +4352,7 @@
         <v>8851280</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="20">
         <v>0.01</v>
@@ -4246,7 +4370,7 @@
         <v>200</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I36" s="20">
         <v>184</v>
@@ -4260,7 +4384,7 @@
         <v>8851281</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" s="20">
         <v>0.01</v>
@@ -4278,7 +4402,7 @@
         <v>200</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I37" s="20">
         <v>194</v>
@@ -4292,7 +4416,7 @@
         <v>8855877</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C38" s="20">
         <v>0.01</v>
@@ -4310,7 +4434,7 @@
         <v>200</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I38" s="20">
         <v>54</v>
@@ -4324,7 +4448,7 @@
         <v>8855878</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" s="20">
         <v>0.01</v>
@@ -4342,7 +4466,7 @@
         <v>200</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I39" s="20">
         <v>99</v>
@@ -4356,7 +4480,7 @@
         <v>8855876</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="20">
         <v>0.01</v>
@@ -4374,7 +4498,7 @@
         <v>200</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I40" s="20">
         <v>119</v>
@@ -4388,7 +4512,7 @@
         <v>8855875</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C41" s="20">
         <v>0.01</v>
@@ -4406,7 +4530,7 @@
         <v>200</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I41" s="20">
         <v>124</v>
@@ -4420,7 +4544,7 @@
         <v>8861303</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42" s="20">
         <v>0.01</v>
@@ -4438,7 +4562,7 @@
         <v>200</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I42" s="20"/>
     </row>
@@ -4447,7 +4571,7 @@
         <v>8861304</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="20">
         <v>0.01</v>
@@ -4465,7 +4589,7 @@
         <v>200</v>
       </c>
       <c r="H43" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I43" s="20"/>
     </row>
@@ -4474,7 +4598,7 @@
         <v>8861305</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C44" s="20">
         <v>0.01</v>
@@ -4492,7 +4616,7 @@
         <v>200</v>
       </c>
       <c r="H44" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I44" s="20"/>
     </row>
@@ -4501,7 +4625,7 @@
         <v>8890426</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C45" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4519,7 +4643,7 @@
         <v>200</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I45" s="34">
         <v>38</v>
@@ -4533,7 +4657,7 @@
         <v>8890517</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4551,7 +4675,7 @@
         <v>200</v>
       </c>
       <c r="H46" s="34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I46" s="34">
         <v>25</v>
@@ -4565,7 +4689,7 @@
         <v>8890518</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C47" s="44">
         <v>2.9999999999999997E-4</v>
@@ -4583,10 +4707,10 @@
         <v>200</v>
       </c>
       <c r="H47" s="44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L47" s="44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -4594,7 +4718,7 @@
         <v>8890519</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C48" s="44">
         <v>2.9999999999999997E-4</v>
@@ -4612,10 +4736,10 @@
         <v>200</v>
       </c>
       <c r="H48" s="44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L48" s="44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -4623,7 +4747,7 @@
         <v>8891498</v>
       </c>
       <c r="B49" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C49" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4641,7 +4765,7 @@
         <v>200</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I49" s="34">
         <v>71</v>
@@ -4655,7 +4779,7 @@
         <v>8891500</v>
       </c>
       <c r="B50" s="44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C50" s="44">
         <v>2.9999999999999997E-4</v>
@@ -4673,10 +4797,10 @@
         <v>200</v>
       </c>
       <c r="H50" s="44" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L50" s="44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -4684,7 +4808,7 @@
         <v>8892012</v>
       </c>
       <c r="B51" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C51" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4702,7 +4826,7 @@
         <v>200</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I51" s="34">
         <v>62</v>
@@ -4716,7 +4840,7 @@
         <v>8892013</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C52" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4734,7 +4858,7 @@
         <v>200</v>
       </c>
       <c r="H52" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I52" s="34">
         <v>56</v>
@@ -4748,7 +4872,7 @@
         <v>8891997</v>
       </c>
       <c r="B53" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C53" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4766,7 +4890,7 @@
         <v>200</v>
       </c>
       <c r="H53" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I53" s="34">
         <v>92</v>
@@ -4780,7 +4904,7 @@
         <v>8892881</v>
       </c>
       <c r="B54" s="34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C54" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4798,7 +4922,7 @@
         <v>200</v>
       </c>
       <c r="H54" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I54" s="34">
         <v>156</v>
@@ -4812,7 +4936,7 @@
         <v>8892879</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C55" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4830,7 +4954,7 @@
         <v>200</v>
       </c>
       <c r="H55" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I55" s="34">
         <v>92</v>
@@ -4844,7 +4968,7 @@
         <v>8892956</v>
       </c>
       <c r="B56" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C56" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4862,7 +4986,7 @@
         <v>200</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I56" s="34">
         <v>121</v>
@@ -4876,7 +5000,7 @@
         <v>8892957</v>
       </c>
       <c r="B57" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C57" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4894,7 +5018,7 @@
         <v>200</v>
       </c>
       <c r="H57" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I57" s="34">
         <v>129</v>
@@ -4908,7 +5032,7 @@
         <v>8894359</v>
       </c>
       <c r="B58" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C58" s="34">
         <v>2.9999999999999997E-4</v>
@@ -4926,7 +5050,7 @@
         <v>200</v>
       </c>
       <c r="H58" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I58" s="34">
         <v>62</v>
@@ -4940,7 +5064,7 @@
         <v>8894360</v>
       </c>
       <c r="B59" s="44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C59" s="44">
         <v>2.9999999999999997E-4</v>
@@ -4958,10 +5082,10 @@
         <v>200</v>
       </c>
       <c r="H59" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L59" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -4969,7 +5093,7 @@
         <v>8894361</v>
       </c>
       <c r="B60" s="44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C60" s="44">
         <v>2.9999999999999997E-4</v>
@@ -4987,10 +5111,10 @@
         <v>200</v>
       </c>
       <c r="H60" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L60" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -4998,7 +5122,7 @@
         <v>8894362</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C61" s="34">
         <v>2.9999999999999997E-4</v>
@@ -5016,7 +5140,7 @@
         <v>200</v>
       </c>
       <c r="H61" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I61" s="34">
         <v>73</v>
@@ -5030,7 +5154,7 @@
         <v>8894678</v>
       </c>
       <c r="B62" s="44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C62" s="44">
         <v>1E-4</v>
@@ -5048,10 +5172,10 @@
         <v>200</v>
       </c>
       <c r="H62" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L62" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -5059,7 +5183,7 @@
         <v>8894677</v>
       </c>
       <c r="B63" s="44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C63" s="44">
         <v>1E-4</v>
@@ -5077,10 +5201,10 @@
         <v>200</v>
       </c>
       <c r="H63" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L63" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -5088,7 +5212,7 @@
         <v>8894676</v>
       </c>
       <c r="B64" s="44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C64" s="44">
         <v>1E-3</v>
@@ -5106,10 +5230,10 @@
         <v>200</v>
       </c>
       <c r="H64" s="44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L64" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:35" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -5117,7 +5241,7 @@
         <v>8894675</v>
       </c>
       <c r="B65" s="44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C65" s="44">
         <v>1E-3</v>
@@ -5135,10 +5259,10 @@
         <v>200</v>
       </c>
       <c r="H65" s="44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L65" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5146,7 +5270,7 @@
         <v>8908438</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C66" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5164,13 +5288,13 @@
         <v>200</v>
       </c>
       <c r="H66" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I66" s="9">
         <v>39</v>
       </c>
       <c r="L66" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5178,7 +5302,7 @@
         <v>8908439</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C67" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5196,10 +5320,10 @@
         <v>200</v>
       </c>
       <c r="H67" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="L67" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="L67" s="9" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5207,7 +5331,7 @@
         <v>8908441</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C68" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5225,13 +5349,13 @@
         <v>200</v>
       </c>
       <c r="H68" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I68" s="9">
         <v>17</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -5239,7 +5363,7 @@
         <v>8908440</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C69" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5257,7 +5381,7 @@
         <v>200</v>
       </c>
       <c r="H69" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.2">
@@ -5265,7 +5389,7 @@
         <v>8910616</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C70" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5283,7 +5407,7 @@
         <v>200</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
@@ -5318,7 +5442,7 @@
         <v>8910618</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C71" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5336,7 +5460,7 @@
         <v>200</v>
       </c>
       <c r="H71" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
@@ -5371,7 +5495,7 @@
         <v>8910792</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C72" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5389,7 +5513,7 @@
         <v>200</v>
       </c>
       <c r="H72" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
@@ -5424,7 +5548,7 @@
         <v>8910797</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C73" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5442,7 +5566,7 @@
         <v>200</v>
       </c>
       <c r="H73" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
@@ -5477,7 +5601,7 @@
         <v>8910798</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C74" s="9">
         <v>2.9999999999999997E-4</v>
@@ -5495,7 +5619,7 @@
         <v>200</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
@@ -5530,7 +5654,7 @@
         <v>8910799</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C75" s="16">
         <v>2.9999999999999997E-4</v>
@@ -5548,7 +5672,7 @@
         <v>200</v>
       </c>
       <c r="H75" s="16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
@@ -5620,22 +5744,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -5645,7 +5769,7 @@
         <v>8857317</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C2" s="13">
         <v>0.01</v>
@@ -5674,7 +5798,7 @@
       </c>
       <c r="L2" s="27"/>
       <c r="M2" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N2" s="5"/>
     </row>
@@ -5683,7 +5807,7 @@
         <v>8857726</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" s="13">
         <v>1E-3</v>
@@ -5711,7 +5835,7 @@
         <v>228.8038</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -5719,7 +5843,7 @@
         <v>8857843</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13">
         <v>1E-4</v>
@@ -5747,7 +5871,7 @@
         <v>253.19319999999999</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -5755,7 +5879,7 @@
         <v>8858089</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" s="13">
         <v>1.0000000000000001E-5</v>
@@ -5783,7 +5907,7 @@
         <v>271.25310000000002</v>
       </c>
       <c r="M5" s="25" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -5791,7 +5915,7 @@
         <v>8858108</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6" s="23">
         <v>0.01</v>
@@ -5812,7 +5936,7 @@
         <v>1</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -5820,7 +5944,7 @@
         <v>8858347</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="23">
         <v>1E-3</v>
@@ -5847,7 +5971,7 @@
         <v>248.65</v>
       </c>
       <c r="M7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -5855,7 +5979,7 @@
         <v>8858348</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="23">
         <v>1E-4</v>
@@ -5882,7 +6006,7 @@
         <v>249.9675</v>
       </c>
       <c r="M8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -5890,7 +6014,7 @@
         <v>8859036</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" s="23">
         <v>0.01</v>
@@ -5915,7 +6039,7 @@
         <v>235.17</v>
       </c>
       <c r="M9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -5923,7 +6047,7 @@
         <v>8860382</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" s="23">
         <v>0.01</v>
@@ -5950,7 +6074,7 @@
         <v>8899275</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" s="52">
         <v>1E-4</v>
@@ -5972,7 +6096,7 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -5980,7 +6104,7 @@
         <v>8903282</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C12" s="52">
         <v>1E-4</v>
@@ -6012,7 +6136,7 @@
         <v>8914629</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C13" s="52">
         <v>1E-4</v>
@@ -6023,7 +6147,7 @@
       <c r="E13" s="53">
         <v>128</v>
       </c>
-      <c r="F13" s="79">
+      <c r="F13" s="54">
         <v>5</v>
       </c>
       <c r="G13" s="55" t="b">
@@ -6044,7 +6168,7 @@
         <v>8915820</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" s="52">
         <v>1E-4</v>
@@ -6055,7 +6179,7 @@
       <c r="E14" s="53">
         <v>128</v>
       </c>
-      <c r="F14" s="79">
+      <c r="F14" s="54">
         <v>5</v>
       </c>
       <c r="G14" s="55" t="b">
@@ -6068,7 +6192,7 @@
         <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -6107,22 +6231,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="2"/>
     </row>
@@ -6131,7 +6255,7 @@
         <v>8914630</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="52">
         <v>1E-4</v>
@@ -6196,22 +6320,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="2"/>
     </row>
@@ -6220,7 +6344,7 @@
         <v>8914631</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="52">
         <v>1E-4</v>
@@ -6288,22 +6412,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="29"/>
     </row>
@@ -6312,7 +6436,7 @@
         <v>8859060</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23">
         <v>0.01</v>
@@ -6339,7 +6463,7 @@
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="30" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6347,7 +6471,7 @@
         <v>8860416</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="23">
         <v>0.01</v>
@@ -6373,7 +6497,7 @@
       <c r="K3" s="28"/>
       <c r="L3" s="28"/>
       <c r="M3" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6381,7 +6505,7 @@
         <v>8914574</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4">
         <v>1E-4</v>
@@ -6446,22 +6570,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="2"/>
     </row>
@@ -6470,7 +6594,7 @@
         <v>8859128</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="60">
         <v>0.01</v>
@@ -6499,7 +6623,7 @@
         <v>0.74560000000000004</v>
       </c>
       <c r="M2" s="61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -6507,7 +6631,7 @@
         <v>8860385</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" s="60">
         <v>0.01</v>
@@ -6531,7 +6655,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
@@ -6539,7 +6663,7 @@
         <v>8899274</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" s="64">
         <v>1E-4</v>
@@ -6563,7 +6687,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="61" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6571,7 +6695,7 @@
         <v>8900559</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F5">
         <v>79</v>
@@ -6594,7 +6718,7 @@
         <v>8914675</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6">
         <v>6</v>
@@ -6612,7 +6736,7 @@
         <v>0.8266</v>
       </c>
       <c r="M6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -6656,22 +6780,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="26" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -6679,7 +6803,7 @@
         <v>8859127</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23">
         <v>0.01</v>
@@ -6708,7 +6832,7 @@
         <v>0.68789999999999996</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6716,7 +6840,7 @@
         <v>8860384</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="23">
         <v>0.01</v>
@@ -6740,7 +6864,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6748,7 +6872,7 @@
         <v>8897293</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" s="23">
         <v>0.01</v>
@@ -6775,7 +6899,7 @@
         <v>0.71530000000000005</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6783,7 +6907,7 @@
         <v>8897746</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="23">
         <v>1E-3</v>
@@ -6810,7 +6934,7 @@
         <v>0.71530000000000005</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -6818,7 +6942,7 @@
         <v>8897747</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C6" s="23">
         <v>1E-4</v>
@@ -6845,7 +6969,7 @@
         <v>0.86380000000000001</v>
       </c>
       <c r="M6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -6853,7 +6977,7 @@
         <v>8900562</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7" s="23">
         <v>1E-4</v>
@@ -6877,7 +7001,7 @@
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -6885,7 +7009,7 @@
         <v>8901570</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C8" s="76">
         <v>1E-4</v>
@@ -6917,7 +7041,7 @@
         <v>8914674</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C9" s="76">
         <v>1E-4</v>
@@ -6944,7 +7068,7 @@
         <v>0.89970000000000006</v>
       </c>
       <c r="M9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -6986,22 +7110,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H1" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="49" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="50" t="s">
         <v>109</v>
-      </c>
-      <c r="K1" s="50" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="51"/>
     </row>
@@ -7010,7 +7134,7 @@
         <v>8899123</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="52">
         <v>1E-4</v>
@@ -7037,7 +7161,7 @@
         <v>0.85660000000000003</v>
       </c>
       <c r="M2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -7045,7 +7169,7 @@
         <v>8900561</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C3" s="52">
         <v>1E-4</v>
@@ -7069,7 +7193,7 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -7077,7 +7201,7 @@
         <v>8901571</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" s="70">
         <v>1E-4</v>
@@ -7109,7 +7233,7 @@
         <v>8915168</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C5" s="70">
         <v>1E-4</v>
@@ -7146,7 +7270,7 @@
   <dimension ref="A1:AI49"/>
   <sheetViews>
     <sheetView topLeftCell="A32" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7182,10 +7306,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>7</v>
@@ -7221,7 +7345,7 @@
         <v>8544579</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="8">
         <v>0.03</v>
@@ -7239,7 +7363,7 @@
         <v>50</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -7250,7 +7374,7 @@
         <v>8548727</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8">
         <v>3.0000000000000001E-3</v>
@@ -7276,7 +7400,7 @@
         <v>8618521</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8">
         <v>0.03</v>
@@ -7294,7 +7418,7 @@
         <v>50</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -7305,7 +7429,7 @@
         <v>8630046</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="35">
         <v>0.03</v>
@@ -7323,7 +7447,7 @@
         <v>100</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
@@ -7334,7 +7458,7 @@
         <v>8643007</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="6">
         <v>0.03</v>
@@ -7352,7 +7476,7 @@
         <v>100</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
@@ -7360,7 +7484,7 @@
         <v>8643330</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" s="6">
         <v>0.03</v>
@@ -7383,7 +7507,7 @@
         <v>8704485</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6">
         <v>3.0000000000000001E-3</v>
@@ -7401,7 +7525,7 @@
         <v>100</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.2">
@@ -7409,7 +7533,7 @@
         <v>8704666</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="6">
         <v>2.9999999999999997E-4</v>
@@ -7432,7 +7556,7 @@
         <v>8714665</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8">
         <v>3.0000000000000001E-3</v>
@@ -7450,10 +7574,10 @@
         <v>100</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -7464,7 +7588,7 @@
         <v>8714947</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="8">
         <v>0.03</v>
@@ -7490,7 +7614,7 @@
         <v>8715114</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6">
         <v>3</v>
@@ -7513,7 +7637,7 @@
         <v>8719970</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="6">
         <v>30</v>
@@ -7536,7 +7660,7 @@
         <v>8725293</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" s="6">
         <v>0.03</v>
@@ -7554,10 +7678,10 @@
         <v>100</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
@@ -7565,7 +7689,7 @@
         <v>8727149</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="6">
         <v>0.3</v>
@@ -7583,7 +7707,7 @@
         <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
@@ -7591,7 +7715,7 @@
         <v>8733913</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C16" s="6">
         <v>0.3</v>
@@ -7609,10 +7733,10 @@
         <v>100</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -7620,7 +7744,7 @@
         <v>8735495</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C17" s="6">
         <v>0.03</v>
@@ -7638,7 +7762,7 @@
         <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -7646,7 +7770,7 @@
         <v>8736656</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6">
         <v>0.3</v>
@@ -7664,7 +7788,7 @@
         <v>100</v>
       </c>
       <c r="H18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -7672,7 +7796,7 @@
         <v>8741212</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6">
         <v>0.03</v>
@@ -7690,15 +7814,15 @@
         <v>300</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="6">
         <v>0.03</v>
@@ -7716,10 +7840,10 @@
         <v>300</v>
       </c>
       <c r="H20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -7727,7 +7851,7 @@
         <v>8751286</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6">
         <v>0.03</v>
@@ -7745,13 +7869,13 @@
         <v>300</v>
       </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -7759,7 +7883,7 @@
         <v>8760687</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="6">
         <v>0.03</v>
@@ -7777,10 +7901,10 @@
         <v>300</v>
       </c>
       <c r="H22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -7788,7 +7912,7 @@
         <v>8761020</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C23" s="6">
         <v>0.03</v>
@@ -7806,10 +7930,10 @@
         <v>300</v>
       </c>
       <c r="H23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.2">
@@ -7817,7 +7941,7 @@
         <v>8763825</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C24" s="37">
         <v>0.03</v>
@@ -7835,7 +7959,7 @@
         <v>300</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J24" s="37"/>
       <c r="K24" s="37"/>
@@ -7846,7 +7970,7 @@
         <v>8763833</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C25" s="6">
         <v>0.03</v>
@@ -7864,7 +7988,7 @@
         <v>300</v>
       </c>
       <c r="H25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -7872,7 +7996,7 @@
         <v>8763845</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C26" s="6">
         <v>0.03</v>
@@ -7890,7 +8014,7 @@
         <v>300</v>
       </c>
       <c r="H26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -7898,7 +8022,7 @@
         <v>8764388</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="6">
         <v>0.03</v>
@@ -7916,7 +8040,7 @@
         <v>300</v>
       </c>
       <c r="H27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -7924,7 +8048,7 @@
         <v>8775747</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" s="6">
         <v>0.03</v>
@@ -7942,10 +8066,10 @@
         <v>480</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -7953,7 +8077,7 @@
         <v>8776341</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="6">
         <v>0.3</v>
@@ -7971,7 +8095,7 @@
         <v>500</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -7979,7 +8103,7 @@
         <v>8782858</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="6">
         <v>0.3</v>
@@ -7997,7 +8121,7 @@
         <v>500</v>
       </c>
       <c r="H30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -8005,7 +8129,7 @@
         <v>8783455</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31" s="6">
         <v>0.03</v>
@@ -8023,7 +8147,7 @@
         <v>500</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -8031,7 +8155,7 @@
         <v>8786623</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C32" s="6">
         <v>3</v>
@@ -8049,7 +8173,7 @@
         <v>500</v>
       </c>
       <c r="H32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -8057,7 +8181,7 @@
         <v>8850812</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="6">
         <v>0.3</v>
@@ -8075,7 +8199,7 @@
         <v>500</v>
       </c>
       <c r="H33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -8083,7 +8207,7 @@
         <v>8850814</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34" s="6">
         <v>3</v>
@@ -8101,7 +8225,7 @@
         <v>500</v>
       </c>
       <c r="H34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -8109,7 +8233,7 @@
         <v>8852324</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C35" s="6">
         <v>0.3</v>
@@ -8132,7 +8256,7 @@
         <v>8852325</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36" s="6">
         <v>3</v>
@@ -8155,7 +8279,7 @@
         <v>8852525</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C37" s="6">
         <v>3</v>
@@ -8178,7 +8302,7 @@
         <v>8858578</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" s="6">
         <v>3</v>
@@ -8201,7 +8325,7 @@
         <v>8878103</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C39" s="39">
         <v>0.03</v>
@@ -8219,7 +8343,7 @@
         <v>100</v>
       </c>
       <c r="I39" s="34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J39" s="39"/>
       <c r="K39" s="39"/>
@@ -8230,7 +8354,7 @@
         <v>8878104</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C40" s="39">
         <v>0.03</v>
@@ -8256,7 +8380,7 @@
         <v>8893496</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C41" s="39">
         <v>0.3</v>
@@ -8280,7 +8404,7 @@
         <v>8893498</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C42" s="39">
         <v>0.3</v>
@@ -8304,7 +8428,7 @@
         <v>8897030</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C43" s="39">
         <v>0.03</v>
@@ -8330,7 +8454,7 @@
         <v>8899242</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C44" s="39">
         <v>0.3</v>
@@ -8346,7 +8470,7 @@
       </c>
       <c r="G44" s="39"/>
       <c r="I44" s="34" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J44" s="39"/>
       <c r="K44" s="39"/>
@@ -8357,7 +8481,7 @@
         <v>8905233</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C45" s="39">
         <v>0.3</v>

</xml_diff>

<commit_message>
add MoCo version selection in MoCoClf and MoCoClf_train
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bolin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E899C16-016F-FE4E-BA9D-45FDFDB903F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18B225C0-19D4-2C47-B5C3-4780FA4A5889}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="820" windowWidth="20720" windowHeight="9040" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="1800" yWindow="620" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="195">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -584,6 +584,51 @@
   </si>
   <si>
     <t>Res50-noFC-100-4 + sce3</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV2</t>
+  </si>
+  <si>
+    <t>8899242_600</t>
+  </si>
+  <si>
+    <t>8899242_660</t>
+  </si>
+  <si>
+    <t>8899242_680</t>
+  </si>
+  <si>
+    <t>8905233_800</t>
+  </si>
+  <si>
+    <t>8905233_880</t>
+  </si>
+  <si>
+    <t>Ord MoCo (alpha=2, exp, with color jitter)</t>
+  </si>
+  <si>
+    <t>LabelMoCo (with color jitter)</t>
+  </si>
+  <si>
+    <t>trivial solutiion</t>
+  </si>
+  <si>
+    <t>trivial solution</t>
+  </si>
+  <si>
+    <t>260, 400, 480</t>
+  </si>
+  <si>
+    <t>discarded</t>
+  </si>
+  <si>
+    <t>9031422_480</t>
+  </si>
+  <si>
+    <t>9031422_400</t>
+  </si>
+  <si>
+    <t>9031422_260</t>
   </si>
 </sst>
 </file>
@@ -613,7 +658,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,6 +725,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -741,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -921,6 +972,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="125" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -3201,16 +3275,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI75"/>
+  <dimension ref="A1:AI83"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" zoomScale="139" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="139" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
@@ -5702,6 +5776,214 @@
       <c r="AH75" s="9"/>
       <c r="AI75" s="9"/>
     </row>
+    <row r="76" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A76" s="9">
+        <v>9028624</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D76" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="16">
+        <v>128</v>
+      </c>
+      <c r="F76" s="9">
+        <v>1</v>
+      </c>
+      <c r="G76" s="9">
+        <v>50</v>
+      </c>
+      <c r="H76" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A77" s="9">
+        <v>9028626</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C77" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D77" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" s="16">
+        <v>128</v>
+      </c>
+      <c r="F77" s="9">
+        <v>1</v>
+      </c>
+      <c r="G77" s="9">
+        <v>50</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A78" s="16">
+        <v>9028627</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C78" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D78" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" s="16">
+        <v>128</v>
+      </c>
+      <c r="F78" s="9">
+        <v>1</v>
+      </c>
+      <c r="G78" s="9">
+        <v>50</v>
+      </c>
+      <c r="H78" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="79" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A79" s="16">
+        <v>9028628</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D79" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" s="16">
+        <v>128</v>
+      </c>
+      <c r="F79" s="9">
+        <v>1</v>
+      </c>
+      <c r="G79" s="9">
+        <v>50</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="80" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A80" s="16">
+        <v>9028629</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D80" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" s="16">
+        <v>128</v>
+      </c>
+      <c r="F80" s="9">
+        <v>1</v>
+      </c>
+      <c r="G80" s="9">
+        <v>50</v>
+      </c>
+      <c r="H80" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="87">
+        <v>9052142</v>
+      </c>
+      <c r="B81" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C81" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D81" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" s="87">
+        <v>128</v>
+      </c>
+      <c r="F81" s="34">
+        <v>1</v>
+      </c>
+      <c r="G81" s="34">
+        <v>50</v>
+      </c>
+      <c r="H81" s="34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="87">
+        <v>9052143</v>
+      </c>
+      <c r="B82" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C82" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D82" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="87">
+        <v>128</v>
+      </c>
+      <c r="F82" s="34">
+        <v>1</v>
+      </c>
+      <c r="G82" s="34">
+        <v>50</v>
+      </c>
+      <c r="H82" s="34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="87">
+        <v>9052145</v>
+      </c>
+      <c r="B83" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C83" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D83" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="87">
+        <v>128</v>
+      </c>
+      <c r="F83" s="34">
+        <v>1</v>
+      </c>
+      <c r="G83" s="34">
+        <v>50</v>
+      </c>
+      <c r="H83" s="34" t="s">
+        <v>194</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7267,23 +7549,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI49"/>
+  <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A21" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="56.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="29" style="6" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="37" style="11" customWidth="1"/>
+    <col min="4" max="5" width="8.33203125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="6" style="6" customWidth="1"/>
+    <col min="8" max="8" width="5.5" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" customWidth="1"/>
     <col min="10" max="10" width="19" style="6" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" style="6" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="6" customWidth="1"/>
@@ -7296,7 +7577,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -7347,7 +7628,7 @@
       <c r="B2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="82">
         <v>0.03</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -7376,7 +7657,7 @@
       <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="82">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -7402,7 +7683,7 @@
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="82">
         <v>0.03</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -7431,7 +7712,7 @@
       <c r="B5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="83">
         <v>0.03</v>
       </c>
       <c r="D5" s="35" t="s">
@@ -7460,7 +7741,7 @@
       <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="11">
         <v>0.03</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -7486,7 +7767,7 @@
       <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="11">
         <v>0.03</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -7509,7 +7790,7 @@
       <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="11">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -7535,7 +7816,7 @@
       <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="11">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -7558,7 +7839,7 @@
       <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="82">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -7590,7 +7871,7 @@
       <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="82">
         <v>0.03</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -7616,7 +7897,7 @@
       <c r="B12" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="11">
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
@@ -7639,7 +7920,7 @@
       <c r="B13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="11">
         <v>30</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -7662,7 +7943,7 @@
       <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="11">
         <v>0.03</v>
       </c>
       <c r="D14" s="6" t="s">
@@ -7691,7 +7972,7 @@
       <c r="B15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="11">
         <v>0.3</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -7717,7 +7998,7 @@
       <c r="B16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="11">
         <v>0.3</v>
       </c>
       <c r="D16" s="6" t="s">
@@ -7746,7 +8027,7 @@
       <c r="B17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="11">
         <v>0.03</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -7772,7 +8053,7 @@
       <c r="B18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="11">
         <v>0.3</v>
       </c>
       <c r="D18" s="6" t="s">
@@ -7798,7 +8079,7 @@
       <c r="B19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="11">
         <v>0.03</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -7824,7 +8105,7 @@
       <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="11">
         <v>0.03</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -7853,7 +8134,7 @@
       <c r="B21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="11">
         <v>0.03</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -7885,7 +8166,7 @@
       <c r="B22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="11">
         <v>0.03</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -7914,7 +8195,7 @@
       <c r="B23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="11">
         <v>0.03</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -7943,7 +8224,7 @@
       <c r="B24" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="84">
         <v>0.03</v>
       </c>
       <c r="D24" s="37" t="s">
@@ -7972,7 +8253,7 @@
       <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="11">
         <v>0.03</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -7998,7 +8279,7 @@
       <c r="B26" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="11">
         <v>0.03</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -8024,7 +8305,7 @@
       <c r="B27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="11">
         <v>0.03</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -8050,7 +8331,7 @@
       <c r="B28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="11">
         <v>0.03</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -8079,7 +8360,7 @@
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="11">
         <v>0.3</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -8105,7 +8386,7 @@
       <c r="B30" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="11">
         <v>0.3</v>
       </c>
       <c r="D30" s="6" t="s">
@@ -8131,7 +8412,7 @@
       <c r="B31" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="11">
         <v>0.03</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -8157,7 +8438,7 @@
       <c r="B32" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="11">
         <v>3</v>
       </c>
       <c r="D32" s="6" t="s">
@@ -8183,7 +8464,7 @@
       <c r="B33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="11">
         <v>0.3</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -8209,7 +8490,7 @@
       <c r="B34" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="11">
         <v>3</v>
       </c>
       <c r="D34" s="6" t="s">
@@ -8235,7 +8516,7 @@
       <c r="B35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="11">
         <v>0.3</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -8255,97 +8536,99 @@
       <c r="A36" s="6">
         <v>8852325</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="6">
+      <c r="D36" s="6">
         <v>3</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="6">
-        <v>128</v>
+      <c r="E36" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="F36" s="6">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G36" s="6">
+        <v>1</v>
+      </c>
+      <c r="H36" s="6">
         <v>500</v>
       </c>
+      <c r="J36"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>8852525</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="6">
+      <c r="D37" s="6">
         <v>3</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="6">
-        <v>128</v>
+      <c r="E37" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="F37" s="6">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G37" s="6">
+        <v>1</v>
+      </c>
+      <c r="H37" s="6">
         <v>500</v>
       </c>
+      <c r="J37"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>8858578</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="C38" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="6">
+      <c r="D38" s="6">
         <v>3</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="6">
-        <v>128</v>
+      <c r="E38" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="F38" s="6">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G38" s="6">
+        <v>1</v>
+      </c>
+      <c r="H38" s="6">
         <v>500</v>
       </c>
+      <c r="J38"/>
     </row>
     <row r="39" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32">
         <v>8878103</v>
       </c>
-      <c r="B39" s="39" t="s">
+      <c r="C39" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="39">
+      <c r="D39" s="39">
         <v>0.03</v>
       </c>
-      <c r="D39" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="39">
-        <v>128</v>
+      <c r="E39" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F39" s="39">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G39" s="39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="39">
         <v>100</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="J39" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="J39" s="39"/>
       <c r="K39" s="39"/>
       <c r="L39" s="39"/>
     </row>
@@ -8353,25 +8636,24 @@
       <c r="A40" s="32">
         <v>8878104</v>
       </c>
-      <c r="B40" s="39" t="s">
+      <c r="C40" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="39">
+      <c r="D40" s="39">
         <v>0.03</v>
       </c>
-      <c r="D40" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="39">
-        <v>128</v>
+      <c r="E40" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F40" s="39">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G40" s="39">
+        <v>1</v>
+      </c>
+      <c r="H40" s="39">
         <v>300</v>
       </c>
-      <c r="J40" s="39"/>
       <c r="K40" s="39"/>
       <c r="L40" s="39"/>
     </row>
@@ -8379,23 +8661,22 @@
       <c r="A41" s="39">
         <v>8893496</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="C41" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="39">
+      <c r="D41" s="39">
         <v>0.3</v>
       </c>
-      <c r="D41" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="39">
-        <v>128</v>
+      <c r="E41" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F41" s="39">
-        <v>1</v>
-      </c>
-      <c r="G41" s="39"/>
-      <c r="J41" s="39"/>
+        <v>128</v>
+      </c>
+      <c r="G41" s="39">
+        <v>1</v>
+      </c>
+      <c r="H41" s="39"/>
       <c r="K41" s="39"/>
       <c r="L41" s="39"/>
     </row>
@@ -8403,23 +8684,22 @@
       <c r="A42" s="39">
         <v>8893498</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="C42" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="39">
+      <c r="D42" s="39">
         <v>0.3</v>
       </c>
-      <c r="D42" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="39">
-        <v>128</v>
+      <c r="E42" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F42" s="39">
-        <v>1</v>
-      </c>
-      <c r="G42" s="39"/>
-      <c r="J42" s="39"/>
+        <v>128</v>
+      </c>
+      <c r="G42" s="39">
+        <v>1</v>
+      </c>
+      <c r="H42" s="39"/>
       <c r="K42" s="39"/>
       <c r="L42" s="39"/>
     </row>
@@ -8427,25 +8707,24 @@
       <c r="A43" s="39">
         <v>8897030</v>
       </c>
-      <c r="B43" s="39" t="s">
+      <c r="C43" s="85" t="s">
         <v>150</v>
       </c>
-      <c r="C43" s="39">
+      <c r="D43" s="39">
         <v>0.03</v>
       </c>
-      <c r="D43" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="39">
-        <v>128</v>
+      <c r="E43" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F43" s="39">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G43" s="39">
+        <v>1</v>
+      </c>
+      <c r="H43" s="39">
         <v>300</v>
       </c>
-      <c r="J43" s="39"/>
       <c r="K43" s="39"/>
       <c r="L43" s="39"/>
     </row>
@@ -8453,26 +8732,25 @@
       <c r="A44" s="39">
         <v>8899242</v>
       </c>
-      <c r="B44" s="39" t="s">
+      <c r="C44" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="C44" s="39">
+      <c r="D44" s="39">
         <v>0.3</v>
       </c>
-      <c r="D44" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="39">
-        <v>128</v>
+      <c r="E44" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F44" s="39">
-        <v>1</v>
-      </c>
-      <c r="G44" s="39"/>
-      <c r="I44" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="G44" s="39">
+        <v>1</v>
+      </c>
+      <c r="H44" s="39"/>
+      <c r="J44" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="J44" s="39"/>
       <c r="K44" s="39"/>
       <c r="L44" s="39"/>
     </row>
@@ -8480,73 +8758,164 @@
       <c r="A45" s="39">
         <v>8905233</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="C45" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="39">
+      <c r="D45" s="39">
         <v>0.3</v>
       </c>
-      <c r="D45" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="39">
-        <v>128</v>
+      <c r="E45" s="39" t="s">
+        <v>5</v>
       </c>
       <c r="F45" s="39">
-        <v>1</v>
-      </c>
-      <c r="G45" s="39"/>
-      <c r="J45" s="39"/>
+        <v>128</v>
+      </c>
+      <c r="G45" s="39">
+        <v>1</v>
+      </c>
+      <c r="H45" s="39"/>
       <c r="K45" s="39"/>
       <c r="L45" s="39"/>
     </row>
     <row r="46" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="A46" s="39">
+        <v>9031422</v>
+      </c>
+      <c r="C46" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" s="39">
+        <v>0.3</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" s="39">
+        <v>128</v>
+      </c>
+      <c r="G46" s="39">
+        <v>1</v>
+      </c>
+      <c r="H46" s="39"/>
+      <c r="J46" s="34" t="s">
+        <v>190</v>
+      </c>
       <c r="K46" s="39"/>
       <c r="L46" s="39"/>
     </row>
-    <row r="47" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="39"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
+    <row r="47" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="79">
+        <v>9031424</v>
+      </c>
+      <c r="C47" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="79">
+        <v>0.3</v>
+      </c>
+      <c r="E47" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="79">
+        <v>128</v>
+      </c>
+      <c r="G47" s="79">
+        <v>1</v>
+      </c>
+      <c r="H47" s="79"/>
+      <c r="J47" s="80" t="s">
+        <v>188</v>
+      </c>
+      <c r="K47" s="79"/>
+      <c r="L47" s="79"/>
     </row>
     <row r="48" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="39"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="J48" s="39"/>
+      <c r="A48" s="39">
+        <v>9031633</v>
+      </c>
+      <c r="C48" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="39">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="39">
+        <v>128</v>
+      </c>
+      <c r="G48" s="39">
+        <v>1</v>
+      </c>
+      <c r="H48" s="39"/>
+      <c r="J48" s="34" t="s">
+        <v>191</v>
+      </c>
       <c r="K48" s="39"/>
       <c r="L48" s="39"/>
     </row>
-    <row r="49" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
+    <row r="49" spans="1:20" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="79">
+        <v>9031630</v>
+      </c>
+      <c r="C49" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="D49" s="79">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E49" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="F49" s="79">
+        <v>128</v>
+      </c>
+      <c r="G49" s="79">
+        <v>1</v>
+      </c>
+      <c r="H49" s="79"/>
+      <c r="J49" s="80" t="s">
+        <v>189</v>
+      </c>
+      <c r="K49" s="79"/>
+      <c r="L49" s="79"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>9052126</v>
+      </c>
+      <c r="B50" s="81">
+        <v>44964</v>
+      </c>
+      <c r="C50" s="85" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50" s="39">
+        <v>30</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="39">
+        <v>128</v>
+      </c>
+      <c r="G50" s="39">
+        <v>1</v>
+      </c>
+      <c r="H50" s="39"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="34"/>
+      <c r="N50" s="34"/>
+      <c r="O50" s="34"/>
+      <c r="P50" s="34"/>
+      <c r="Q50" s="34"/>
+      <c r="R50" s="34"/>
+      <c r="S50" s="34"/>
+      <c r="T50" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update MoCoV3 such that we discard the trained projection layer in MoCo
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18B225C0-19D4-2C47-B5C3-4780FA4A5889}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50F66937-1F89-7740-88CB-E9A21405FC20}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="620" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="196">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t>9031422_260</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3</t>
   </si>
 </sst>
 </file>
@@ -3275,10 +3278,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI83"/>
+  <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:XFD83"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="139" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5981,6 +5984,78 @@
         <v>50</v>
       </c>
       <c r="H83" s="34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B84" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C84" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D84" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" s="87">
+        <v>128</v>
+      </c>
+      <c r="F84" s="34">
+        <v>1</v>
+      </c>
+      <c r="G84" s="34">
+        <v>50</v>
+      </c>
+      <c r="H84" s="34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D85" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="87">
+        <v>128</v>
+      </c>
+      <c r="F85" s="34">
+        <v>1</v>
+      </c>
+      <c r="G85" s="34">
+        <v>50</v>
+      </c>
+      <c r="H85" s="34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="87">
+        <v>9060799</v>
+      </c>
+      <c r="B86" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D86" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="87">
+        <v>128</v>
+      </c>
+      <c r="F86" s="34">
+        <v>1</v>
+      </c>
+      <c r="G86" s="34">
+        <v>50</v>
+      </c>
+      <c r="H86" s="34" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added autoaug to LabelMoCoDataset
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50F66937-1F89-7740-88CB-E9A21405FC20}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2363DC36-65A0-D64A-98E6-42D8ADC065BC}"/>
   <bookViews>
-    <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -3280,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="139" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5988,6 +5988,9 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="87">
+        <v>9062085</v>
+      </c>
       <c r="B84" s="34" t="s">
         <v>195</v>
       </c>
@@ -6011,6 +6014,9 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="87">
+        <v>9062086</v>
+      </c>
       <c r="B85" s="34" t="s">
         <v>195</v>
       </c>
@@ -6035,7 +6041,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="87">
-        <v>9060799</v>
+        <v>9062088</v>
       </c>
       <c r="B86" s="34" t="s">
         <v>195</v>
@@ -7626,7 +7632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="156" workbookViewId="0">
+    <sheetView topLeftCell="A36" zoomScale="156" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update linear projector in MoCo models
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2363DC36-65A0-D64A-98E6-42D8ADC065BC}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B770AB9C-76D8-554B-8AC1-32A3AF95FAF1}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="197">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>OrdMoCoClfV3</t>
+  </si>
+  <si>
+    <t>MoCo (projector)</t>
   </si>
 </sst>
 </file>
@@ -3280,7 +3283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="139" workbookViewId="0">
+    <sheetView topLeftCell="A66" zoomScale="139" workbookViewId="0">
       <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
@@ -7630,10 +7633,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI50"/>
+  <dimension ref="A1:AI51"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="156" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8998,6 +9001,29 @@
       <c r="S50" s="34"/>
       <c r="T50" s="34"/>
     </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>9062591</v>
+      </c>
+      <c r="B51" s="81">
+        <v>44969</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" s="39">
+        <v>30</v>
+      </c>
+      <c r="E51" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="39">
+        <v>128</v>
+      </c>
+      <c r="G51" s="39">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update MoCoClfV3 according to the updated MoCo class (with normalization and flatten before linear projector)
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B770AB9C-76D8-554B-8AC1-32A3AF95FAF1}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CF2AAB4-D941-5140-B50E-89C94AF4C2B2}"/>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="205">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -635,6 +635,30 @@
   </si>
   <si>
     <t>MoCo (projector)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">looks very similar to 9062591, terminated, restart from 9062591 </t>
+  </si>
+  <si>
+    <t>looks good</t>
+  </si>
+  <si>
+    <t>unstable, training loss not decreaseing</t>
+  </si>
+  <si>
+    <t>MoCo (projector, start from 9052126_190)</t>
+  </si>
+  <si>
+    <t>still decreasing, restart from 190 below</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector)</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector)</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, start from 9063219_190)</t>
   </si>
 </sst>
 </file>
@@ -3283,8 +3307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI86"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="139" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView topLeftCell="A72" zoomScale="139" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7633,10 +7657,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI51"/>
+  <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="156" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7649,7 +7673,7 @@
     <col min="7" max="7" width="6" style="6" customWidth="1"/>
     <col min="8" max="8" width="5.5" customWidth="1"/>
     <col min="9" max="9" width="5.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19" style="6" customWidth="1"/>
+    <col min="10" max="10" width="19" style="11" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" style="6" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="6" customWidth="1"/>
   </cols>
@@ -7680,7 +7704,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="10"/>
-      <c r="J1" s="2"/>
+      <c r="J1" s="29"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -7730,7 +7754,7 @@
       <c r="H2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="82"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
     </row>
@@ -7756,7 +7780,7 @@
       <c r="G3" s="8">
         <v>50</v>
       </c>
-      <c r="J3" s="8"/>
+      <c r="J3" s="82"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
     </row>
@@ -7785,7 +7809,7 @@
       <c r="H4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="82"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
     </row>
@@ -7814,7 +7838,7 @@
       <c r="H5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="35"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="35"/>
       <c r="L5" s="35"/>
     </row>
@@ -7944,7 +7968,7 @@
       <c r="I10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="8"/>
+      <c r="J10" s="82"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
     </row>
@@ -7970,7 +7994,7 @@
       <c r="G11" s="8">
         <v>100</v>
       </c>
-      <c r="J11" s="8"/>
+      <c r="J11" s="82"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
@@ -8239,7 +8263,7 @@
       <c r="I21" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="11" t="s">
         <v>51</v>
       </c>
     </row>
@@ -8326,7 +8350,7 @@
       <c r="H24" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="37"/>
+      <c r="J24" s="84"/>
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
     </row>
@@ -8638,7 +8662,6 @@
       <c r="H36" s="6">
         <v>500</v>
       </c>
-      <c r="J36"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
@@ -8662,7 +8685,6 @@
       <c r="H37" s="6">
         <v>500</v>
       </c>
-      <c r="J37"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
@@ -8686,7 +8708,6 @@
       <c r="H38" s="6">
         <v>500</v>
       </c>
-      <c r="J38"/>
     </row>
     <row r="39" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32">
@@ -8710,7 +8731,7 @@
       <c r="H39" s="39">
         <v>100</v>
       </c>
-      <c r="J39" s="34" t="s">
+      <c r="J39" s="85" t="s">
         <v>122</v>
       </c>
       <c r="K39" s="39"/>
@@ -8738,6 +8759,7 @@
       <c r="H40" s="39">
         <v>300</v>
       </c>
+      <c r="J40" s="85"/>
       <c r="K40" s="39"/>
       <c r="L40" s="39"/>
     </row>
@@ -8761,6 +8783,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="39"/>
+      <c r="J41" s="85"/>
       <c r="K41" s="39"/>
       <c r="L41" s="39"/>
     </row>
@@ -8784,6 +8807,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="39"/>
+      <c r="J42" s="85"/>
       <c r="K42" s="39"/>
       <c r="L42" s="39"/>
     </row>
@@ -8809,6 +8833,7 @@
       <c r="H43" s="39">
         <v>300</v>
       </c>
+      <c r="J43" s="85"/>
       <c r="K43" s="39"/>
       <c r="L43" s="39"/>
     </row>
@@ -8832,7 +8857,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="39"/>
-      <c r="J44" s="34" t="s">
+      <c r="J44" s="85" t="s">
         <v>164</v>
       </c>
       <c r="K44" s="39"/>
@@ -8858,6 +8883,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="39"/>
+      <c r="J45" s="85"/>
       <c r="K45" s="39"/>
       <c r="L45" s="39"/>
     </row>
@@ -8881,7 +8907,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="39"/>
-      <c r="J46" s="34" t="s">
+      <c r="J46" s="85" t="s">
         <v>190</v>
       </c>
       <c r="K46" s="39"/>
@@ -8907,7 +8933,7 @@
         <v>1</v>
       </c>
       <c r="H47" s="79"/>
-      <c r="J47" s="80" t="s">
+      <c r="J47" s="86" t="s">
         <v>188</v>
       </c>
       <c r="K47" s="79"/>
@@ -8933,7 +8959,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="39"/>
-      <c r="J48" s="34" t="s">
+      <c r="J48" s="85" t="s">
         <v>191</v>
       </c>
       <c r="K48" s="39"/>
@@ -8959,7 +8985,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="79"/>
-      <c r="J49" s="80" t="s">
+      <c r="J49" s="86" t="s">
         <v>189</v>
       </c>
       <c r="K49" s="79"/>
@@ -8989,7 +9015,7 @@
       </c>
       <c r="H50" s="39"/>
       <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
+      <c r="J50" s="85"/>
       <c r="K50" s="39"/>
       <c r="L50" s="39"/>
       <c r="M50" s="34"/>
@@ -9023,6 +9049,136 @@
       <c r="G51" s="39">
         <v>1</v>
       </c>
+      <c r="J51" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>9062616</v>
+      </c>
+      <c r="B52" s="81">
+        <v>44969</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D52" s="39">
+        <v>30</v>
+      </c>
+      <c r="E52" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="39">
+        <v>128</v>
+      </c>
+      <c r="G52" s="39">
+        <v>1</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>9063219</v>
+      </c>
+      <c r="B53" s="81">
+        <v>44970</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D53" s="39">
+        <v>30</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="39">
+        <v>128</v>
+      </c>
+      <c r="G53" s="39">
+        <v>1</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>9067187</v>
+      </c>
+      <c r="B54" s="81">
+        <v>44971</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D54" s="39">
+        <v>0.03</v>
+      </c>
+      <c r="E54" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="39">
+        <v>128</v>
+      </c>
+      <c r="G54" s="39">
+        <v>1</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>9069292</v>
+      </c>
+      <c r="B55" s="81">
+        <v>44972</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D55" s="39">
+        <v>0.03</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F55" s="39">
+        <v>128</v>
+      </c>
+      <c r="G55" s="39">
+        <v>1</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>9069293</v>
+      </c>
+      <c r="B56" s="81">
+        <v>44972</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="39">
+        <v>30</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" s="39">
+        <v>128</v>
+      </c>
+      <c r="G56" s="39">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update the model initialization function in functions to include MoCoClfV3 as an option
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CF2AAB4-D941-5140-B50E-89C94AF4C2B2}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66E52563-D83C-D145-BA53-D25EAB526EA5}"/>
   <bookViews>
-    <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="208">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -659,6 +659,15 @@
   </si>
   <si>
     <t>OrdMoCo (projector, start from 9063219_190)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3</t>
+  </si>
+  <si>
+    <t>9062616_170</t>
+  </si>
+  <si>
+    <t>9063219_140</t>
   </si>
 </sst>
 </file>
@@ -688,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -761,6 +770,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -822,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1025,6 +1046,26 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3305,10 +3346,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI86"/>
+  <dimension ref="A1:AI88"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" zoomScale="139" workbookViewId="0">
-      <selection activeCell="H90" sqref="H90"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="139" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3320,7 +3361,7 @@
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14" style="11" customWidth="1"/>
     <col min="9" max="9" width="6" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3346,7 +3387,7 @@
       <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="90" t="s">
         <v>19</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -3407,7 +3448,7 @@
       <c r="G2">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="I2" t="s">
@@ -3438,7 +3479,7 @@
       <c r="G3">
         <v>50</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J3" s="7">
@@ -3473,7 +3514,7 @@
       <c r="G4">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="11" t="s">
         <v>27</v>
       </c>
       <c r="L4" t="s">
@@ -3502,7 +3543,7 @@
       <c r="G5">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="11" t="s">
         <v>26</v>
       </c>
       <c r="L5" t="s">
@@ -3531,7 +3572,7 @@
       <c r="G6">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="11" t="s">
         <v>26</v>
       </c>
       <c r="L6" t="s">
@@ -3560,7 +3601,7 @@
       <c r="G7">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="11" t="s">
         <v>26</v>
       </c>
       <c r="L7" t="s">
@@ -3589,7 +3630,7 @@
       <c r="G8">
         <v>50</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3615,7 +3656,7 @@
       <c r="G9">
         <v>50</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="11" t="s">
         <v>48</v>
       </c>
       <c r="L9" t="s">
@@ -3644,7 +3685,7 @@
       <c r="G10">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="11" t="s">
         <v>48</v>
       </c>
       <c r="L10" t="s">
@@ -3673,7 +3714,7 @@
       <c r="G11">
         <v>50</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="11" t="s">
         <v>60</v>
       </c>
       <c r="L11" t="s">
@@ -3705,7 +3746,7 @@
       <c r="G12">
         <v>30</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L12" t="s">
@@ -3737,7 +3778,7 @@
       <c r="G13">
         <v>30</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="11" t="s">
         <v>60</v>
       </c>
       <c r="L13" t="s">
@@ -3769,7 +3810,7 @@
       <c r="G14">
         <v>30</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L14" t="s">
@@ -3801,7 +3842,7 @@
       <c r="G15">
         <v>30</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="K15" s="7">
@@ -3839,7 +3880,7 @@
       <c r="G16">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="11" t="s">
         <v>61</v>
       </c>
       <c r="K16" s="7">
@@ -3877,7 +3918,7 @@
       <c r="G17">
         <v>100</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="11" t="s">
         <v>60</v>
       </c>
       <c r="L17" t="s">
@@ -3909,7 +3950,7 @@
       <c r="G18">
         <v>100</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="11" t="s">
         <v>61</v>
       </c>
       <c r="L18" t="s">
@@ -3941,7 +3982,7 @@
       <c r="G19">
         <v>100</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="11" t="s">
         <v>60</v>
       </c>
       <c r="I19">
@@ -3976,7 +4017,7 @@
       <c r="G20">
         <v>100</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="11" t="s">
         <v>61</v>
       </c>
       <c r="I20">
@@ -4011,7 +4052,7 @@
       <c r="G21">
         <v>100</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="11" t="s">
         <v>27</v>
       </c>
       <c r="I21">
@@ -4078,7 +4119,7 @@
       <c r="G23">
         <v>100</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4104,7 +4145,7 @@
       <c r="G24">
         <v>100</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4130,7 +4171,7 @@
       <c r="G25" s="9">
         <v>100</v>
       </c>
-      <c r="H25" s="9" t="s">
+      <c r="H25" s="82" t="s">
         <v>61</v>
       </c>
       <c r="I25" s="9">
@@ -4165,7 +4206,7 @@
       <c r="G26" s="9">
         <v>100</v>
       </c>
-      <c r="H26" s="9" t="s">
+      <c r="H26" s="82" t="s">
         <v>27</v>
       </c>
       <c r="I26" s="9">
@@ -4197,7 +4238,7 @@
       <c r="G27" s="9">
         <v>100</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="82" t="s">
         <v>61</v>
       </c>
       <c r="I27" s="9">
@@ -4229,7 +4270,7 @@
       <c r="G28" s="9">
         <v>100</v>
       </c>
-      <c r="H28" s="9" t="s">
+      <c r="H28" s="82" t="s">
         <v>27</v>
       </c>
       <c r="I28" s="9">
@@ -4261,7 +4302,7 @@
       <c r="G29" s="20">
         <v>100</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="91" t="s">
         <v>61</v>
       </c>
       <c r="I29" s="20">
@@ -4293,7 +4334,7 @@
       <c r="G30" s="20">
         <v>100</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="91" t="s">
         <v>27</v>
       </c>
       <c r="I30" s="20">
@@ -4325,7 +4366,7 @@
       <c r="G31" s="20">
         <v>100</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="91" t="s">
         <v>27</v>
       </c>
       <c r="I31" s="20">
@@ -4357,7 +4398,7 @@
       <c r="G32" s="20">
         <v>100</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="91" t="s">
         <v>61</v>
       </c>
       <c r="I32" s="20">
@@ -4389,7 +4430,7 @@
       <c r="G33" s="21">
         <v>200</v>
       </c>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="92" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4415,7 +4456,7 @@
       <c r="G34" s="21">
         <v>200</v>
       </c>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="92" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4441,7 +4482,7 @@
       <c r="G35" s="20">
         <v>200</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="91" t="s">
         <v>97</v>
       </c>
       <c r="I35" s="20">
@@ -4473,7 +4514,7 @@
       <c r="G36" s="20">
         <v>200</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="91" t="s">
         <v>97</v>
       </c>
       <c r="I36" s="20">
@@ -4505,7 +4546,7 @@
       <c r="G37" s="20">
         <v>200</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="91" t="s">
         <v>97</v>
       </c>
       <c r="I37" s="20">
@@ -4537,7 +4578,7 @@
       <c r="G38" s="20">
         <v>200</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="91" t="s">
         <v>101</v>
       </c>
       <c r="I38" s="20">
@@ -4569,7 +4610,7 @@
       <c r="G39" s="20">
         <v>200</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="91" t="s">
         <v>102</v>
       </c>
       <c r="I39" s="20">
@@ -4601,7 +4642,7 @@
       <c r="G40" s="20">
         <v>200</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="91" t="s">
         <v>101</v>
       </c>
       <c r="I40" s="20">
@@ -4633,7 +4674,7 @@
       <c r="G41" s="20">
         <v>200</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="91" t="s">
         <v>102</v>
       </c>
       <c r="I41" s="20">
@@ -4665,7 +4706,7 @@
       <c r="G42" s="20">
         <v>200</v>
       </c>
-      <c r="H42" s="20" t="s">
+      <c r="H42" s="91" t="s">
         <v>120</v>
       </c>
       <c r="I42" s="20"/>
@@ -4692,7 +4733,7 @@
       <c r="G43" s="20">
         <v>200</v>
       </c>
-      <c r="H43" s="20" t="s">
+      <c r="H43" s="91" t="s">
         <v>120</v>
       </c>
       <c r="I43" s="20"/>
@@ -4719,7 +4760,7 @@
       <c r="G44" s="20">
         <v>200</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="91" t="s">
         <v>120</v>
       </c>
       <c r="I44" s="20"/>
@@ -4746,7 +4787,7 @@
       <c r="G45" s="34">
         <v>200</v>
       </c>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="85" t="s">
         <v>128</v>
       </c>
       <c r="I45" s="34">
@@ -4778,7 +4819,7 @@
       <c r="G46" s="34">
         <v>200</v>
       </c>
-      <c r="H46" s="34" t="s">
+      <c r="H46" s="85" t="s">
         <v>129</v>
       </c>
       <c r="I46" s="34">
@@ -4810,7 +4851,7 @@
       <c r="G47" s="44">
         <v>200</v>
       </c>
-      <c r="H47" s="44" t="s">
+      <c r="H47" s="93" t="s">
         <v>131</v>
       </c>
       <c r="L47" s="44" t="s">
@@ -4839,7 +4880,7 @@
       <c r="G48" s="44">
         <v>200</v>
       </c>
-      <c r="H48" s="44" t="s">
+      <c r="H48" s="93" t="s">
         <v>132</v>
       </c>
       <c r="L48" s="44" t="s">
@@ -4868,7 +4909,7 @@
       <c r="G49" s="34">
         <v>200</v>
       </c>
-      <c r="H49" s="34" t="s">
+      <c r="H49" s="85" t="s">
         <v>131</v>
       </c>
       <c r="I49" s="34">
@@ -4900,7 +4941,7 @@
       <c r="G50" s="44">
         <v>200</v>
       </c>
-      <c r="H50" s="44" t="s">
+      <c r="H50" s="93" t="s">
         <v>128</v>
       </c>
       <c r="L50" s="44" t="s">
@@ -4929,7 +4970,7 @@
       <c r="G51" s="34">
         <v>200</v>
       </c>
-      <c r="H51" s="34" t="s">
+      <c r="H51" s="85" t="s">
         <v>131</v>
       </c>
       <c r="I51" s="34">
@@ -4961,7 +5002,7 @@
       <c r="G52" s="34">
         <v>200</v>
       </c>
-      <c r="H52" s="34" t="s">
+      <c r="H52" s="85" t="s">
         <v>132</v>
       </c>
       <c r="I52" s="34">
@@ -4993,7 +5034,7 @@
       <c r="G53" s="34">
         <v>200</v>
       </c>
-      <c r="H53" s="34" t="s">
+      <c r="H53" s="85" t="s">
         <v>128</v>
       </c>
       <c r="I53" s="34">
@@ -5025,7 +5066,7 @@
       <c r="G54" s="34">
         <v>200</v>
       </c>
-      <c r="H54" s="34" t="s">
+      <c r="H54" s="85" t="s">
         <v>131</v>
       </c>
       <c r="I54" s="34">
@@ -5057,7 +5098,7 @@
       <c r="G55" s="34">
         <v>200</v>
       </c>
-      <c r="H55" s="34" t="s">
+      <c r="H55" s="85" t="s">
         <v>128</v>
       </c>
       <c r="I55" s="34">
@@ -5089,7 +5130,7 @@
       <c r="G56" s="34">
         <v>200</v>
       </c>
-      <c r="H56" s="34" t="s">
+      <c r="H56" s="85" t="s">
         <v>131</v>
       </c>
       <c r="I56" s="34">
@@ -5121,7 +5162,7 @@
       <c r="G57" s="34">
         <v>200</v>
       </c>
-      <c r="H57" s="34" t="s">
+      <c r="H57" s="85" t="s">
         <v>128</v>
       </c>
       <c r="I57" s="34">
@@ -5153,7 +5194,7 @@
       <c r="G58" s="34">
         <v>200</v>
       </c>
-      <c r="H58" s="34" t="s">
+      <c r="H58" s="85" t="s">
         <v>147</v>
       </c>
       <c r="I58" s="34">
@@ -5185,7 +5226,7 @@
       <c r="G59" s="44">
         <v>200</v>
       </c>
-      <c r="H59" s="44" t="s">
+      <c r="H59" s="93" t="s">
         <v>148</v>
       </c>
       <c r="L59" s="44" t="s">
@@ -5214,7 +5255,7 @@
       <c r="G60" s="44">
         <v>200</v>
       </c>
-      <c r="H60" s="44" t="s">
+      <c r="H60" s="93" t="s">
         <v>148</v>
       </c>
       <c r="L60" s="44" t="s">
@@ -5243,7 +5284,7 @@
       <c r="G61" s="34">
         <v>200</v>
       </c>
-      <c r="H61" s="34" t="s">
+      <c r="H61" s="85" t="s">
         <v>147</v>
       </c>
       <c r="I61" s="34">
@@ -5275,7 +5316,7 @@
       <c r="G62" s="44">
         <v>200</v>
       </c>
-      <c r="H62" s="44" t="s">
+      <c r="H62" s="93" t="s">
         <v>148</v>
       </c>
       <c r="L62" s="44" t="s">
@@ -5304,7 +5345,7 @@
       <c r="G63" s="44">
         <v>200</v>
       </c>
-      <c r="H63" s="44" t="s">
+      <c r="H63" s="93" t="s">
         <v>148</v>
       </c>
       <c r="L63" s="44" t="s">
@@ -5333,7 +5374,7 @@
       <c r="G64" s="44">
         <v>200</v>
       </c>
-      <c r="H64" s="44" t="s">
+      <c r="H64" s="93" t="s">
         <v>131</v>
       </c>
       <c r="L64" s="44" t="s">
@@ -5362,7 +5403,7 @@
       <c r="G65" s="44">
         <v>200</v>
       </c>
-      <c r="H65" s="44" t="s">
+      <c r="H65" s="93" t="s">
         <v>131</v>
       </c>
       <c r="L65" s="44" t="s">
@@ -5391,7 +5432,7 @@
       <c r="G66" s="9">
         <v>200</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="H66" s="82" t="s">
         <v>166</v>
       </c>
       <c r="I66" s="9">
@@ -5423,7 +5464,7 @@
       <c r="G67" s="9">
         <v>200</v>
       </c>
-      <c r="H67" s="9" t="s">
+      <c r="H67" s="82" t="s">
         <v>166</v>
       </c>
       <c r="L67" s="9" t="s">
@@ -5452,7 +5493,7 @@
       <c r="G68" s="9">
         <v>200</v>
       </c>
-      <c r="H68" s="9" t="s">
+      <c r="H68" s="82" t="s">
         <v>167</v>
       </c>
       <c r="I68" s="9">
@@ -5484,7 +5525,7 @@
       <c r="G69" s="9">
         <v>200</v>
       </c>
-      <c r="H69" s="9" t="s">
+      <c r="H69" s="82" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5510,7 +5551,7 @@
       <c r="G70" s="9">
         <v>200</v>
       </c>
-      <c r="H70" s="9" t="s">
+      <c r="H70" s="82" t="s">
         <v>169</v>
       </c>
       <c r="I70" s="9"/>
@@ -5563,7 +5604,7 @@
       <c r="G71" s="9">
         <v>200</v>
       </c>
-      <c r="H71" s="9" t="s">
+      <c r="H71" s="82" t="s">
         <v>170</v>
       </c>
       <c r="I71" s="9"/>
@@ -5616,7 +5657,7 @@
       <c r="G72" s="9">
         <v>200</v>
       </c>
-      <c r="H72" s="9" t="s">
+      <c r="H72" s="82" t="s">
         <v>171</v>
       </c>
       <c r="I72" s="9"/>
@@ -5669,7 +5710,7 @@
       <c r="G73" s="9">
         <v>200</v>
       </c>
-      <c r="H73" s="9" t="s">
+      <c r="H73" s="82" t="s">
         <v>172</v>
       </c>
       <c r="I73" s="9"/>
@@ -5722,7 +5763,7 @@
       <c r="G74" s="9">
         <v>200</v>
       </c>
-      <c r="H74" s="9" t="s">
+      <c r="H74" s="82" t="s">
         <v>173</v>
       </c>
       <c r="I74" s="9"/>
@@ -5775,7 +5816,7 @@
       <c r="G75" s="16">
         <v>200</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H75" s="94" t="s">
         <v>174</v>
       </c>
       <c r="I75" s="9"/>
@@ -5828,7 +5869,7 @@
       <c r="G76" s="9">
         <v>50</v>
       </c>
-      <c r="H76" s="9" t="s">
+      <c r="H76" s="82" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5854,7 +5895,7 @@
       <c r="G77" s="9">
         <v>50</v>
       </c>
-      <c r="H77" s="9" t="s">
+      <c r="H77" s="82" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5880,7 +5921,7 @@
       <c r="G78" s="9">
         <v>50</v>
       </c>
-      <c r="H78" s="9" t="s">
+      <c r="H78" s="82" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5906,7 +5947,7 @@
       <c r="G79" s="9">
         <v>50</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="H79" s="82" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5932,164 +5973,216 @@
       <c r="G80" s="9">
         <v>50</v>
       </c>
-      <c r="H80" s="9" t="s">
+      <c r="H80" s="82" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="87">
+    <row r="81" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="88">
         <v>9052142</v>
       </c>
-      <c r="B81" s="34" t="s">
+      <c r="B81" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C81" s="87">
+      <c r="C81" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D81" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" s="87">
-        <v>128</v>
-      </c>
-      <c r="F81" s="34">
-        <v>1</v>
-      </c>
-      <c r="G81" s="34">
+      <c r="D81" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" s="88">
+        <v>128</v>
+      </c>
+      <c r="F81" s="89">
+        <v>1</v>
+      </c>
+      <c r="G81" s="89">
         <v>50</v>
       </c>
-      <c r="H81" s="34" t="s">
+      <c r="H81" s="95" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="87">
+    <row r="82" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="88">
         <v>9052143</v>
       </c>
-      <c r="B82" s="34" t="s">
+      <c r="B82" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C82" s="87">
+      <c r="C82" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D82" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E82" s="87">
-        <v>128</v>
-      </c>
-      <c r="F82" s="34">
-        <v>1</v>
-      </c>
-      <c r="G82" s="34">
+      <c r="D82" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" s="88">
+        <v>128</v>
+      </c>
+      <c r="F82" s="89">
+        <v>1</v>
+      </c>
+      <c r="G82" s="89">
         <v>50</v>
       </c>
-      <c r="H82" s="34" t="s">
+      <c r="H82" s="95" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="87">
+    <row r="83" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="88">
         <v>9052145</v>
       </c>
-      <c r="B83" s="34" t="s">
+      <c r="B83" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C83" s="87">
+      <c r="C83" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D83" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E83" s="87">
-        <v>128</v>
-      </c>
-      <c r="F83" s="34">
-        <v>1</v>
-      </c>
-      <c r="G83" s="34">
+      <c r="D83" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="88">
+        <v>128</v>
+      </c>
+      <c r="F83" s="89">
+        <v>1</v>
+      </c>
+      <c r="G83" s="89">
         <v>50</v>
       </c>
-      <c r="H83" s="34" t="s">
+      <c r="H83" s="95" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="87">
+    <row r="84" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="88">
         <v>9062085</v>
       </c>
-      <c r="B84" s="34" t="s">
+      <c r="B84" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="C84" s="87">
+      <c r="C84" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D84" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E84" s="87">
-        <v>128</v>
-      </c>
-      <c r="F84" s="34">
-        <v>1</v>
-      </c>
-      <c r="G84" s="34">
+      <c r="D84" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" s="88">
+        <v>128</v>
+      </c>
+      <c r="F84" s="89">
+        <v>1</v>
+      </c>
+      <c r="G84" s="89">
         <v>50</v>
       </c>
-      <c r="H84" s="34" t="s">
+      <c r="H84" s="95" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="87">
+    <row r="85" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="88">
         <v>9062086</v>
       </c>
-      <c r="B85" s="34" t="s">
+      <c r="B85" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="C85" s="87">
+      <c r="C85" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D85" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E85" s="87">
-        <v>128</v>
-      </c>
-      <c r="F85" s="34">
-        <v>1</v>
-      </c>
-      <c r="G85" s="34">
+      <c r="D85" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" s="88">
+        <v>128</v>
+      </c>
+      <c r="F85" s="89">
+        <v>1</v>
+      </c>
+      <c r="G85" s="89">
         <v>50</v>
       </c>
-      <c r="H85" s="34" t="s">
+      <c r="H85" s="95" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="87">
+    <row r="86" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="88">
         <v>9062088</v>
       </c>
-      <c r="B86" s="34" t="s">
+      <c r="B86" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="C86" s="87">
+      <c r="C86" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D86" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E86" s="87">
-        <v>128</v>
-      </c>
-      <c r="F86" s="34">
-        <v>1</v>
-      </c>
-      <c r="G86" s="34">
+      <c r="D86" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" s="88">
+        <v>128</v>
+      </c>
+      <c r="F86" s="89">
+        <v>1</v>
+      </c>
+      <c r="G86" s="89">
         <v>50</v>
       </c>
-      <c r="H86" s="34" t="s">
+      <c r="H86" s="95" t="s">
         <v>194</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="87">
+        <v>9069877</v>
+      </c>
+      <c r="B87" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="C87" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D87" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="87">
+        <v>128</v>
+      </c>
+      <c r="F87" s="34">
+        <v>1</v>
+      </c>
+      <c r="G87" s="34">
+        <v>50</v>
+      </c>
+      <c r="H87" s="85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="87">
+        <v>9072918</v>
+      </c>
+      <c r="B88" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C88" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D88" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" s="87">
+        <v>128</v>
+      </c>
+      <c r="F88" s="34">
+        <v>1</v>
+      </c>
+      <c r="G88" s="34">
+        <v>50</v>
+      </c>
+      <c r="H88" s="85" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -7659,8 +7752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A44" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add MoCoCLfFeaV3 as an option
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66E52563-D83C-D145-BA53-D25EAB526EA5}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5AF1F6B-9016-BF4A-8919-881EF1BEFB82}"/>
   <bookViews>
     <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="212">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -668,6 +668,18 @@
   </si>
   <si>
     <t>9063219_140</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + n lanes + speed</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + road type one hot + cyc infras one hot + oneway</t>
+  </si>
+  <si>
+    <t>really bad performance</t>
   </si>
 </sst>
 </file>
@@ -843,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1066,6 +1078,8 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3346,63 +3360,65 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI88"/>
+  <dimension ref="A1:AI91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="139" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="139" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" customWidth="1"/>
     <col min="6" max="6" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" customWidth="1"/>
     <col min="8" max="8" width="14" style="11" customWidth="1"/>
-    <col min="9" max="9" width="6" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="I1" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -3430,65 +3446,65 @@
       <c r="A2">
         <v>8637608</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>128</v>
+      <c r="E2" t="s">
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <v>50</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="7"/>
       <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>8639430</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>128</v>
+      <c r="E3" t="s">
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>50</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="7">
+      <c r="K3" s="7">
         <v>0.6</v>
       </c>
-      <c r="K3" s="7">
+      <c r="L3" s="7">
         <v>0.42</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3496,28 +3512,28 @@
       <c r="A4">
         <v>8641783</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>128</v>
+      <c r="E4" t="s">
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>50</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3525,28 +3541,28 @@
       <c r="A5">
         <v>8641803</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>128</v>
+      <c r="E5" t="s">
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
         <v>50</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3554,28 +3570,28 @@
       <c r="A6">
         <v>8641912</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>128</v>
+      <c r="E6" t="s">
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
         <v>50</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3583,28 +3599,28 @@
       <c r="A7">
         <v>8642199</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>128</v>
+      <c r="E7" t="s">
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>50</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3612,25 +3628,25 @@
       <c r="A8">
         <v>8642862</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>128</v>
+      <c r="E8" t="s">
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>50</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3638,28 +3654,28 @@
       <c r="A9">
         <v>8757293</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>128</v>
+      <c r="E9" t="s">
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>50</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3667,28 +3683,28 @@
       <c r="A10">
         <v>8757377</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.3</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>128</v>
+      <c r="E10" t="s">
+        <v>5</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>50</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3696,31 +3712,31 @@
       <c r="A11">
         <v>8773343</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.3</v>
       </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>128</v>
+      <c r="E11" t="s">
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>50</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>63</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3728,31 +3744,31 @@
       <c r="A12">
         <v>8773369</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.3</v>
       </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>128</v>
+      <c r="E12" t="s">
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>30</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>63</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3760,31 +3776,31 @@
       <c r="A13">
         <v>8773429</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.3</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>128</v>
+      <c r="E13" t="s">
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>30</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>65</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3792,31 +3808,31 @@
       <c r="A14">
         <v>8773428</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.3</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>128</v>
+      <c r="E14" t="s">
+        <v>5</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>30</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>65</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3824,37 +3840,37 @@
       <c r="A15">
         <v>8773794</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.3</v>
       </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>128</v>
+      <c r="E15" t="s">
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>30</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="K15" s="7">
+      <c r="L15" s="7">
         <v>0.64</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>67</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>68</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3862,1522 +3878,1522 @@
       <c r="A16">
         <v>8773772</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.3</v>
       </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>128</v>
+      <c r="E16" t="s">
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>30</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K16" s="7">
+      <c r="L16" s="7">
         <v>0.64</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>67</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>68</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8775647</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>0.3</v>
       </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <v>128</v>
+      <c r="E17" t="s">
+        <v>5</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
         <v>100</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>72</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8775648</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>0.3</v>
       </c>
-      <c r="D18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18">
-        <v>128</v>
+      <c r="E18" t="s">
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
         <v>100</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>72</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8775782</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>0.03</v>
       </c>
-      <c r="D19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <v>128</v>
+      <c r="E19" t="s">
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>100</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>28</v>
       </c>
-      <c r="K19" s="12">
+      <c r="L19" s="12">
         <v>0.64810000000000001</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8775783</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>18</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>0.03</v>
       </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <v>128</v>
+      <c r="E20" t="s">
+        <v>5</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
         <v>100</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>46</v>
       </c>
-      <c r="K20" s="12">
+      <c r="L20" s="12">
         <v>0.64690000000000003</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8776347</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>0.03</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21">
-        <v>128</v>
+      <c r="E21" t="s">
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
         <v>100</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>24</v>
       </c>
-      <c r="K21" s="12">
+      <c r="L21" s="12">
         <v>0.6331</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8782883</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>0.03</v>
       </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22">
-        <v>128</v>
+      <c r="E22" t="s">
+        <v>5</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
         <v>100</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="I22" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>4</v>
       </c>
-      <c r="K22" s="12">
+      <c r="L22" s="12">
         <v>0.62539999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8784006</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>79</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>0.03</v>
       </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23">
-        <v>128</v>
+      <c r="E23" t="s">
+        <v>5</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
         <v>100</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="I23" s="11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>8784007</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>79</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>0.03</v>
       </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24">
-        <v>128</v>
+      <c r="E24" t="s">
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
         <v>100</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="I24" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>8836483</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C25" s="9">
+      <c r="D25" s="9">
         <v>0.03</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="9">
-        <v>128</v>
+      <c r="E25" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F25" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G25" s="9">
+        <v>1</v>
+      </c>
+      <c r="H25" s="9">
         <v>100</v>
       </c>
-      <c r="H25" s="82" t="s">
+      <c r="I25" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="I25" s="9">
+      <c r="J25" s="9">
         <v>94</v>
       </c>
-      <c r="K25" s="17">
+      <c r="L25" s="17">
         <v>0.80400000000000005</v>
       </c>
-      <c r="L25" s="9" t="s">
+      <c r="M25" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>8836482</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="9">
+      <c r="D26" s="9">
         <v>0.03</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="9">
-        <v>128</v>
+      <c r="E26" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F26" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G26" s="9">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9">
         <v>100</v>
       </c>
-      <c r="H26" s="82" t="s">
+      <c r="I26" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="I26" s="9">
+      <c r="J26" s="9">
         <v>99</v>
       </c>
-      <c r="K26" s="17">
+      <c r="L26" s="17">
         <v>0.80200000000000005</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>8836484</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="9">
+      <c r="D27" s="9">
         <v>0.03</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="9">
-        <v>128</v>
+      <c r="E27" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F27" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G27" s="9">
+        <v>1</v>
+      </c>
+      <c r="H27" s="9">
         <v>100</v>
       </c>
-      <c r="H27" s="82" t="s">
+      <c r="I27" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="I27" s="9">
+      <c r="J27" s="9">
         <v>89</v>
       </c>
-      <c r="K27" s="17">
+      <c r="L27" s="17">
         <v>0.6986</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="16">
         <v>8836485</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="9">
+      <c r="D28" s="9">
         <v>0.03</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="9">
-        <v>128</v>
+      <c r="E28" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F28" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G28" s="9">
+        <v>1</v>
+      </c>
+      <c r="H28" s="9">
         <v>100</v>
       </c>
-      <c r="H28" s="82" t="s">
+      <c r="I28" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="9">
+      <c r="J28" s="9">
         <v>99</v>
       </c>
-      <c r="K28" s="17">
+      <c r="L28" s="17">
         <v>0.6966</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>8837319</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="C29" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="20">
+      <c r="D29" s="20">
         <v>0.03</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="20">
-        <v>128</v>
+      <c r="E29" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F29" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G29" s="20">
+        <v>1</v>
+      </c>
+      <c r="H29" s="20">
         <v>100</v>
       </c>
-      <c r="H29" s="91" t="s">
+      <c r="I29" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="I29" s="20">
+      <c r="J29" s="20">
         <v>114</v>
       </c>
-      <c r="K29" s="22">
+      <c r="L29" s="22">
         <v>0.80900000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>8837321</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="C30" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="20">
+      <c r="D30" s="20">
         <v>0.03</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="20">
-        <v>128</v>
+      <c r="E30" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F30" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G30" s="20">
+        <v>1</v>
+      </c>
+      <c r="H30" s="20">
         <v>100</v>
       </c>
-      <c r="H30" s="91" t="s">
+      <c r="I30" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="20">
+      <c r="J30" s="20">
         <v>59</v>
       </c>
-      <c r="K30" s="22">
+      <c r="L30" s="22">
         <v>0.80369999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>8837322</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="C31" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="20">
+      <c r="D31" s="20">
         <v>0.03</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="20">
-        <v>128</v>
+      <c r="E31" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F31" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G31" s="20">
+        <v>1</v>
+      </c>
+      <c r="H31" s="20">
         <v>100</v>
       </c>
-      <c r="H31" s="91" t="s">
+      <c r="I31" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="I31" s="20">
+      <c r="J31" s="20">
         <v>59</v>
       </c>
-      <c r="K31" s="22">
+      <c r="L31" s="22">
         <v>0.6966</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>8837323</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="C32" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="20">
+      <c r="D32" s="20">
         <v>0.03</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="20">
-        <v>128</v>
+      <c r="E32" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F32" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G32" s="20">
+        <v>1</v>
+      </c>
+      <c r="H32" s="20">
         <v>100</v>
       </c>
-      <c r="H32" s="91" t="s">
+      <c r="I32" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="I32" s="20">
+      <c r="J32" s="20">
         <v>114</v>
       </c>
-      <c r="K32" s="22">
+      <c r="L32" s="22">
         <v>0.70130000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21">
         <v>8838183</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="C33" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="21">
+      <c r="D33" s="21">
         <v>0.01</v>
       </c>
-      <c r="D33" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="21">
-        <v>128</v>
+      <c r="E33" s="21" t="s">
+        <v>5</v>
       </c>
       <c r="F33" s="21">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G33" s="21">
+        <v>1</v>
+      </c>
+      <c r="H33" s="21">
         <v>200</v>
       </c>
-      <c r="H33" s="92" t="s">
+      <c r="I33" s="92" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21">
         <v>8838185</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="C34" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C34" s="21">
+      <c r="D34" s="21">
         <v>0.01</v>
       </c>
-      <c r="D34" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="21">
-        <v>128</v>
+      <c r="E34" s="21" t="s">
+        <v>5</v>
       </c>
       <c r="F34" s="21">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G34" s="21">
+        <v>1</v>
+      </c>
+      <c r="H34" s="21">
         <v>200</v>
       </c>
-      <c r="H34" s="92" t="s">
+      <c r="I34" s="92" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>8851279</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="C35" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="20">
+      <c r="D35" s="20">
         <v>0.01</v>
       </c>
-      <c r="D35" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="20">
-        <v>128</v>
+      <c r="E35" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F35" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G35" s="20">
+        <v>1</v>
+      </c>
+      <c r="H35" s="20">
         <v>200</v>
       </c>
-      <c r="H35" s="91" t="s">
+      <c r="I35" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="I35" s="20">
+      <c r="J35" s="20">
         <v>84</v>
       </c>
-      <c r="K35" s="12">
+      <c r="L35" s="12">
         <v>0.69669999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="20">
         <v>8851280</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="C36" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="20">
+      <c r="D36" s="20">
         <v>0.01</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="20">
-        <v>128</v>
+      <c r="E36" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F36" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G36" s="20">
+        <v>1</v>
+      </c>
+      <c r="H36" s="20">
         <v>200</v>
       </c>
-      <c r="H36" s="91" t="s">
+      <c r="I36" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="I36" s="20">
+      <c r="J36" s="20">
         <v>184</v>
       </c>
-      <c r="K36" s="22">
+      <c r="L36" s="22">
         <v>0.80059999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>8851281</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="C37" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="20">
+      <c r="D37" s="20">
         <v>0.01</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="20">
-        <v>128</v>
+      <c r="E37" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F37" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G37" s="20">
+        <v>1</v>
+      </c>
+      <c r="H37" s="20">
         <v>200</v>
       </c>
-      <c r="H37" s="91" t="s">
+      <c r="I37" s="91" t="s">
         <v>97</v>
       </c>
-      <c r="I37" s="20">
+      <c r="J37" s="20">
         <v>194</v>
       </c>
-      <c r="K37" s="22">
+      <c r="L37" s="22">
         <v>0.63029999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="20">
         <v>8855877</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="C38" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="20">
+      <c r="D38" s="20">
         <v>0.01</v>
       </c>
-      <c r="D38" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="20">
-        <v>128</v>
+      <c r="E38" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F38" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G38" s="20">
+        <v>1</v>
+      </c>
+      <c r="H38" s="20">
         <v>200</v>
       </c>
-      <c r="H38" s="91" t="s">
+      <c r="I38" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="I38" s="20">
+      <c r="J38" s="20">
         <v>54</v>
       </c>
-      <c r="K38" s="12" t="s">
+      <c r="L38" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <v>8855878</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="C39" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="20">
+      <c r="D39" s="20">
         <v>0.01</v>
       </c>
-      <c r="D39" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="20">
-        <v>128</v>
+      <c r="E39" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F39" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G39" s="20">
+        <v>1</v>
+      </c>
+      <c r="H39" s="20">
         <v>200</v>
       </c>
-      <c r="H39" s="91" t="s">
+      <c r="I39" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="I39" s="20">
+      <c r="J39" s="20">
         <v>99</v>
       </c>
-      <c r="K39" s="22">
+      <c r="L39" s="22">
         <v>0.58150000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>8855876</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="C40" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="20">
+      <c r="D40" s="20">
         <v>0.01</v>
       </c>
-      <c r="D40" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E40" s="20">
-        <v>128</v>
+      <c r="E40" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F40" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G40" s="20">
+        <v>1</v>
+      </c>
+      <c r="H40" s="20">
         <v>200</v>
       </c>
-      <c r="H40" s="91" t="s">
+      <c r="I40" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="I40" s="20">
+      <c r="J40" s="20">
         <v>119</v>
       </c>
-      <c r="K40" s="12">
+      <c r="L40" s="12">
         <v>0.80079999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>8855875</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="C41" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="20">
+      <c r="D41" s="20">
         <v>0.01</v>
       </c>
-      <c r="D41" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E41" s="20">
-        <v>128</v>
+      <c r="E41" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F41" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G41" s="20">
+        <v>1</v>
+      </c>
+      <c r="H41" s="20">
         <v>200</v>
       </c>
-      <c r="H41" s="91" t="s">
+      <c r="I41" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="I41" s="20">
+      <c r="J41" s="20">
         <v>124</v>
       </c>
-      <c r="K41" s="12">
+      <c r="L41" s="12">
         <v>0.79479999999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>8861303</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="C42" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C42" s="20">
+      <c r="D42" s="20">
         <v>0.01</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="20">
-        <v>128</v>
+      <c r="E42" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F42" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G42" s="20">
+        <v>1</v>
+      </c>
+      <c r="H42" s="20">
         <v>200</v>
       </c>
-      <c r="H42" s="91" t="s">
+      <c r="I42" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="I42" s="20"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <v>8861304</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="C43" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="20">
+      <c r="D43" s="20">
         <v>0.01</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="20">
-        <v>128</v>
+      <c r="E43" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F43" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G43" s="20">
+        <v>1</v>
+      </c>
+      <c r="H43" s="20">
         <v>200</v>
       </c>
-      <c r="H43" s="91" t="s">
+      <c r="I43" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="I43" s="20"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <v>8861305</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="C44" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="20">
+      <c r="D44" s="20">
         <v>0.01</v>
       </c>
-      <c r="D44" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E44" s="20">
-        <v>128</v>
+      <c r="E44" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="F44" s="20">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G44" s="20">
+        <v>1</v>
+      </c>
+      <c r="H44" s="20">
         <v>200</v>
       </c>
-      <c r="H44" s="91" t="s">
+      <c r="I44" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="I44" s="20"/>
-    </row>
-    <row r="45" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="34">
         <v>8890426</v>
       </c>
-      <c r="B45" s="34" t="s">
+      <c r="C45" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="34">
+      <c r="D45" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D45" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="34">
-        <v>128</v>
+      <c r="E45" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F45" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G45" s="34">
+        <v>1</v>
+      </c>
+      <c r="H45" s="34">
         <v>200</v>
       </c>
-      <c r="H45" s="85" t="s">
-        <v>128</v>
-      </c>
-      <c r="I45" s="34">
+      <c r="I45" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="J45" s="34">
         <v>38</v>
       </c>
-      <c r="K45" s="47">
+      <c r="L45" s="47">
         <v>0.58679999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="34">
         <v>8890517</v>
       </c>
-      <c r="B46" s="34" t="s">
+      <c r="C46" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="34">
+      <c r="D46" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D46" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="34">
-        <v>128</v>
+      <c r="E46" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F46" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G46" s="34">
+        <v>1</v>
+      </c>
+      <c r="H46" s="34">
         <v>200</v>
       </c>
-      <c r="H46" s="85" t="s">
+      <c r="I46" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="I46" s="34">
+      <c r="J46" s="34">
         <v>25</v>
       </c>
-      <c r="K46" s="47">
+      <c r="L46" s="47">
         <v>0.58009999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="44">
         <v>8890518</v>
       </c>
-      <c r="B47" s="44" t="s">
+      <c r="C47" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="44">
+      <c r="D47" s="44">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D47" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="44">
-        <v>128</v>
+      <c r="E47" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F47" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G47" s="44">
+        <v>1</v>
+      </c>
+      <c r="H47" s="44">
         <v>200</v>
       </c>
-      <c r="H47" s="93" t="s">
+      <c r="I47" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="L47" s="44" t="s">
+      <c r="M47" s="44" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="46">
         <v>8890519</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="C48" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="44">
+      <c r="D48" s="44">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D48" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="44">
-        <v>128</v>
+      <c r="E48" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F48" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G48" s="44">
+        <v>1</v>
+      </c>
+      <c r="H48" s="44">
         <v>200</v>
       </c>
-      <c r="H48" s="93" t="s">
+      <c r="I48" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="L48" s="44" t="s">
+      <c r="M48" s="44" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="34">
         <v>8891498</v>
       </c>
-      <c r="B49" s="34" t="s">
+      <c r="C49" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C49" s="34">
+      <c r="D49" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D49" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="34">
-        <v>128</v>
+      <c r="E49" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F49" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G49" s="34">
+        <v>1</v>
+      </c>
+      <c r="H49" s="34">
         <v>200</v>
       </c>
-      <c r="H49" s="85" t="s">
+      <c r="I49" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="I49" s="34">
+      <c r="J49" s="34">
         <v>71</v>
       </c>
-      <c r="K49" s="47">
+      <c r="L49" s="47">
         <v>0.80759999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44">
         <v>8891500</v>
       </c>
-      <c r="B50" s="44" t="s">
+      <c r="C50" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="C50" s="44">
+      <c r="D50" s="44">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D50" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E50" s="44">
-        <v>128</v>
+      <c r="E50" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F50" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G50" s="44">
+        <v>1</v>
+      </c>
+      <c r="H50" s="44">
         <v>200</v>
       </c>
-      <c r="H50" s="93" t="s">
-        <v>128</v>
-      </c>
-      <c r="L50" s="44" t="s">
+      <c r="I50" s="93" t="s">
+        <v>128</v>
+      </c>
+      <c r="M50" s="44" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34">
         <v>8892012</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="C51" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="34">
+      <c r="D51" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D51" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="34">
-        <v>128</v>
+      <c r="E51" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F51" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G51" s="34">
+        <v>1</v>
+      </c>
+      <c r="H51" s="34">
         <v>200</v>
       </c>
-      <c r="H51" s="85" t="s">
+      <c r="I51" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="I51" s="34">
+      <c r="J51" s="34">
         <v>62</v>
       </c>
-      <c r="K51" s="47">
+      <c r="L51" s="47">
         <v>0.63360000000000005</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34">
         <v>8892013</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="C52" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="34">
+      <c r="D52" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D52" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="34">
-        <v>128</v>
+      <c r="E52" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F52" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G52" s="34">
+        <v>1</v>
+      </c>
+      <c r="H52" s="34">
         <v>200</v>
       </c>
-      <c r="H52" s="85" t="s">
+      <c r="I52" s="85" t="s">
         <v>132</v>
       </c>
-      <c r="I52" s="34">
+      <c r="J52" s="34">
         <v>56</v>
       </c>
-      <c r="K52" s="47">
+      <c r="L52" s="47">
         <v>0.61980000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34">
         <v>8891997</v>
       </c>
-      <c r="B53" s="34" t="s">
+      <c r="C53" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="34">
+      <c r="D53" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D53" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E53" s="34">
-        <v>128</v>
+      <c r="E53" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F53" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G53" s="34">
+        <v>1</v>
+      </c>
+      <c r="H53" s="34">
         <v>200</v>
       </c>
-      <c r="H53" s="85" t="s">
-        <v>128</v>
-      </c>
-      <c r="I53" s="34">
+      <c r="I53" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="J53" s="34">
         <v>92</v>
       </c>
-      <c r="K53" s="47">
+      <c r="L53" s="47">
         <v>0.80520000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="34">
         <v>8892881</v>
       </c>
-      <c r="B54" s="34" t="s">
+      <c r="C54" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="34">
+      <c r="D54" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D54" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E54" s="34">
-        <v>128</v>
+      <c r="E54" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F54" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G54" s="34">
+        <v>1</v>
+      </c>
+      <c r="H54" s="34">
         <v>200</v>
       </c>
-      <c r="H54" s="85" t="s">
+      <c r="I54" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="I54" s="34">
+      <c r="J54" s="34">
         <v>156</v>
       </c>
-      <c r="K54" s="47">
+      <c r="L54" s="47">
         <v>0.80979999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="34">
         <v>8892879</v>
       </c>
-      <c r="B55" s="34" t="s">
+      <c r="C55" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C55" s="34">
+      <c r="D55" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D55" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="34">
-        <v>128</v>
+      <c r="E55" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F55" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G55" s="34">
+        <v>1</v>
+      </c>
+      <c r="H55" s="34">
         <v>200</v>
       </c>
-      <c r="H55" s="85" t="s">
-        <v>128</v>
-      </c>
-      <c r="I55" s="34">
+      <c r="I55" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="J55" s="34">
         <v>92</v>
       </c>
-      <c r="K55" s="47">
+      <c r="L55" s="47">
         <v>0.80520000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="34">
         <v>8892956</v>
       </c>
-      <c r="B56" s="34" t="s">
+      <c r="C56" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C56" s="34">
+      <c r="D56" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D56" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E56" s="34">
-        <v>128</v>
+      <c r="E56" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F56" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G56" s="34">
+        <v>1</v>
+      </c>
+      <c r="H56" s="34">
         <v>200</v>
       </c>
-      <c r="H56" s="85" t="s">
+      <c r="I56" s="85" t="s">
         <v>131</v>
       </c>
-      <c r="I56" s="34">
+      <c r="J56" s="34">
         <v>121</v>
       </c>
-      <c r="K56" s="47">
+      <c r="L56" s="47">
         <v>0.68089999999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="34">
         <v>8892957</v>
       </c>
-      <c r="B57" s="34" t="s">
+      <c r="C57" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C57" s="34">
+      <c r="D57" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D57" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E57" s="34">
-        <v>128</v>
+      <c r="E57" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F57" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G57" s="34">
+        <v>1</v>
+      </c>
+      <c r="H57" s="34">
         <v>200</v>
       </c>
-      <c r="H57" s="85" t="s">
-        <v>128</v>
-      </c>
-      <c r="I57" s="34">
+      <c r="I57" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="J57" s="34">
         <v>129</v>
       </c>
-      <c r="K57" s="47">
+      <c r="L57" s="47">
         <v>0.6492</v>
       </c>
     </row>
-    <row r="58" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="34">
         <v>8894359</v>
       </c>
-      <c r="B58" s="34" t="s">
+      <c r="C58" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C58" s="34">
+      <c r="D58" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D58" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E58" s="34">
-        <v>128</v>
+      <c r="E58" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F58" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G58" s="34">
+        <v>1</v>
+      </c>
+      <c r="H58" s="34">
         <v>200</v>
       </c>
-      <c r="H58" s="85" t="s">
+      <c r="I58" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="I58" s="34">
+      <c r="J58" s="34">
         <v>62</v>
       </c>
-      <c r="K58" s="47">
+      <c r="L58" s="47">
         <v>0.65590000000000004</v>
       </c>
     </row>
-    <row r="59" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="44">
         <v>8894360</v>
       </c>
-      <c r="B59" s="44" t="s">
+      <c r="C59" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C59" s="44">
+      <c r="D59" s="44">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D59" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="44">
-        <v>128</v>
+      <c r="E59" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F59" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G59" s="44">
+        <v>1</v>
+      </c>
+      <c r="H59" s="44">
         <v>200</v>
       </c>
-      <c r="H59" s="93" t="s">
+      <c r="I59" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="L59" s="44" t="s">
+      <c r="M59" s="44" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44">
         <v>8894361</v>
       </c>
-      <c r="B60" s="44" t="s">
+      <c r="C60" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C60" s="44">
+      <c r="D60" s="44">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D60" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="44">
-        <v>128</v>
+      <c r="E60" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F60" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G60" s="44">
+        <v>1</v>
+      </c>
+      <c r="H60" s="44">
         <v>200</v>
       </c>
-      <c r="H60" s="93" t="s">
+      <c r="I60" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="L60" s="44" t="s">
+      <c r="M60" s="44" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="34">
         <v>8894362</v>
       </c>
-      <c r="B61" s="34" t="s">
+      <c r="C61" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="34">
+      <c r="D61" s="34">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D61" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="34">
-        <v>128</v>
+      <c r="E61" s="34" t="s">
+        <v>5</v>
       </c>
       <c r="F61" s="34">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G61" s="34">
+        <v>1</v>
+      </c>
+      <c r="H61" s="34">
         <v>200</v>
       </c>
-      <c r="H61" s="85" t="s">
+      <c r="I61" s="85" t="s">
         <v>147</v>
       </c>
-      <c r="I61" s="34">
+      <c r="J61" s="34">
         <v>73</v>
       </c>
-      <c r="K61" s="47">
+      <c r="L61" s="47">
         <v>0.79820000000000002</v>
       </c>
     </row>
-    <row r="62" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="44">
         <v>8894678</v>
       </c>
-      <c r="B62" s="44" t="s">
+      <c r="C62" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C62" s="44">
+      <c r="D62" s="44">
         <v>1E-4</v>
       </c>
-      <c r="D62" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E62" s="44">
-        <v>128</v>
+      <c r="E62" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F62" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G62" s="44">
+        <v>1</v>
+      </c>
+      <c r="H62" s="44">
         <v>200</v>
       </c>
-      <c r="H62" s="93" t="s">
+      <c r="I62" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="L62" s="44" t="s">
+      <c r="M62" s="44" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="44">
         <v>8894677</v>
       </c>
-      <c r="B63" s="44" t="s">
+      <c r="C63" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="44">
+      <c r="D63" s="44">
         <v>1E-4</v>
       </c>
-      <c r="D63" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="44">
-        <v>128</v>
+      <c r="E63" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F63" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G63" s="44">
+        <v>1</v>
+      </c>
+      <c r="H63" s="44">
         <v>200</v>
       </c>
-      <c r="H63" s="93" t="s">
+      <c r="I63" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="L63" s="44" t="s">
+      <c r="M63" s="44" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44">
         <v>8894676</v>
       </c>
-      <c r="B64" s="44" t="s">
+      <c r="C64" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="C64" s="44">
+      <c r="D64" s="44">
         <v>1E-3</v>
       </c>
-      <c r="D64" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E64" s="44">
-        <v>128</v>
+      <c r="E64" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F64" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G64" s="44">
+        <v>1</v>
+      </c>
+      <c r="H64" s="44">
         <v>200</v>
       </c>
-      <c r="H64" s="93" t="s">
+      <c r="I64" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="L64" s="44" t="s">
+      <c r="M64" s="44" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5385,28 +5401,28 @@
       <c r="A65" s="44">
         <v>8894675</v>
       </c>
-      <c r="B65" s="44" t="s">
+      <c r="C65" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C65" s="44">
+      <c r="D65" s="44">
         <v>1E-3</v>
       </c>
-      <c r="D65" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="E65" s="44">
-        <v>128</v>
+      <c r="E65" s="44" t="s">
+        <v>5</v>
       </c>
       <c r="F65" s="44">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G65" s="44">
+        <v>1</v>
+      </c>
+      <c r="H65" s="44">
         <v>200</v>
       </c>
-      <c r="H65" s="93" t="s">
+      <c r="I65" s="93" t="s">
         <v>131</v>
       </c>
-      <c r="L65" s="44" t="s">
+      <c r="M65" s="44" t="s">
         <v>151</v>
       </c>
     </row>
@@ -5414,31 +5430,31 @@
       <c r="A66" s="9">
         <v>8908438</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="9">
+      <c r="D66" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" s="9">
-        <v>128</v>
+      <c r="E66" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F66" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G66" s="9">
+        <v>1</v>
+      </c>
+      <c r="H66" s="9">
         <v>200</v>
       </c>
-      <c r="H66" s="82" t="s">
+      <c r="I66" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="I66" s="9">
+      <c r="J66" s="9">
         <v>39</v>
       </c>
-      <c r="L66" s="9" t="s">
+      <c r="M66" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5446,28 +5462,28 @@
       <c r="A67" s="9">
         <v>8908439</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="C67" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="9">
+      <c r="D67" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E67" s="9">
-        <v>128</v>
+      <c r="E67" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F67" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G67" s="9">
+        <v>1</v>
+      </c>
+      <c r="H67" s="9">
         <v>200</v>
       </c>
-      <c r="H67" s="82" t="s">
+      <c r="I67" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="L67" s="9" t="s">
+      <c r="M67" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5475,31 +5491,31 @@
       <c r="A68" s="78">
         <v>8908441</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C68" s="9">
+      <c r="D68" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E68" s="9">
-        <v>128</v>
+      <c r="E68" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F68" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G68" s="9">
+        <v>1</v>
+      </c>
+      <c r="H68" s="9">
         <v>200</v>
       </c>
-      <c r="H68" s="82" t="s">
+      <c r="I68" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="I68" s="9">
+      <c r="J68" s="9">
         <v>17</v>
       </c>
-      <c r="L68" s="9" t="s">
+      <c r="M68" s="9" t="s">
         <v>168</v>
       </c>
     </row>
@@ -5507,25 +5523,25 @@
       <c r="A69" s="9">
         <v>8908440</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C69" s="9">
+      <c r="D69" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D69" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E69" s="9">
-        <v>128</v>
+      <c r="E69" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F69" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G69" s="9">
+        <v>1</v>
+      </c>
+      <c r="H69" s="9">
         <v>200</v>
       </c>
-      <c r="H69" s="82" t="s">
+      <c r="I69" s="82" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5533,28 +5549,27 @@
       <c r="A70" s="9">
         <v>8910616</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="C70" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C70" s="9">
+      <c r="D70" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D70" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E70" s="9">
-        <v>128</v>
+      <c r="E70" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F70" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G70" s="9">
+        <v>1</v>
+      </c>
+      <c r="H70" s="9">
         <v>200</v>
       </c>
-      <c r="H70" s="82" t="s">
+      <c r="I70" s="82" t="s">
         <v>169</v>
       </c>
-      <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
@@ -5586,28 +5601,27 @@
       <c r="A71" s="9">
         <v>8910618</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="C71" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C71" s="9">
+      <c r="D71" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D71" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E71" s="9">
-        <v>128</v>
+      <c r="E71" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F71" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G71" s="9">
+        <v>1</v>
+      </c>
+      <c r="H71" s="9">
         <v>200</v>
       </c>
-      <c r="H71" s="82" t="s">
+      <c r="I71" s="82" t="s">
         <v>170</v>
       </c>
-      <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
@@ -5639,28 +5653,27 @@
       <c r="A72" s="9">
         <v>8910792</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="C72" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="9">
+      <c r="D72" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="9">
-        <v>128</v>
+      <c r="E72" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F72" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G72" s="9">
+        <v>1</v>
+      </c>
+      <c r="H72" s="9">
         <v>200</v>
       </c>
-      <c r="H72" s="82" t="s">
+      <c r="I72" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
@@ -5692,28 +5705,27 @@
       <c r="A73" s="9">
         <v>8910797</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="9">
+      <c r="D73" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73" s="9">
-        <v>128</v>
+      <c r="E73" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F73" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G73" s="9">
+        <v>1</v>
+      </c>
+      <c r="H73" s="9">
         <v>200</v>
       </c>
-      <c r="H73" s="82" t="s">
+      <c r="I73" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
@@ -5745,28 +5757,27 @@
       <c r="A74" s="9">
         <v>8910798</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="C74" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C74" s="9">
+      <c r="D74" s="9">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E74" s="9">
-        <v>128</v>
+      <c r="E74" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F74" s="9">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G74" s="9">
+        <v>1</v>
+      </c>
+      <c r="H74" s="9">
         <v>200</v>
       </c>
-      <c r="H74" s="82" t="s">
+      <c r="I74" s="82" t="s">
         <v>173</v>
       </c>
-      <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
@@ -5798,28 +5809,27 @@
       <c r="A75" s="9">
         <v>8910799</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="C75" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="C75" s="16">
+      <c r="D75" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D75" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E75" s="16">
-        <v>128</v>
+      <c r="E75" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="F75" s="16">
-        <v>1</v>
+        <v>128</v>
       </c>
       <c r="G75" s="16">
+        <v>1</v>
+      </c>
+      <c r="H75" s="16">
         <v>200</v>
       </c>
-      <c r="H75" s="94" t="s">
+      <c r="I75" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
@@ -5851,25 +5861,25 @@
       <c r="A76" s="9">
         <v>9028624</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="C76" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C76" s="16">
+      <c r="D76" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D76" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E76" s="16">
-        <v>128</v>
-      </c>
-      <c r="F76" s="9">
-        <v>1</v>
+      <c r="E76" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" s="16">
+        <v>128</v>
       </c>
       <c r="G76" s="9">
+        <v>1</v>
+      </c>
+      <c r="H76" s="9">
         <v>50</v>
       </c>
-      <c r="H76" s="82" t="s">
+      <c r="I76" s="82" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5877,25 +5887,25 @@
       <c r="A77" s="9">
         <v>9028626</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="C77" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C77" s="16">
+      <c r="D77" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D77" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77" s="16">
-        <v>128</v>
-      </c>
-      <c r="F77" s="9">
-        <v>1</v>
+      <c r="E77" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="16">
+        <v>128</v>
       </c>
       <c r="G77" s="9">
+        <v>1</v>
+      </c>
+      <c r="H77" s="9">
         <v>50</v>
       </c>
-      <c r="H77" s="82" t="s">
+      <c r="I77" s="82" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5903,25 +5913,25 @@
       <c r="A78" s="16">
         <v>9028627</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C78" s="16">
+      <c r="D78" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D78" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E78" s="16">
-        <v>128</v>
-      </c>
-      <c r="F78" s="9">
-        <v>1</v>
+      <c r="E78" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" s="16">
+        <v>128</v>
       </c>
       <c r="G78" s="9">
+        <v>1</v>
+      </c>
+      <c r="H78" s="9">
         <v>50</v>
       </c>
-      <c r="H78" s="82" t="s">
+      <c r="I78" s="82" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5929,25 +5939,25 @@
       <c r="A79" s="16">
         <v>9028628</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="C79" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C79" s="16">
+      <c r="D79" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D79" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E79" s="16">
-        <v>128</v>
-      </c>
-      <c r="F79" s="9">
-        <v>1</v>
+      <c r="E79" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="16">
+        <v>128</v>
       </c>
       <c r="G79" s="9">
+        <v>1</v>
+      </c>
+      <c r="H79" s="9">
         <v>50</v>
       </c>
-      <c r="H79" s="82" t="s">
+      <c r="I79" s="82" t="s">
         <v>184</v>
       </c>
     </row>
@@ -5955,234 +5965,336 @@
       <c r="A80" s="16">
         <v>9028629</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="C80" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C80" s="16">
+      <c r="D80" s="16">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D80" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E80" s="16">
-        <v>128</v>
-      </c>
-      <c r="F80" s="9">
-        <v>1</v>
+      <c r="E80" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="16">
+        <v>128</v>
       </c>
       <c r="G80" s="9">
+        <v>1</v>
+      </c>
+      <c r="H80" s="9">
         <v>50</v>
       </c>
-      <c r="H80" s="82" t="s">
+      <c r="I80" s="82" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="81" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="88">
         <v>9052142</v>
       </c>
-      <c r="B81" s="89" t="s">
+      <c r="C81" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C81" s="88">
+      <c r="D81" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D81" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E81" s="88">
-        <v>128</v>
-      </c>
-      <c r="F81" s="89">
-        <v>1</v>
+      <c r="E81" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" s="88">
+        <v>128</v>
       </c>
       <c r="G81" s="89">
+        <v>1</v>
+      </c>
+      <c r="H81" s="89">
         <v>50</v>
       </c>
-      <c r="H81" s="95" t="s">
+      <c r="I81" s="95" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="88">
         <v>9052143</v>
       </c>
-      <c r="B82" s="89" t="s">
+      <c r="C82" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C82" s="88">
+      <c r="D82" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D82" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E82" s="88">
-        <v>128</v>
-      </c>
-      <c r="F82" s="89">
-        <v>1</v>
+      <c r="E82" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="88">
+        <v>128</v>
       </c>
       <c r="G82" s="89">
+        <v>1</v>
+      </c>
+      <c r="H82" s="89">
         <v>50</v>
       </c>
-      <c r="H82" s="95" t="s">
+      <c r="I82" s="95" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="88">
         <v>9052145</v>
       </c>
-      <c r="B83" s="89" t="s">
+      <c r="C83" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="C83" s="88">
+      <c r="D83" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D83" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E83" s="88">
-        <v>128</v>
-      </c>
-      <c r="F83" s="89">
-        <v>1</v>
+      <c r="E83" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F83" s="88">
+        <v>128</v>
       </c>
       <c r="G83" s="89">
+        <v>1</v>
+      </c>
+      <c r="H83" s="89">
         <v>50</v>
       </c>
-      <c r="H83" s="95" t="s">
+      <c r="I83" s="95" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="88">
         <v>9062085</v>
       </c>
-      <c r="B84" s="89" t="s">
+      <c r="C84" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="C84" s="88">
+      <c r="D84" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D84" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E84" s="88">
-        <v>128</v>
-      </c>
-      <c r="F84" s="89">
-        <v>1</v>
+      <c r="E84" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F84" s="88">
+        <v>128</v>
       </c>
       <c r="G84" s="89">
+        <v>1</v>
+      </c>
+      <c r="H84" s="89">
         <v>50</v>
       </c>
-      <c r="H84" s="95" t="s">
+      <c r="I84" s="95" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="88">
         <v>9062086</v>
       </c>
-      <c r="B85" s="89" t="s">
+      <c r="C85" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="C85" s="88">
+      <c r="D85" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D85" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E85" s="88">
-        <v>128</v>
-      </c>
-      <c r="F85" s="89">
-        <v>1</v>
+      <c r="E85" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" s="88">
+        <v>128</v>
       </c>
       <c r="G85" s="89">
+        <v>1</v>
+      </c>
+      <c r="H85" s="89">
         <v>50</v>
       </c>
-      <c r="H85" s="95" t="s">
+      <c r="I85" s="95" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="88">
         <v>9062088</v>
       </c>
-      <c r="B86" s="89" t="s">
+      <c r="C86" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="C86" s="88">
+      <c r="D86" s="88">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D86" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="E86" s="88">
-        <v>128</v>
-      </c>
-      <c r="F86" s="89">
-        <v>1</v>
+      <c r="E86" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" s="88">
+        <v>128</v>
       </c>
       <c r="G86" s="89">
+        <v>1</v>
+      </c>
+      <c r="H86" s="89">
         <v>50</v>
       </c>
-      <c r="H86" s="95" t="s">
+      <c r="I86" s="95" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="87">
         <v>9069877</v>
       </c>
-      <c r="B87" s="34" t="s">
+      <c r="B87" s="96">
+        <v>44607</v>
+      </c>
+      <c r="C87" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="C87" s="87">
+      <c r="D87" s="87">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D87" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E87" s="87">
-        <v>128</v>
-      </c>
-      <c r="F87" s="34">
-        <v>1</v>
+      <c r="E87" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F87" s="87">
+        <v>128</v>
       </c>
       <c r="G87" s="34">
+        <v>1</v>
+      </c>
+      <c r="H87" s="34">
         <v>50</v>
       </c>
-      <c r="H87" s="85" t="s">
+      <c r="I87" s="85" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J87" s="34">
+        <v>48</v>
+      </c>
+      <c r="K87" s="47">
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="87">
         <v>9072918</v>
       </c>
-      <c r="B88" s="34" t="s">
+      <c r="B88" s="96">
+        <v>44607</v>
+      </c>
+      <c r="C88" s="34" t="s">
         <v>195</v>
       </c>
-      <c r="C88" s="87">
+      <c r="D88" s="87">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="D88" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="E88" s="87">
-        <v>128</v>
-      </c>
-      <c r="F88" s="34">
-        <v>1</v>
+      <c r="E88" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F88" s="87">
+        <v>128</v>
       </c>
       <c r="G88" s="34">
+        <v>1</v>
+      </c>
+      <c r="H88" s="34">
         <v>50</v>
       </c>
-      <c r="H88" s="85" t="s">
+      <c r="I88" s="85" t="s">
         <v>207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="87">
+        <v>9073202</v>
+      </c>
+      <c r="B89" s="96">
+        <v>44607</v>
+      </c>
+      <c r="C89" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E89" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="87">
+        <v>128</v>
+      </c>
+      <c r="G89" s="34">
+        <v>1</v>
+      </c>
+      <c r="H89" s="34">
+        <v>50</v>
+      </c>
+      <c r="I89" s="85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="87">
+        <v>9073205</v>
+      </c>
+      <c r="B90" s="96">
+        <v>44607</v>
+      </c>
+      <c r="C90" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="D90" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E90" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F90" s="87">
+        <v>128</v>
+      </c>
+      <c r="G90" s="34">
+        <v>1</v>
+      </c>
+      <c r="H90" s="34">
+        <v>50</v>
+      </c>
+      <c r="I90" s="85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="46">
+        <v>9073207</v>
+      </c>
+      <c r="B91" s="97">
+        <v>44607</v>
+      </c>
+      <c r="C91" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="D91" s="46">
+        <v>0.3</v>
+      </c>
+      <c r="E91" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" s="46">
+        <v>128</v>
+      </c>
+      <c r="G91" s="44">
+        <v>1</v>
+      </c>
+      <c r="H91" s="44">
+        <v>50</v>
+      </c>
+      <c r="I91" s="93" t="s">
+        <v>207</v>
+      </c>
+      <c r="L91" s="44" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update MoCo checkpoint rule to avoid accident re-start from 0
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5AF1F6B-9016-BF4A-8919-881EF1BEFB82}"/>
+  <xr:revisionPtr revIDLastSave="231" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2442B7AB-2A6D-A246-8393-1BAAACB451F1}"/>
   <bookViews>
-    <workbookView xWindow="-31900" yWindow="1400" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="19360" yWindow="620" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="224">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -680,6 +680,42 @@
   </si>
   <si>
     <t>really bad performance</t>
+  </si>
+  <si>
+    <t>looks good but hasn't converge yet, inc lr</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, start from 9062616_190)</t>
+  </si>
+  <si>
+    <t>9069293_300</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3 + road type one hot + cyc infras one hot + oneway</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3 + n lanes + speed</t>
+  </si>
+  <si>
+    <t>loss looks very unstable, consider decreasing lr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ordMoCo hasn't converged yet </t>
+  </si>
+  <si>
+    <t>Wrong MoCoFea Version</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist)</t>
+  </si>
+  <si>
+    <t>9081486_140</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist, start from 9081486_210)</t>
+  </si>
+  <si>
+    <t>accidentiy terminated, re-start from 210 below</t>
   </si>
 </sst>
 </file>
@@ -855,7 +891,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1080,6 +1116,9 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3360,10 +3399,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI91"/>
+  <dimension ref="A1:AI98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="139" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView topLeftCell="A74" zoomScale="168" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5987,7 +6026,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="81" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="88">
         <v>9052142</v>
       </c>
@@ -6013,7 +6052,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="82" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="88">
         <v>9052143</v>
       </c>
@@ -6039,7 +6078,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="88">
         <v>9052145</v>
       </c>
@@ -6065,7 +6104,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="88">
         <v>9062085</v>
       </c>
@@ -6091,7 +6130,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="85" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="88">
         <v>9062086</v>
       </c>
@@ -6117,7 +6156,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="86" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="88">
         <v>9062088</v>
       </c>
@@ -6143,7 +6182,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="87">
         <v>9069877</v>
       </c>
@@ -6178,94 +6217,112 @@
         <v>0.65200000000000002</v>
       </c>
     </row>
-    <row r="88" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="87">
+    <row r="88" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="46">
         <v>9072918</v>
       </c>
-      <c r="B88" s="96">
+      <c r="B88" s="97">
         <v>44607</v>
       </c>
-      <c r="C88" s="34" t="s">
+      <c r="C88" s="44" t="s">
         <v>195</v>
       </c>
-      <c r="D88" s="87">
+      <c r="D88" s="46">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E88" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="F88" s="87">
-        <v>128</v>
-      </c>
-      <c r="G88" s="34">
-        <v>1</v>
-      </c>
-      <c r="H88" s="34">
+      <c r="E88" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F88" s="46">
+        <v>128</v>
+      </c>
+      <c r="G88" s="44">
+        <v>1</v>
+      </c>
+      <c r="H88" s="44">
         <v>50</v>
       </c>
-      <c r="I88" s="85" t="s">
+      <c r="I88" s="93" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="87">
+      <c r="L88" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="P88" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="46">
         <v>9073202</v>
       </c>
-      <c r="B89" s="96">
+      <c r="B89" s="97">
         <v>44607</v>
       </c>
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="D89" s="87">
+      <c r="D89" s="46">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E89" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="F89" s="87">
-        <v>128</v>
-      </c>
-      <c r="G89" s="34">
-        <v>1</v>
-      </c>
-      <c r="H89" s="34">
+      <c r="E89" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="46">
+        <v>128</v>
+      </c>
+      <c r="G89" s="44">
+        <v>1</v>
+      </c>
+      <c r="H89" s="44">
         <v>50</v>
       </c>
-      <c r="I89" s="85" t="s">
+      <c r="I89" s="93" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="87">
+      <c r="L89" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="P89" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="46">
         <v>9073205</v>
       </c>
-      <c r="B90" s="96">
+      <c r="B90" s="97">
         <v>44607</v>
       </c>
-      <c r="C90" s="34" t="s">
+      <c r="C90" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D90" s="87">
+      <c r="D90" s="46">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E90" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="F90" s="87">
-        <v>128</v>
-      </c>
-      <c r="G90" s="34">
-        <v>1</v>
-      </c>
-      <c r="H90" s="34">
+      <c r="E90" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F90" s="46">
+        <v>128</v>
+      </c>
+      <c r="G90" s="44">
+        <v>1</v>
+      </c>
+      <c r="H90" s="44">
         <v>50</v>
       </c>
-      <c r="I90" s="85" t="s">
+      <c r="I90" s="93" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L90" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="P90" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="46">
         <v>9073207</v>
       </c>
@@ -6295,6 +6352,242 @@
       </c>
       <c r="L91" s="44" t="s">
         <v>211</v>
+      </c>
+      <c r="P91" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="46">
+        <v>9078965</v>
+      </c>
+      <c r="B92" s="97">
+        <v>44608</v>
+      </c>
+      <c r="C92" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="D92" s="46">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E92" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="46">
+        <v>128</v>
+      </c>
+      <c r="G92" s="44">
+        <v>1</v>
+      </c>
+      <c r="H92" s="44">
+        <v>50</v>
+      </c>
+      <c r="I92" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="J92" s="44">
+        <v>44</v>
+      </c>
+      <c r="P92" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="46">
+        <v>9078966</v>
+      </c>
+      <c r="B93" s="97">
+        <v>44608</v>
+      </c>
+      <c r="C93" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="D93" s="46">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E93" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F93" s="46">
+        <v>128</v>
+      </c>
+      <c r="G93" s="44">
+        <v>1</v>
+      </c>
+      <c r="H93" s="44">
+        <v>50</v>
+      </c>
+      <c r="I93" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="J93" s="44">
+        <v>9</v>
+      </c>
+      <c r="P93" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="46">
+        <v>9078892</v>
+      </c>
+      <c r="B94" s="97">
+        <v>44609</v>
+      </c>
+      <c r="C94" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="D94" s="46">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E94" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F94" s="46">
+        <v>128</v>
+      </c>
+      <c r="G94" s="44">
+        <v>1</v>
+      </c>
+      <c r="H94" s="44">
+        <v>50</v>
+      </c>
+      <c r="I94" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="J94" s="44">
+        <v>41</v>
+      </c>
+      <c r="P94" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="46">
+        <v>8078894</v>
+      </c>
+      <c r="B95" s="97">
+        <v>44609</v>
+      </c>
+      <c r="C95" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="D95" s="46">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E95" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" s="46">
+        <v>128</v>
+      </c>
+      <c r="G95" s="44">
+        <v>1</v>
+      </c>
+      <c r="H95" s="44">
+        <v>50</v>
+      </c>
+      <c r="I95" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="J95" s="44">
+        <v>12</v>
+      </c>
+      <c r="P95" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="87">
+        <v>9078991</v>
+      </c>
+      <c r="B96" s="96">
+        <v>44609</v>
+      </c>
+      <c r="C96" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D96" s="87">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E96" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="87">
+        <v>128</v>
+      </c>
+      <c r="G96" s="34">
+        <v>1</v>
+      </c>
+      <c r="H96" s="34">
+        <v>50</v>
+      </c>
+      <c r="I96" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="J96" s="34">
+        <v>38</v>
+      </c>
+      <c r="K96" s="47">
+        <v>0.64</v>
+      </c>
+      <c r="L96" s="34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="96">
+        <v>44609</v>
+      </c>
+      <c r="C97" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D97" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E97" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F97" s="87">
+        <v>128</v>
+      </c>
+      <c r="G97" s="34">
+        <v>1</v>
+      </c>
+      <c r="H97" s="34">
+        <v>50</v>
+      </c>
+      <c r="I97" s="34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="87">
+        <v>9088638</v>
+      </c>
+      <c r="B98" s="96">
+        <v>44609</v>
+      </c>
+      <c r="C98" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D98" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E98" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="87">
+        <v>128</v>
+      </c>
+      <c r="G98" s="34">
+        <v>1</v>
+      </c>
+      <c r="H98" s="34">
+        <v>50</v>
+      </c>
+      <c r="I98" s="34" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -7862,10 +8155,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI56"/>
+  <dimension ref="A1:AI59"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9170,7 +9463,7 @@
       <c r="K48" s="39"/>
       <c r="L48" s="39"/>
     </row>
-    <row r="49" spans="1:20" s="80" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="79">
         <v>9031630</v>
       </c>
@@ -9196,11 +9489,11 @@
       <c r="K49" s="79"/>
       <c r="L49" s="79"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="6">
+    <row r="50" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="39">
         <v>9052126</v>
       </c>
-      <c r="B50" s="81">
+      <c r="B50" s="98">
         <v>44964</v>
       </c>
       <c r="C50" s="85" t="s">
@@ -9219,27 +9512,18 @@
         <v>1</v>
       </c>
       <c r="H50" s="39"/>
-      <c r="I50" s="34"/>
       <c r="J50" s="85"/>
       <c r="K50" s="39"/>
       <c r="L50" s="39"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="34"/>
-      <c r="O50" s="34"/>
-      <c r="P50" s="34"/>
-      <c r="Q50" s="34"/>
-      <c r="R50" s="34"/>
-      <c r="S50" s="34"/>
-      <c r="T50" s="34"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="6">
+    </row>
+    <row r="51" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="39">
         <v>9062591</v>
       </c>
-      <c r="B51" s="81">
+      <c r="B51" s="98">
         <v>44969</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="85" t="s">
         <v>196</v>
       </c>
       <c r="D51" s="39">
@@ -9254,18 +9538,20 @@
       <c r="G51" s="39">
         <v>1</v>
       </c>
-      <c r="J51" s="11" t="s">
+      <c r="J51" s="85" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A52" s="6">
+      <c r="K51" s="39"/>
+      <c r="L51" s="39"/>
+    </row>
+    <row r="52" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="39">
         <v>9062616</v>
       </c>
-      <c r="B52" s="81">
+      <c r="B52" s="98">
         <v>44969</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="85" t="s">
         <v>202</v>
       </c>
       <c r="D52" s="39">
@@ -9280,18 +9566,20 @@
       <c r="G52" s="39">
         <v>1</v>
       </c>
-      <c r="J52" s="11" t="s">
+      <c r="J52" s="85" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A53" s="6">
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+    </row>
+    <row r="53" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="39">
         <v>9063219</v>
       </c>
-      <c r="B53" s="81">
+      <c r="B53" s="98">
         <v>44970</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="85" t="s">
         <v>203</v>
       </c>
       <c r="D53" s="39">
@@ -9306,18 +9594,20 @@
       <c r="G53" s="39">
         <v>1</v>
       </c>
-      <c r="J53" s="11" t="s">
+      <c r="J53" s="85" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A54" s="6">
+      <c r="K53" s="39"/>
+      <c r="L53" s="39"/>
+    </row>
+    <row r="54" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="39">
         <v>9067187</v>
       </c>
-      <c r="B54" s="81">
+      <c r="B54" s="98">
         <v>44971</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="85" t="s">
         <v>196</v>
       </c>
       <c r="D54" s="39">
@@ -9332,18 +9622,20 @@
       <c r="G54" s="39">
         <v>1</v>
       </c>
-      <c r="J54" s="11" t="s">
+      <c r="J54" s="85" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A55" s="6">
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+    </row>
+    <row r="55" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="39">
         <v>9069292</v>
       </c>
-      <c r="B55" s="81">
+      <c r="B55" s="98">
         <v>44972</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="85" t="s">
         <v>200</v>
       </c>
       <c r="D55" s="39">
@@ -9358,18 +9650,18 @@
       <c r="G55" s="39">
         <v>1</v>
       </c>
-      <c r="J55" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A56" s="6">
+      <c r="J55" s="85"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="39"/>
+    </row>
+    <row r="56" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="39">
         <v>9069293</v>
       </c>
-      <c r="B56" s="81">
+      <c r="B56" s="98">
         <v>44972</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="85" t="s">
         <v>204</v>
       </c>
       <c r="D56" s="39">
@@ -9382,6 +9674,86 @@
         <v>128</v>
       </c>
       <c r="G56" s="39">
+        <v>1</v>
+      </c>
+      <c r="J56" s="85"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="39"/>
+    </row>
+    <row r="57" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="39">
+        <v>9075022</v>
+      </c>
+      <c r="B57" s="98">
+        <v>44973</v>
+      </c>
+      <c r="C57" s="85" t="s">
+        <v>213</v>
+      </c>
+      <c r="D57" s="39">
+        <v>30</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57" s="39">
+        <v>128</v>
+      </c>
+      <c r="G57" s="39">
+        <v>1</v>
+      </c>
+      <c r="J57" s="85"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="39"/>
+    </row>
+    <row r="58" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="39">
+        <v>9081486</v>
+      </c>
+      <c r="B58" s="98">
+        <v>44974</v>
+      </c>
+      <c r="C58" s="85" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="39">
+        <v>30</v>
+      </c>
+      <c r="E58" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F58" s="39">
+        <v>128</v>
+      </c>
+      <c r="G58" s="39">
+        <v>1</v>
+      </c>
+      <c r="J58" s="85" t="s">
+        <v>223</v>
+      </c>
+      <c r="K58" s="39"/>
+      <c r="L58" s="39"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>9088855</v>
+      </c>
+      <c r="B59" s="81">
+        <v>44976</v>
+      </c>
+      <c r="C59" s="85" t="s">
+        <v>222</v>
+      </c>
+      <c r="D59" s="39">
+        <v>30</v>
+      </c>
+      <c r="E59" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="39">
+        <v>128</v>
+      </c>
+      <c r="G59" s="39">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add hl-inc option in MoCo train to control whether or not to increase the dist between LTS2 and LTS3
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2442B7AB-2A6D-A246-8393-1BAAACB451F1}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEF48E73-FE8D-0E47-A60D-FC72EE961FEF}"/>
   <bookViews>
-    <workbookView xWindow="19360" yWindow="620" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-50480" yWindow="1600" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="227">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -716,6 +716,15 @@
   </si>
   <si>
     <t>accidentiy terminated, re-start from 210 below</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist, alpha=1)</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist, alpha=3)</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist, alpha=2, start from 9069293_300)</t>
   </si>
 </sst>
 </file>
@@ -745,7 +754,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +839,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -891,7 +906,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1119,6 +1134,17 @@
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1435,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A19" zoomScale="174" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2359,62 +2385,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="32">
+    <row r="25" spans="1:33" s="103" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="99">
         <v>8886900</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="99" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="99">
         <v>1E-3</v>
       </c>
-      <c r="D25" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="32">
-        <v>128</v>
-      </c>
-      <c r="F25" s="32">
+      <c r="D25" s="99" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="99">
+        <v>128</v>
+      </c>
+      <c r="F25" s="99">
         <v>7</v>
       </c>
-      <c r="G25" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="40">
+      <c r="G25" s="99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="101">
         <v>0.66200000000000003</v>
       </c>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33" t="s">
+      <c r="K25" s="102"/>
+      <c r="L25" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
-      <c r="S25" s="33"/>
-      <c r="T25" s="33"/>
-      <c r="U25" s="33"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="33"/>
-      <c r="Y25" s="33"/>
-      <c r="Z25" s="33"/>
-      <c r="AA25" s="33"/>
-      <c r="AB25" s="33"/>
-      <c r="AC25" s="33"/>
-      <c r="AD25" s="33"/>
-      <c r="AE25" s="33"/>
-      <c r="AF25" s="33"/>
-      <c r="AG25" s="33"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="102"/>
+      <c r="P25" s="102"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="102"/>
+      <c r="S25" s="102"/>
+      <c r="T25" s="102"/>
+      <c r="U25" s="102"/>
+      <c r="V25" s="102"/>
+      <c r="W25" s="102"/>
+      <c r="X25" s="102"/>
+      <c r="Y25" s="102"/>
+      <c r="Z25" s="102"/>
+      <c r="AA25" s="102"/>
+      <c r="AB25" s="102"/>
+      <c r="AC25" s="102"/>
+      <c r="AD25" s="102"/>
+      <c r="AE25" s="102"/>
+      <c r="AF25" s="102"/>
+      <c r="AG25" s="102"/>
     </row>
     <row r="26" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
@@ -2471,62 +2497,62 @@
       <c r="AF26" s="43"/>
       <c r="AG26" s="43"/>
     </row>
-    <row r="27" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32">
+    <row r="27" spans="1:33" s="103" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="99">
         <v>8886880</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="32">
+      <c r="C27" s="99">
         <v>0.01</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="32">
-        <v>128</v>
-      </c>
-      <c r="F27" s="32">
+      <c r="D27" s="99" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="99">
+        <v>128</v>
+      </c>
+      <c r="F27" s="99">
         <v>64</v>
       </c>
-      <c r="G27" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="40">
+      <c r="G27" s="99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" s="101">
         <v>0.81730000000000003</v>
       </c>
-      <c r="K27" s="33" t="s">
+      <c r="K27" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
-      <c r="Y27" s="33"/>
-      <c r="Z27" s="33"/>
-      <c r="AA27" s="33"/>
-      <c r="AB27" s="33"/>
-      <c r="AC27" s="33"/>
-      <c r="AD27" s="33"/>
-      <c r="AE27" s="33"/>
-      <c r="AF27" s="33"/>
-      <c r="AG27" s="33"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
+      <c r="N27" s="102"/>
+      <c r="O27" s="102"/>
+      <c r="P27" s="102"/>
+      <c r="Q27" s="102"/>
+      <c r="R27" s="102"/>
+      <c r="S27" s="102"/>
+      <c r="T27" s="102"/>
+      <c r="U27" s="102"/>
+      <c r="V27" s="102"/>
+      <c r="W27" s="102"/>
+      <c r="X27" s="102"/>
+      <c r="Y27" s="102"/>
+      <c r="Z27" s="102"/>
+      <c r="AA27" s="102"/>
+      <c r="AB27" s="102"/>
+      <c r="AC27" s="102"/>
+      <c r="AD27" s="102"/>
+      <c r="AE27" s="102"/>
+      <c r="AF27" s="102"/>
+      <c r="AG27" s="102"/>
     </row>
     <row r="28" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32">
@@ -2854,60 +2880,60 @@
       <c r="AF33" s="43"/>
       <c r="AG33" s="43"/>
     </row>
-    <row r="34" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="32">
+    <row r="34" spans="1:33" s="103" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="99">
         <v>8890095</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="32">
+      <c r="C34" s="99">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D34" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="32">
-        <v>128</v>
-      </c>
-      <c r="F34" s="32">
+      <c r="D34" s="99" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="99">
+        <v>128</v>
+      </c>
+      <c r="F34" s="99">
         <v>8</v>
       </c>
-      <c r="G34" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" s="40">
+      <c r="G34" s="99" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="99" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="99" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" s="101">
         <v>0.68869999999999998</v>
       </c>
-      <c r="K34" s="33"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="33"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="33"/>
-      <c r="R34" s="33"/>
-      <c r="S34" s="33"/>
-      <c r="T34" s="33"/>
-      <c r="U34" s="33"/>
-      <c r="V34" s="33"/>
-      <c r="W34" s="33"/>
-      <c r="X34" s="33"/>
-      <c r="Y34" s="33"/>
-      <c r="Z34" s="33"/>
-      <c r="AA34" s="33"/>
-      <c r="AB34" s="33"/>
-      <c r="AC34" s="33"/>
-      <c r="AD34" s="33"/>
-      <c r="AE34" s="33"/>
-      <c r="AF34" s="33"/>
-      <c r="AG34" s="33"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="102"/>
+      <c r="O34" s="102"/>
+      <c r="P34" s="102"/>
+      <c r="Q34" s="102"/>
+      <c r="R34" s="102"/>
+      <c r="S34" s="102"/>
+      <c r="T34" s="102"/>
+      <c r="U34" s="102"/>
+      <c r="V34" s="102"/>
+      <c r="W34" s="102"/>
+      <c r="X34" s="102"/>
+      <c r="Y34" s="102"/>
+      <c r="Z34" s="102"/>
+      <c r="AA34" s="102"/>
+      <c r="AB34" s="102"/>
+      <c r="AC34" s="102"/>
+      <c r="AD34" s="102"/>
+      <c r="AE34" s="102"/>
+      <c r="AF34" s="102"/>
+      <c r="AG34" s="102"/>
     </row>
     <row r="35" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32">
@@ -3401,8 +3427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI98"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="168" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView zoomScale="168" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:XFD98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6535,7 +6561,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="97" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B97" s="96">
         <v>44609</v>
       </c>
@@ -6561,7 +6587,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="98" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="87">
         <v>9088638</v>
       </c>
@@ -6588,6 +6614,12 @@
       </c>
       <c r="I98" s="34" t="s">
         <v>221</v>
+      </c>
+      <c r="J98" s="34">
+        <v>7</v>
+      </c>
+      <c r="K98" s="47">
+        <v>0.59799999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -6601,7 +6633,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView zoomScale="214" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8155,10 +8187,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI59"/>
+  <dimension ref="A1:AI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9757,6 +9789,75 @@
         <v>1</v>
       </c>
     </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>9089404</v>
+      </c>
+      <c r="B60" s="81">
+        <v>44976</v>
+      </c>
+      <c r="C60" s="85" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" s="39">
+        <v>30</v>
+      </c>
+      <c r="E60" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="39">
+        <v>128</v>
+      </c>
+      <c r="G60" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>9089403</v>
+      </c>
+      <c r="B61" s="81">
+        <v>44976</v>
+      </c>
+      <c r="C61" s="85" t="s">
+        <v>225</v>
+      </c>
+      <c r="D61" s="39">
+        <v>30</v>
+      </c>
+      <c r="E61" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="39">
+        <v>128</v>
+      </c>
+      <c r="G61" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>9094403</v>
+      </c>
+      <c r="B62" s="81">
+        <v>44977</v>
+      </c>
+      <c r="C62" s="85" t="s">
+        <v>226</v>
+      </c>
+      <c r="D62" s="39">
+        <v>30</v>
+      </c>
+      <c r="E62" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="39">
+        <v>128</v>
+      </c>
+      <c r="G62" s="39">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add frozen/no-frozen option to MoCo_Clf_train. This only applies to MoCoClfV3 onward
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEF48E73-FE8D-0E47-A60D-FC72EE961FEF}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F09B0DC-E811-FE49-8408-0C0A3200602F}"/>
   <bookViews>
-    <workbookView xWindow="-50480" yWindow="1600" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-50480" yWindow="1600" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="229">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -725,6 +725,12 @@
   </si>
   <si>
     <t>OrdMoCo (projector, inc high-low stress dist, alpha=2, start from 9069293_300)</t>
+  </si>
+  <si>
+    <t>9088855_319</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3 (no frozen)</t>
   </si>
 </sst>
 </file>
@@ -906,7 +912,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1111,24 +1117,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1145,6 +1133,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2385,62 +2384,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" s="103" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="99">
+    <row r="25" spans="1:33" s="97" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="93">
         <v>8886900</v>
       </c>
-      <c r="B25" s="99" t="s">
+      <c r="B25" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="99">
+      <c r="C25" s="93">
         <v>1E-3</v>
       </c>
-      <c r="D25" s="99" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="99">
-        <v>128</v>
-      </c>
-      <c r="F25" s="99">
+      <c r="D25" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="93">
+        <v>128</v>
+      </c>
+      <c r="F25" s="93">
         <v>7</v>
       </c>
-      <c r="G25" s="99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="99" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="101">
+      <c r="G25" s="93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="93" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="93" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="95">
         <v>0.66200000000000003</v>
       </c>
-      <c r="K25" s="102"/>
-      <c r="L25" s="102" t="s">
+      <c r="K25" s="96"/>
+      <c r="L25" s="96" t="s">
         <v>121</v>
       </c>
-      <c r="M25" s="102"/>
-      <c r="N25" s="102"/>
-      <c r="O25" s="102"/>
-      <c r="P25" s="102"/>
-      <c r="Q25" s="102"/>
-      <c r="R25" s="102"/>
-      <c r="S25" s="102"/>
-      <c r="T25" s="102"/>
-      <c r="U25" s="102"/>
-      <c r="V25" s="102"/>
-      <c r="W25" s="102"/>
-      <c r="X25" s="102"/>
-      <c r="Y25" s="102"/>
-      <c r="Z25" s="102"/>
-      <c r="AA25" s="102"/>
-      <c r="AB25" s="102"/>
-      <c r="AC25" s="102"/>
-      <c r="AD25" s="102"/>
-      <c r="AE25" s="102"/>
-      <c r="AF25" s="102"/>
-      <c r="AG25" s="102"/>
+      <c r="M25" s="96"/>
+      <c r="N25" s="96"/>
+      <c r="O25" s="96"/>
+      <c r="P25" s="96"/>
+      <c r="Q25" s="96"/>
+      <c r="R25" s="96"/>
+      <c r="S25" s="96"/>
+      <c r="T25" s="96"/>
+      <c r="U25" s="96"/>
+      <c r="V25" s="96"/>
+      <c r="W25" s="96"/>
+      <c r="X25" s="96"/>
+      <c r="Y25" s="96"/>
+      <c r="Z25" s="96"/>
+      <c r="AA25" s="96"/>
+      <c r="AB25" s="96"/>
+      <c r="AC25" s="96"/>
+      <c r="AD25" s="96"/>
+      <c r="AE25" s="96"/>
+      <c r="AF25" s="96"/>
+      <c r="AG25" s="96"/>
     </row>
     <row r="26" spans="1:33" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
@@ -2497,62 +2496,62 @@
       <c r="AF26" s="43"/>
       <c r="AG26" s="43"/>
     </row>
-    <row r="27" spans="1:33" s="103" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="99">
+    <row r="27" spans="1:33" s="97" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="93">
         <v>8886880</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="99">
+      <c r="C27" s="93">
         <v>0.01</v>
       </c>
-      <c r="D27" s="99" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="99">
-        <v>128</v>
-      </c>
-      <c r="F27" s="99">
+      <c r="D27" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="93">
+        <v>128</v>
+      </c>
+      <c r="F27" s="93">
         <v>64</v>
       </c>
-      <c r="G27" s="99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="99" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="101">
+      <c r="G27" s="93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="93" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="93" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" s="95">
         <v>0.81730000000000003</v>
       </c>
-      <c r="K27" s="102" t="s">
+      <c r="K27" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="L27" s="102"/>
-      <c r="M27" s="102"/>
-      <c r="N27" s="102"/>
-      <c r="O27" s="102"/>
-      <c r="P27" s="102"/>
-      <c r="Q27" s="102"/>
-      <c r="R27" s="102"/>
-      <c r="S27" s="102"/>
-      <c r="T27" s="102"/>
-      <c r="U27" s="102"/>
-      <c r="V27" s="102"/>
-      <c r="W27" s="102"/>
-      <c r="X27" s="102"/>
-      <c r="Y27" s="102"/>
-      <c r="Z27" s="102"/>
-      <c r="AA27" s="102"/>
-      <c r="AB27" s="102"/>
-      <c r="AC27" s="102"/>
-      <c r="AD27" s="102"/>
-      <c r="AE27" s="102"/>
-      <c r="AF27" s="102"/>
-      <c r="AG27" s="102"/>
+      <c r="L27" s="96"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="96"/>
+      <c r="O27" s="96"/>
+      <c r="P27" s="96"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="96"/>
+      <c r="S27" s="96"/>
+      <c r="T27" s="96"/>
+      <c r="U27" s="96"/>
+      <c r="V27" s="96"/>
+      <c r="W27" s="96"/>
+      <c r="X27" s="96"/>
+      <c r="Y27" s="96"/>
+      <c r="Z27" s="96"/>
+      <c r="AA27" s="96"/>
+      <c r="AB27" s="96"/>
+      <c r="AC27" s="96"/>
+      <c r="AD27" s="96"/>
+      <c r="AE27" s="96"/>
+      <c r="AF27" s="96"/>
+      <c r="AG27" s="96"/>
     </row>
     <row r="28" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32">
@@ -2880,60 +2879,60 @@
       <c r="AF33" s="43"/>
       <c r="AG33" s="43"/>
     </row>
-    <row r="34" spans="1:33" s="103" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="99">
+    <row r="34" spans="1:33" s="97" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="93">
         <v>8890095</v>
       </c>
-      <c r="B34" s="100" t="s">
+      <c r="B34" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="99">
+      <c r="C34" s="93">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="D34" s="99" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="99">
-        <v>128</v>
-      </c>
-      <c r="F34" s="99">
+      <c r="D34" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="93">
+        <v>128</v>
+      </c>
+      <c r="F34" s="93">
         <v>8</v>
       </c>
-      <c r="G34" s="99" t="b">
-        <v>0</v>
-      </c>
-      <c r="H34" s="99" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="99" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" s="101">
+      <c r="G34" s="93" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="93" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="93" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" s="95">
         <v>0.68869999999999998</v>
       </c>
-      <c r="K34" s="102"/>
-      <c r="L34" s="102"/>
-      <c r="M34" s="102"/>
-      <c r="N34" s="102"/>
-      <c r="O34" s="102"/>
-      <c r="P34" s="102"/>
-      <c r="Q34" s="102"/>
-      <c r="R34" s="102"/>
-      <c r="S34" s="102"/>
-      <c r="T34" s="102"/>
-      <c r="U34" s="102"/>
-      <c r="V34" s="102"/>
-      <c r="W34" s="102"/>
-      <c r="X34" s="102"/>
-      <c r="Y34" s="102"/>
-      <c r="Z34" s="102"/>
-      <c r="AA34" s="102"/>
-      <c r="AB34" s="102"/>
-      <c r="AC34" s="102"/>
-      <c r="AD34" s="102"/>
-      <c r="AE34" s="102"/>
-      <c r="AF34" s="102"/>
-      <c r="AG34" s="102"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="96"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="96"/>
+      <c r="O34" s="96"/>
+      <c r="P34" s="96"/>
+      <c r="Q34" s="96"/>
+      <c r="R34" s="96"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="96"/>
+      <c r="U34" s="96"/>
+      <c r="V34" s="96"/>
+      <c r="W34" s="96"/>
+      <c r="X34" s="96"/>
+      <c r="Y34" s="96"/>
+      <c r="Z34" s="96"/>
+      <c r="AA34" s="96"/>
+      <c r="AB34" s="96"/>
+      <c r="AC34" s="96"/>
+      <c r="AD34" s="96"/>
+      <c r="AE34" s="96"/>
+      <c r="AF34" s="96"/>
+      <c r="AG34" s="96"/>
     </row>
     <row r="35" spans="1:33" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="32">
@@ -3425,10 +3424,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI98"/>
+  <dimension ref="A1:AI100"/>
   <sheetViews>
-    <sheetView zoomScale="168" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD98"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="168" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3441,7 +3440,7 @@
     <col min="6" max="6" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" customWidth="1"/>
     <col min="8" max="8" width="14" style="11" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="99" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3469,7 +3468,7 @@
       <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="98" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -3529,7 +3528,7 @@
       <c r="H2">
         <v>50</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="99" t="s">
         <v>20</v>
       </c>
       <c r="J2" t="s">
@@ -3560,7 +3559,7 @@
       <c r="H3">
         <v>50</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="99" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="7">
@@ -3595,7 +3594,7 @@
       <c r="H4">
         <v>50</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="99" t="s">
         <v>27</v>
       </c>
       <c r="M4" t="s">
@@ -3624,7 +3623,7 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="99" t="s">
         <v>26</v>
       </c>
       <c r="M5" t="s">
@@ -3653,7 +3652,7 @@
       <c r="H6">
         <v>50</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="99" t="s">
         <v>26</v>
       </c>
       <c r="M6" t="s">
@@ -3682,7 +3681,7 @@
       <c r="H7">
         <v>50</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="99" t="s">
         <v>26</v>
       </c>
       <c r="M7" t="s">
@@ -3711,7 +3710,7 @@
       <c r="H8">
         <v>50</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="99" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3737,7 +3736,7 @@
       <c r="H9">
         <v>50</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="99" t="s">
         <v>48</v>
       </c>
       <c r="M9" t="s">
@@ -3766,7 +3765,7 @@
       <c r="H10">
         <v>50</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="99" t="s">
         <v>48</v>
       </c>
       <c r="M10" t="s">
@@ -3795,7 +3794,7 @@
       <c r="H11">
         <v>50</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="99" t="s">
         <v>60</v>
       </c>
       <c r="M11" t="s">
@@ -3827,7 +3826,7 @@
       <c r="H12">
         <v>30</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="99" t="s">
         <v>61</v>
       </c>
       <c r="M12" t="s">
@@ -3859,7 +3858,7 @@
       <c r="H13">
         <v>30</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="99" t="s">
         <v>60</v>
       </c>
       <c r="M13" t="s">
@@ -3891,7 +3890,7 @@
       <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="99" t="s">
         <v>61</v>
       </c>
       <c r="M14" t="s">
@@ -3923,7 +3922,7 @@
       <c r="H15">
         <v>30</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="99" t="s">
         <v>60</v>
       </c>
       <c r="L15" s="7">
@@ -3961,7 +3960,7 @@
       <c r="H16">
         <v>30</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="99" t="s">
         <v>61</v>
       </c>
       <c r="L16" s="7">
@@ -3999,7 +3998,7 @@
       <c r="H17">
         <v>100</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="99" t="s">
         <v>60</v>
       </c>
       <c r="M17" t="s">
@@ -4031,7 +4030,7 @@
       <c r="H18">
         <v>100</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="99" t="s">
         <v>61</v>
       </c>
       <c r="M18" t="s">
@@ -4063,7 +4062,7 @@
       <c r="H19">
         <v>100</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="99" t="s">
         <v>60</v>
       </c>
       <c r="J19">
@@ -4098,7 +4097,7 @@
       <c r="H20">
         <v>100</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="99" t="s">
         <v>61</v>
       </c>
       <c r="J20">
@@ -4133,7 +4132,7 @@
       <c r="H21">
         <v>100</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="99" t="s">
         <v>27</v>
       </c>
       <c r="J21">
@@ -4168,7 +4167,7 @@
       <c r="H22">
         <v>100</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="99" t="s">
         <v>78</v>
       </c>
       <c r="J22">
@@ -4200,7 +4199,7 @@
       <c r="H23">
         <v>100</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="99" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4226,7 +4225,7 @@
       <c r="H24">
         <v>100</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="99" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4252,7 +4251,7 @@
       <c r="H25" s="9">
         <v>100</v>
       </c>
-      <c r="I25" s="82" t="s">
+      <c r="I25" s="100" t="s">
         <v>61</v>
       </c>
       <c r="J25" s="9">
@@ -4287,7 +4286,7 @@
       <c r="H26" s="9">
         <v>100</v>
       </c>
-      <c r="I26" s="82" t="s">
+      <c r="I26" s="100" t="s">
         <v>27</v>
       </c>
       <c r="J26" s="9">
@@ -4319,7 +4318,7 @@
       <c r="H27" s="9">
         <v>100</v>
       </c>
-      <c r="I27" s="82" t="s">
+      <c r="I27" s="100" t="s">
         <v>61</v>
       </c>
       <c r="J27" s="9">
@@ -4351,7 +4350,7 @@
       <c r="H28" s="9">
         <v>100</v>
       </c>
-      <c r="I28" s="82" t="s">
+      <c r="I28" s="100" t="s">
         <v>27</v>
       </c>
       <c r="J28" s="9">
@@ -4383,7 +4382,7 @@
       <c r="H29" s="20">
         <v>100</v>
       </c>
-      <c r="I29" s="91" t="s">
+      <c r="I29" s="101" t="s">
         <v>61</v>
       </c>
       <c r="J29" s="20">
@@ -4415,7 +4414,7 @@
       <c r="H30" s="20">
         <v>100</v>
       </c>
-      <c r="I30" s="91" t="s">
+      <c r="I30" s="101" t="s">
         <v>27</v>
       </c>
       <c r="J30" s="20">
@@ -4447,7 +4446,7 @@
       <c r="H31" s="20">
         <v>100</v>
       </c>
-      <c r="I31" s="91" t="s">
+      <c r="I31" s="101" t="s">
         <v>27</v>
       </c>
       <c r="J31" s="20">
@@ -4479,7 +4478,7 @@
       <c r="H32" s="20">
         <v>100</v>
       </c>
-      <c r="I32" s="91" t="s">
+      <c r="I32" s="101" t="s">
         <v>61</v>
       </c>
       <c r="J32" s="20">
@@ -4511,7 +4510,7 @@
       <c r="H33" s="21">
         <v>200</v>
       </c>
-      <c r="I33" s="92" t="s">
+      <c r="I33" s="102" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4537,7 +4536,7 @@
       <c r="H34" s="21">
         <v>200</v>
       </c>
-      <c r="I34" s="92" t="s">
+      <c r="I34" s="102" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4563,7 +4562,7 @@
       <c r="H35" s="20">
         <v>200</v>
       </c>
-      <c r="I35" s="91" t="s">
+      <c r="I35" s="101" t="s">
         <v>97</v>
       </c>
       <c r="J35" s="20">
@@ -4595,7 +4594,7 @@
       <c r="H36" s="20">
         <v>200</v>
       </c>
-      <c r="I36" s="91" t="s">
+      <c r="I36" s="101" t="s">
         <v>97</v>
       </c>
       <c r="J36" s="20">
@@ -4627,7 +4626,7 @@
       <c r="H37" s="20">
         <v>200</v>
       </c>
-      <c r="I37" s="91" t="s">
+      <c r="I37" s="101" t="s">
         <v>97</v>
       </c>
       <c r="J37" s="20">
@@ -4659,7 +4658,7 @@
       <c r="H38" s="20">
         <v>200</v>
       </c>
-      <c r="I38" s="91" t="s">
+      <c r="I38" s="101" t="s">
         <v>101</v>
       </c>
       <c r="J38" s="20">
@@ -4691,7 +4690,7 @@
       <c r="H39" s="20">
         <v>200</v>
       </c>
-      <c r="I39" s="91" t="s">
+      <c r="I39" s="101" t="s">
         <v>102</v>
       </c>
       <c r="J39" s="20">
@@ -4723,7 +4722,7 @@
       <c r="H40" s="20">
         <v>200</v>
       </c>
-      <c r="I40" s="91" t="s">
+      <c r="I40" s="101" t="s">
         <v>101</v>
       </c>
       <c r="J40" s="20">
@@ -4755,7 +4754,7 @@
       <c r="H41" s="20">
         <v>200</v>
       </c>
-      <c r="I41" s="91" t="s">
+      <c r="I41" s="101" t="s">
         <v>102</v>
       </c>
       <c r="J41" s="20">
@@ -4787,7 +4786,7 @@
       <c r="H42" s="20">
         <v>200</v>
       </c>
-      <c r="I42" s="91" t="s">
+      <c r="I42" s="101" t="s">
         <v>120</v>
       </c>
       <c r="J42" s="20"/>
@@ -4814,7 +4813,7 @@
       <c r="H43" s="20">
         <v>200</v>
       </c>
-      <c r="I43" s="91" t="s">
+      <c r="I43" s="101" t="s">
         <v>120</v>
       </c>
       <c r="J43" s="20"/>
@@ -4841,7 +4840,7 @@
       <c r="H44" s="20">
         <v>200</v>
       </c>
-      <c r="I44" s="91" t="s">
+      <c r="I44" s="101" t="s">
         <v>120</v>
       </c>
       <c r="J44" s="20"/>
@@ -4868,7 +4867,7 @@
       <c r="H45" s="34">
         <v>200</v>
       </c>
-      <c r="I45" s="85" t="s">
+      <c r="I45" s="103" t="s">
         <v>128</v>
       </c>
       <c r="J45" s="34">
@@ -4900,7 +4899,7 @@
       <c r="H46" s="34">
         <v>200</v>
       </c>
-      <c r="I46" s="85" t="s">
+      <c r="I46" s="103" t="s">
         <v>129</v>
       </c>
       <c r="J46" s="34">
@@ -4932,7 +4931,7 @@
       <c r="H47" s="44">
         <v>200</v>
       </c>
-      <c r="I47" s="93" t="s">
+      <c r="I47" s="104" t="s">
         <v>131</v>
       </c>
       <c r="M47" s="44" t="s">
@@ -4961,7 +4960,7 @@
       <c r="H48" s="44">
         <v>200</v>
       </c>
-      <c r="I48" s="93" t="s">
+      <c r="I48" s="104" t="s">
         <v>132</v>
       </c>
       <c r="M48" s="44" t="s">
@@ -4990,7 +4989,7 @@
       <c r="H49" s="34">
         <v>200</v>
       </c>
-      <c r="I49" s="85" t="s">
+      <c r="I49" s="103" t="s">
         <v>131</v>
       </c>
       <c r="J49" s="34">
@@ -5022,7 +5021,7 @@
       <c r="H50" s="44">
         <v>200</v>
       </c>
-      <c r="I50" s="93" t="s">
+      <c r="I50" s="104" t="s">
         <v>128</v>
       </c>
       <c r="M50" s="44" t="s">
@@ -5051,7 +5050,7 @@
       <c r="H51" s="34">
         <v>200</v>
       </c>
-      <c r="I51" s="85" t="s">
+      <c r="I51" s="103" t="s">
         <v>131</v>
       </c>
       <c r="J51" s="34">
@@ -5083,7 +5082,7 @@
       <c r="H52" s="34">
         <v>200</v>
       </c>
-      <c r="I52" s="85" t="s">
+      <c r="I52" s="103" t="s">
         <v>132</v>
       </c>
       <c r="J52" s="34">
@@ -5115,7 +5114,7 @@
       <c r="H53" s="34">
         <v>200</v>
       </c>
-      <c r="I53" s="85" t="s">
+      <c r="I53" s="103" t="s">
         <v>128</v>
       </c>
       <c r="J53" s="34">
@@ -5147,7 +5146,7 @@
       <c r="H54" s="34">
         <v>200</v>
       </c>
-      <c r="I54" s="85" t="s">
+      <c r="I54" s="103" t="s">
         <v>131</v>
       </c>
       <c r="J54" s="34">
@@ -5179,7 +5178,7 @@
       <c r="H55" s="34">
         <v>200</v>
       </c>
-      <c r="I55" s="85" t="s">
+      <c r="I55" s="103" t="s">
         <v>128</v>
       </c>
       <c r="J55" s="34">
@@ -5211,7 +5210,7 @@
       <c r="H56" s="34">
         <v>200</v>
       </c>
-      <c r="I56" s="85" t="s">
+      <c r="I56" s="103" t="s">
         <v>131</v>
       </c>
       <c r="J56" s="34">
@@ -5243,7 +5242,7 @@
       <c r="H57" s="34">
         <v>200</v>
       </c>
-      <c r="I57" s="85" t="s">
+      <c r="I57" s="103" t="s">
         <v>128</v>
       </c>
       <c r="J57" s="34">
@@ -5275,7 +5274,7 @@
       <c r="H58" s="34">
         <v>200</v>
       </c>
-      <c r="I58" s="85" t="s">
+      <c r="I58" s="103" t="s">
         <v>147</v>
       </c>
       <c r="J58" s="34">
@@ -5307,7 +5306,7 @@
       <c r="H59" s="44">
         <v>200</v>
       </c>
-      <c r="I59" s="93" t="s">
+      <c r="I59" s="104" t="s">
         <v>148</v>
       </c>
       <c r="M59" s="44" t="s">
@@ -5336,7 +5335,7 @@
       <c r="H60" s="44">
         <v>200</v>
       </c>
-      <c r="I60" s="93" t="s">
+      <c r="I60" s="104" t="s">
         <v>148</v>
       </c>
       <c r="M60" s="44" t="s">
@@ -5365,7 +5364,7 @@
       <c r="H61" s="34">
         <v>200</v>
       </c>
-      <c r="I61" s="85" t="s">
+      <c r="I61" s="103" t="s">
         <v>147</v>
       </c>
       <c r="J61" s="34">
@@ -5397,7 +5396,7 @@
       <c r="H62" s="44">
         <v>200</v>
       </c>
-      <c r="I62" s="93" t="s">
+      <c r="I62" s="104" t="s">
         <v>148</v>
       </c>
       <c r="M62" s="44" t="s">
@@ -5426,7 +5425,7 @@
       <c r="H63" s="44">
         <v>200</v>
       </c>
-      <c r="I63" s="93" t="s">
+      <c r="I63" s="104" t="s">
         <v>148</v>
       </c>
       <c r="M63" s="44" t="s">
@@ -5455,7 +5454,7 @@
       <c r="H64" s="44">
         <v>200</v>
       </c>
-      <c r="I64" s="93" t="s">
+      <c r="I64" s="104" t="s">
         <v>131</v>
       </c>
       <c r="M64" s="44" t="s">
@@ -5484,7 +5483,7 @@
       <c r="H65" s="44">
         <v>200</v>
       </c>
-      <c r="I65" s="93" t="s">
+      <c r="I65" s="104" t="s">
         <v>131</v>
       </c>
       <c r="M65" s="44" t="s">
@@ -5513,7 +5512,7 @@
       <c r="H66" s="9">
         <v>200</v>
       </c>
-      <c r="I66" s="82" t="s">
+      <c r="I66" s="100" t="s">
         <v>166</v>
       </c>
       <c r="J66" s="9">
@@ -5545,7 +5544,7 @@
       <c r="H67" s="9">
         <v>200</v>
       </c>
-      <c r="I67" s="82" t="s">
+      <c r="I67" s="100" t="s">
         <v>166</v>
       </c>
       <c r="M67" s="9" t="s">
@@ -5574,7 +5573,7 @@
       <c r="H68" s="9">
         <v>200</v>
       </c>
-      <c r="I68" s="82" t="s">
+      <c r="I68" s="100" t="s">
         <v>167</v>
       </c>
       <c r="J68" s="9">
@@ -5606,7 +5605,7 @@
       <c r="H69" s="9">
         <v>200</v>
       </c>
-      <c r="I69" s="82" t="s">
+      <c r="I69" s="100" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5632,7 +5631,7 @@
       <c r="H70" s="9">
         <v>200</v>
       </c>
-      <c r="I70" s="82" t="s">
+      <c r="I70" s="100" t="s">
         <v>169</v>
       </c>
       <c r="J70" s="9"/>
@@ -5684,7 +5683,7 @@
       <c r="H71" s="9">
         <v>200</v>
       </c>
-      <c r="I71" s="82" t="s">
+      <c r="I71" s="100" t="s">
         <v>170</v>
       </c>
       <c r="J71" s="9"/>
@@ -5736,7 +5735,7 @@
       <c r="H72" s="9">
         <v>200</v>
       </c>
-      <c r="I72" s="82" t="s">
+      <c r="I72" s="100" t="s">
         <v>171</v>
       </c>
       <c r="J72" s="9"/>
@@ -5788,7 +5787,7 @@
       <c r="H73" s="9">
         <v>200</v>
       </c>
-      <c r="I73" s="82" t="s">
+      <c r="I73" s="100" t="s">
         <v>172</v>
       </c>
       <c r="J73" s="9"/>
@@ -5840,7 +5839,7 @@
       <c r="H74" s="9">
         <v>200</v>
       </c>
-      <c r="I74" s="82" t="s">
+      <c r="I74" s="100" t="s">
         <v>173</v>
       </c>
       <c r="J74" s="9"/>
@@ -5892,7 +5891,7 @@
       <c r="H75" s="16">
         <v>200</v>
       </c>
-      <c r="I75" s="94" t="s">
+      <c r="I75" s="105" t="s">
         <v>174</v>
       </c>
       <c r="J75" s="9"/>
@@ -5944,7 +5943,7 @@
       <c r="H76" s="9">
         <v>50</v>
       </c>
-      <c r="I76" s="82" t="s">
+      <c r="I76" s="100" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5970,7 +5969,7 @@
       <c r="H77" s="9">
         <v>50</v>
       </c>
-      <c r="I77" s="82" t="s">
+      <c r="I77" s="100" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5996,7 +5995,7 @@
       <c r="H78" s="9">
         <v>50</v>
       </c>
-      <c r="I78" s="82" t="s">
+      <c r="I78" s="100" t="s">
         <v>183</v>
       </c>
     </row>
@@ -6022,7 +6021,7 @@
       <c r="H79" s="9">
         <v>50</v>
       </c>
-      <c r="I79" s="82" t="s">
+      <c r="I79" s="100" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6048,7 +6047,7 @@
       <c r="H80" s="9">
         <v>50</v>
       </c>
-      <c r="I80" s="82" t="s">
+      <c r="I80" s="100" t="s">
         <v>185</v>
       </c>
     </row>
@@ -6074,7 +6073,7 @@
       <c r="H81" s="89">
         <v>50</v>
       </c>
-      <c r="I81" s="95" t="s">
+      <c r="I81" s="106" t="s">
         <v>192</v>
       </c>
     </row>
@@ -6100,7 +6099,7 @@
       <c r="H82" s="89">
         <v>50</v>
       </c>
-      <c r="I82" s="95" t="s">
+      <c r="I82" s="106" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6126,7 +6125,7 @@
       <c r="H83" s="89">
         <v>50</v>
       </c>
-      <c r="I83" s="95" t="s">
+      <c r="I83" s="106" t="s">
         <v>194</v>
       </c>
     </row>
@@ -6152,7 +6151,7 @@
       <c r="H84" s="89">
         <v>50</v>
       </c>
-      <c r="I84" s="95" t="s">
+      <c r="I84" s="106" t="s">
         <v>192</v>
       </c>
     </row>
@@ -6178,7 +6177,7 @@
       <c r="H85" s="89">
         <v>50</v>
       </c>
-      <c r="I85" s="95" t="s">
+      <c r="I85" s="106" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6204,7 +6203,7 @@
       <c r="H86" s="89">
         <v>50</v>
       </c>
-      <c r="I86" s="95" t="s">
+      <c r="I86" s="106" t="s">
         <v>194</v>
       </c>
     </row>
@@ -6212,7 +6211,7 @@
       <c r="A87" s="87">
         <v>9069877</v>
       </c>
-      <c r="B87" s="96">
+      <c r="B87" s="90">
         <v>44607</v>
       </c>
       <c r="C87" s="34" t="s">
@@ -6233,7 +6232,7 @@
       <c r="H87" s="34">
         <v>50</v>
       </c>
-      <c r="I87" s="85" t="s">
+      <c r="I87" s="103" t="s">
         <v>206</v>
       </c>
       <c r="J87" s="34">
@@ -6247,7 +6246,7 @@
       <c r="A88" s="46">
         <v>9072918</v>
       </c>
-      <c r="B88" s="97">
+      <c r="B88" s="91">
         <v>44607</v>
       </c>
       <c r="C88" s="44" t="s">
@@ -6268,7 +6267,7 @@
       <c r="H88" s="44">
         <v>50</v>
       </c>
-      <c r="I88" s="93" t="s">
+      <c r="I88" s="104" t="s">
         <v>207</v>
       </c>
       <c r="L88" s="44" t="s">
@@ -6282,7 +6281,7 @@
       <c r="A89" s="46">
         <v>9073202</v>
       </c>
-      <c r="B89" s="97">
+      <c r="B89" s="91">
         <v>44607</v>
       </c>
       <c r="C89" s="44" t="s">
@@ -6303,7 +6302,7 @@
       <c r="H89" s="44">
         <v>50</v>
       </c>
-      <c r="I89" s="93" t="s">
+      <c r="I89" s="104" t="s">
         <v>206</v>
       </c>
       <c r="L89" s="44" t="s">
@@ -6317,7 +6316,7 @@
       <c r="A90" s="46">
         <v>9073205</v>
       </c>
-      <c r="B90" s="97">
+      <c r="B90" s="91">
         <v>44607</v>
       </c>
       <c r="C90" s="44" t="s">
@@ -6338,7 +6337,7 @@
       <c r="H90" s="44">
         <v>50</v>
       </c>
-      <c r="I90" s="93" t="s">
+      <c r="I90" s="104" t="s">
         <v>206</v>
       </c>
       <c r="L90" s="44" t="s">
@@ -6352,7 +6351,7 @@
       <c r="A91" s="46">
         <v>9073207</v>
       </c>
-      <c r="B91" s="97">
+      <c r="B91" s="91">
         <v>44607</v>
       </c>
       <c r="C91" s="44" t="s">
@@ -6373,7 +6372,7 @@
       <c r="H91" s="44">
         <v>50</v>
       </c>
-      <c r="I91" s="93" t="s">
+      <c r="I91" s="104" t="s">
         <v>207</v>
       </c>
       <c r="L91" s="44" t="s">
@@ -6387,7 +6386,7 @@
       <c r="A92" s="46">
         <v>9078965</v>
       </c>
-      <c r="B92" s="97">
+      <c r="B92" s="91">
         <v>44608</v>
       </c>
       <c r="C92" s="44" t="s">
@@ -6408,7 +6407,7 @@
       <c r="H92" s="44">
         <v>50</v>
       </c>
-      <c r="I92" s="93" t="s">
+      <c r="I92" s="104" t="s">
         <v>206</v>
       </c>
       <c r="J92" s="44">
@@ -6422,7 +6421,7 @@
       <c r="A93" s="46">
         <v>9078966</v>
       </c>
-      <c r="B93" s="97">
+      <c r="B93" s="91">
         <v>44608</v>
       </c>
       <c r="C93" s="44" t="s">
@@ -6443,7 +6442,7 @@
       <c r="H93" s="44">
         <v>50</v>
       </c>
-      <c r="I93" s="93" t="s">
+      <c r="I93" s="104" t="s">
         <v>206</v>
       </c>
       <c r="J93" s="44">
@@ -6457,7 +6456,7 @@
       <c r="A94" s="46">
         <v>9078892</v>
       </c>
-      <c r="B94" s="97">
+      <c r="B94" s="91">
         <v>44609</v>
       </c>
       <c r="C94" s="44" t="s">
@@ -6478,7 +6477,7 @@
       <c r="H94" s="44">
         <v>50</v>
       </c>
-      <c r="I94" s="44" t="s">
+      <c r="I94" s="104" t="s">
         <v>214</v>
       </c>
       <c r="J94" s="44">
@@ -6492,7 +6491,7 @@
       <c r="A95" s="46">
         <v>8078894</v>
       </c>
-      <c r="B95" s="97">
+      <c r="B95" s="91">
         <v>44609</v>
       </c>
       <c r="C95" s="44" t="s">
@@ -6513,7 +6512,7 @@
       <c r="H95" s="44">
         <v>50</v>
       </c>
-      <c r="I95" s="44" t="s">
+      <c r="I95" s="104" t="s">
         <v>214</v>
       </c>
       <c r="J95" s="44">
@@ -6527,7 +6526,7 @@
       <c r="A96" s="87">
         <v>9078991</v>
       </c>
-      <c r="B96" s="96">
+      <c r="B96" s="90">
         <v>44609</v>
       </c>
       <c r="C96" s="34" t="s">
@@ -6548,7 +6547,7 @@
       <c r="H96" s="34">
         <v>50</v>
       </c>
-      <c r="I96" s="34" t="s">
+      <c r="I96" s="103" t="s">
         <v>214</v>
       </c>
       <c r="J96" s="34">
@@ -6562,7 +6561,7 @@
       </c>
     </row>
     <row r="97" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="96">
+      <c r="B97" s="90">
         <v>44609</v>
       </c>
       <c r="C97" s="34" t="s">
@@ -6583,7 +6582,7 @@
       <c r="H97" s="34">
         <v>50</v>
       </c>
-      <c r="I97" s="34" t="s">
+      <c r="I97" s="103" t="s">
         <v>214</v>
       </c>
     </row>
@@ -6591,7 +6590,7 @@
       <c r="A98" s="87">
         <v>9088638</v>
       </c>
-      <c r="B98" s="96">
+      <c r="B98" s="90">
         <v>44609</v>
       </c>
       <c r="C98" s="34" t="s">
@@ -6612,7 +6611,7 @@
       <c r="H98" s="34">
         <v>50</v>
       </c>
-      <c r="I98" s="34" t="s">
+      <c r="I98" s="103" t="s">
         <v>221</v>
       </c>
       <c r="J98" s="34">
@@ -6620,6 +6619,64 @@
       </c>
       <c r="K98" s="47">
         <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="34">
+        <v>9095133</v>
+      </c>
+      <c r="B99" s="90">
+        <v>44613</v>
+      </c>
+      <c r="C99" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D99" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E99" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" s="87">
+        <v>128</v>
+      </c>
+      <c r="G99" s="34">
+        <v>1</v>
+      </c>
+      <c r="H99" s="34">
+        <v>50</v>
+      </c>
+      <c r="I99" s="103" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>9095156</v>
+      </c>
+      <c r="B100" s="90">
+        <v>44613</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="D100" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E100" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F100" s="87">
+        <v>128</v>
+      </c>
+      <c r="G100" s="34">
+        <v>1</v>
+      </c>
+      <c r="H100" s="34">
+        <v>50</v>
+      </c>
+      <c r="I100" s="103" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -8189,8 +8246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AI62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A40" zoomScale="156" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9525,7 +9582,7 @@
       <c r="A50" s="39">
         <v>9052126</v>
       </c>
-      <c r="B50" s="98">
+      <c r="B50" s="92">
         <v>44964</v>
       </c>
       <c r="C50" s="85" t="s">
@@ -9552,7 +9609,7 @@
       <c r="A51" s="39">
         <v>9062591</v>
       </c>
-      <c r="B51" s="98">
+      <c r="B51" s="92">
         <v>44969</v>
       </c>
       <c r="C51" s="85" t="s">
@@ -9580,7 +9637,7 @@
       <c r="A52" s="39">
         <v>9062616</v>
       </c>
-      <c r="B52" s="98">
+      <c r="B52" s="92">
         <v>44969</v>
       </c>
       <c r="C52" s="85" t="s">
@@ -9608,7 +9665,7 @@
       <c r="A53" s="39">
         <v>9063219</v>
       </c>
-      <c r="B53" s="98">
+      <c r="B53" s="92">
         <v>44970</v>
       </c>
       <c r="C53" s="85" t="s">
@@ -9636,7 +9693,7 @@
       <c r="A54" s="39">
         <v>9067187</v>
       </c>
-      <c r="B54" s="98">
+      <c r="B54" s="92">
         <v>44971</v>
       </c>
       <c r="C54" s="85" t="s">
@@ -9664,7 +9721,7 @@
       <c r="A55" s="39">
         <v>9069292</v>
       </c>
-      <c r="B55" s="98">
+      <c r="B55" s="92">
         <v>44972</v>
       </c>
       <c r="C55" s="85" t="s">
@@ -9690,7 +9747,7 @@
       <c r="A56" s="39">
         <v>9069293</v>
       </c>
-      <c r="B56" s="98">
+      <c r="B56" s="92">
         <v>44972</v>
       </c>
       <c r="C56" s="85" t="s">
@@ -9716,7 +9773,7 @@
       <c r="A57" s="39">
         <v>9075022</v>
       </c>
-      <c r="B57" s="98">
+      <c r="B57" s="92">
         <v>44973</v>
       </c>
       <c r="C57" s="85" t="s">
@@ -9742,7 +9799,7 @@
       <c r="A58" s="39">
         <v>9081486</v>
       </c>
-      <c r="B58" s="98">
+      <c r="B58" s="92">
         <v>44974</v>
       </c>
       <c r="C58" s="85" t="s">
@@ -9788,6 +9845,9 @@
       <c r="G59" s="39">
         <v>1</v>
       </c>
+      <c r="H59" s="39">
+        <v>319</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
@@ -9837,7 +9897,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
-        <v>9094403</v>
+        <v>9095151</v>
       </c>
       <c r="B62" s="81">
         <v>44977</v>

</xml_diff>

<commit_message>
add multi task encoder
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F09B0DC-E811-FE49-8408-0C0A3200602F}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F95F26CF-FDE0-244C-B97A-EA5AD110717C}"/>
   <bookViews>
-    <workbookView xWindow="-50480" yWindow="1600" windowWidth="30680" windowHeight="21920" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="9160" yWindow="3000" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="230">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -731,6 +731,9 @@
   </si>
   <si>
     <t>OrdMoCoClfV3 (no frozen)</t>
+  </si>
+  <si>
+    <t>Multitask (uniform weight, all features)</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1136,14 +1139,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3424,10 +3419,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI100"/>
+  <dimension ref="A1:AI99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="168" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView topLeftCell="A79" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3440,7 +3435,7 @@
     <col min="6" max="6" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="7.1640625" customWidth="1"/>
     <col min="8" max="8" width="14" style="11" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="99" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -3528,7 +3523,7 @@
       <c r="H2">
         <v>50</v>
       </c>
-      <c r="I2" s="99" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
       <c r="J2" t="s">
@@ -3559,7 +3554,7 @@
       <c r="H3">
         <v>50</v>
       </c>
-      <c r="I3" s="99" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="7">
@@ -3594,7 +3589,7 @@
       <c r="H4">
         <v>50</v>
       </c>
-      <c r="I4" s="99" t="s">
+      <c r="I4" t="s">
         <v>27</v>
       </c>
       <c r="M4" t="s">
@@ -3623,7 +3618,7 @@
       <c r="H5">
         <v>50</v>
       </c>
-      <c r="I5" s="99" t="s">
+      <c r="I5" t="s">
         <v>26</v>
       </c>
       <c r="M5" t="s">
@@ -3652,7 +3647,7 @@
       <c r="H6">
         <v>50</v>
       </c>
-      <c r="I6" s="99" t="s">
+      <c r="I6" t="s">
         <v>26</v>
       </c>
       <c r="M6" t="s">
@@ -3681,7 +3676,7 @@
       <c r="H7">
         <v>50</v>
       </c>
-      <c r="I7" s="99" t="s">
+      <c r="I7" t="s">
         <v>26</v>
       </c>
       <c r="M7" t="s">
@@ -3710,7 +3705,7 @@
       <c r="H8">
         <v>50</v>
       </c>
-      <c r="I8" s="99" t="s">
+      <c r="I8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3736,7 +3731,7 @@
       <c r="H9">
         <v>50</v>
       </c>
-      <c r="I9" s="99" t="s">
+      <c r="I9" t="s">
         <v>48</v>
       </c>
       <c r="M9" t="s">
@@ -3765,7 +3760,7 @@
       <c r="H10">
         <v>50</v>
       </c>
-      <c r="I10" s="99" t="s">
+      <c r="I10" t="s">
         <v>48</v>
       </c>
       <c r="M10" t="s">
@@ -3794,7 +3789,7 @@
       <c r="H11">
         <v>50</v>
       </c>
-      <c r="I11" s="99" t="s">
+      <c r="I11" t="s">
         <v>60</v>
       </c>
       <c r="M11" t="s">
@@ -3826,7 +3821,7 @@
       <c r="H12">
         <v>30</v>
       </c>
-      <c r="I12" s="99" t="s">
+      <c r="I12" t="s">
         <v>61</v>
       </c>
       <c r="M12" t="s">
@@ -3858,7 +3853,7 @@
       <c r="H13">
         <v>30</v>
       </c>
-      <c r="I13" s="99" t="s">
+      <c r="I13" t="s">
         <v>60</v>
       </c>
       <c r="M13" t="s">
@@ -3890,7 +3885,7 @@
       <c r="H14">
         <v>30</v>
       </c>
-      <c r="I14" s="99" t="s">
+      <c r="I14" t="s">
         <v>61</v>
       </c>
       <c r="M14" t="s">
@@ -3922,7 +3917,7 @@
       <c r="H15">
         <v>30</v>
       </c>
-      <c r="I15" s="99" t="s">
+      <c r="I15" t="s">
         <v>60</v>
       </c>
       <c r="L15" s="7">
@@ -3960,7 +3955,7 @@
       <c r="H16">
         <v>30</v>
       </c>
-      <c r="I16" s="99" t="s">
+      <c r="I16" t="s">
         <v>61</v>
       </c>
       <c r="L16" s="7">
@@ -3998,7 +3993,7 @@
       <c r="H17">
         <v>100</v>
       </c>
-      <c r="I17" s="99" t="s">
+      <c r="I17" t="s">
         <v>60</v>
       </c>
       <c r="M17" t="s">
@@ -4030,7 +4025,7 @@
       <c r="H18">
         <v>100</v>
       </c>
-      <c r="I18" s="99" t="s">
+      <c r="I18" t="s">
         <v>61</v>
       </c>
       <c r="M18" t="s">
@@ -4062,7 +4057,7 @@
       <c r="H19">
         <v>100</v>
       </c>
-      <c r="I19" s="99" t="s">
+      <c r="I19" t="s">
         <v>60</v>
       </c>
       <c r="J19">
@@ -4097,7 +4092,7 @@
       <c r="H20">
         <v>100</v>
       </c>
-      <c r="I20" s="99" t="s">
+      <c r="I20" t="s">
         <v>61</v>
       </c>
       <c r="J20">
@@ -4132,7 +4127,7 @@
       <c r="H21">
         <v>100</v>
       </c>
-      <c r="I21" s="99" t="s">
+      <c r="I21" t="s">
         <v>27</v>
       </c>
       <c r="J21">
@@ -4167,7 +4162,7 @@
       <c r="H22">
         <v>100</v>
       </c>
-      <c r="I22" s="99" t="s">
+      <c r="I22" t="s">
         <v>78</v>
       </c>
       <c r="J22">
@@ -4199,7 +4194,7 @@
       <c r="H23">
         <v>100</v>
       </c>
-      <c r="I23" s="99" t="s">
+      <c r="I23" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4225,7 +4220,7 @@
       <c r="H24">
         <v>100</v>
       </c>
-      <c r="I24" s="99" t="s">
+      <c r="I24" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4251,7 +4246,7 @@
       <c r="H25" s="9">
         <v>100</v>
       </c>
-      <c r="I25" s="100" t="s">
+      <c r="I25" s="9" t="s">
         <v>61</v>
       </c>
       <c r="J25" s="9">
@@ -4286,7 +4281,7 @@
       <c r="H26" s="9">
         <v>100</v>
       </c>
-      <c r="I26" s="100" t="s">
+      <c r="I26" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J26" s="9">
@@ -4318,7 +4313,7 @@
       <c r="H27" s="9">
         <v>100</v>
       </c>
-      <c r="I27" s="100" t="s">
+      <c r="I27" s="9" t="s">
         <v>61</v>
       </c>
       <c r="J27" s="9">
@@ -4350,7 +4345,7 @@
       <c r="H28" s="9">
         <v>100</v>
       </c>
-      <c r="I28" s="100" t="s">
+      <c r="I28" s="9" t="s">
         <v>27</v>
       </c>
       <c r="J28" s="9">
@@ -4382,7 +4377,7 @@
       <c r="H29" s="20">
         <v>100</v>
       </c>
-      <c r="I29" s="101" t="s">
+      <c r="I29" s="20" t="s">
         <v>61</v>
       </c>
       <c r="J29" s="20">
@@ -4414,7 +4409,7 @@
       <c r="H30" s="20">
         <v>100</v>
       </c>
-      <c r="I30" s="101" t="s">
+      <c r="I30" s="20" t="s">
         <v>27</v>
       </c>
       <c r="J30" s="20">
@@ -4446,7 +4441,7 @@
       <c r="H31" s="20">
         <v>100</v>
       </c>
-      <c r="I31" s="101" t="s">
+      <c r="I31" s="20" t="s">
         <v>27</v>
       </c>
       <c r="J31" s="20">
@@ -4478,7 +4473,7 @@
       <c r="H32" s="20">
         <v>100</v>
       </c>
-      <c r="I32" s="101" t="s">
+      <c r="I32" s="20" t="s">
         <v>61</v>
       </c>
       <c r="J32" s="20">
@@ -4510,7 +4505,7 @@
       <c r="H33" s="21">
         <v>200</v>
       </c>
-      <c r="I33" s="102" t="s">
+      <c r="I33" s="21" t="s">
         <v>27</v>
       </c>
     </row>
@@ -4536,7 +4531,7 @@
       <c r="H34" s="21">
         <v>200</v>
       </c>
-      <c r="I34" s="102" t="s">
+      <c r="I34" s="21" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4562,7 +4557,7 @@
       <c r="H35" s="20">
         <v>200</v>
       </c>
-      <c r="I35" s="101" t="s">
+      <c r="I35" s="20" t="s">
         <v>97</v>
       </c>
       <c r="J35" s="20">
@@ -4594,7 +4589,7 @@
       <c r="H36" s="20">
         <v>200</v>
       </c>
-      <c r="I36" s="101" t="s">
+      <c r="I36" s="20" t="s">
         <v>97</v>
       </c>
       <c r="J36" s="20">
@@ -4626,7 +4621,7 @@
       <c r="H37" s="20">
         <v>200</v>
       </c>
-      <c r="I37" s="101" t="s">
+      <c r="I37" s="20" t="s">
         <v>97</v>
       </c>
       <c r="J37" s="20">
@@ -4658,7 +4653,7 @@
       <c r="H38" s="20">
         <v>200</v>
       </c>
-      <c r="I38" s="101" t="s">
+      <c r="I38" s="20" t="s">
         <v>101</v>
       </c>
       <c r="J38" s="20">
@@ -4690,7 +4685,7 @@
       <c r="H39" s="20">
         <v>200</v>
       </c>
-      <c r="I39" s="101" t="s">
+      <c r="I39" s="20" t="s">
         <v>102</v>
       </c>
       <c r="J39" s="20">
@@ -4722,7 +4717,7 @@
       <c r="H40" s="20">
         <v>200</v>
       </c>
-      <c r="I40" s="101" t="s">
+      <c r="I40" s="20" t="s">
         <v>101</v>
       </c>
       <c r="J40" s="20">
@@ -4754,7 +4749,7 @@
       <c r="H41" s="20">
         <v>200</v>
       </c>
-      <c r="I41" s="101" t="s">
+      <c r="I41" s="20" t="s">
         <v>102</v>
       </c>
       <c r="J41" s="20">
@@ -4786,7 +4781,7 @@
       <c r="H42" s="20">
         <v>200</v>
       </c>
-      <c r="I42" s="101" t="s">
+      <c r="I42" s="20" t="s">
         <v>120</v>
       </c>
       <c r="J42" s="20"/>
@@ -4813,7 +4808,7 @@
       <c r="H43" s="20">
         <v>200</v>
       </c>
-      <c r="I43" s="101" t="s">
+      <c r="I43" s="20" t="s">
         <v>120</v>
       </c>
       <c r="J43" s="20"/>
@@ -4840,7 +4835,7 @@
       <c r="H44" s="20">
         <v>200</v>
       </c>
-      <c r="I44" s="101" t="s">
+      <c r="I44" s="20" t="s">
         <v>120</v>
       </c>
       <c r="J44" s="20"/>
@@ -4867,7 +4862,7 @@
       <c r="H45" s="34">
         <v>200</v>
       </c>
-      <c r="I45" s="103" t="s">
+      <c r="I45" s="34" t="s">
         <v>128</v>
       </c>
       <c r="J45" s="34">
@@ -4899,7 +4894,7 @@
       <c r="H46" s="34">
         <v>200</v>
       </c>
-      <c r="I46" s="103" t="s">
+      <c r="I46" s="34" t="s">
         <v>129</v>
       </c>
       <c r="J46" s="34">
@@ -4931,7 +4926,7 @@
       <c r="H47" s="44">
         <v>200</v>
       </c>
-      <c r="I47" s="104" t="s">
+      <c r="I47" s="44" t="s">
         <v>131</v>
       </c>
       <c r="M47" s="44" t="s">
@@ -4960,7 +4955,7 @@
       <c r="H48" s="44">
         <v>200</v>
       </c>
-      <c r="I48" s="104" t="s">
+      <c r="I48" s="44" t="s">
         <v>132</v>
       </c>
       <c r="M48" s="44" t="s">
@@ -4989,7 +4984,7 @@
       <c r="H49" s="34">
         <v>200</v>
       </c>
-      <c r="I49" s="103" t="s">
+      <c r="I49" s="34" t="s">
         <v>131</v>
       </c>
       <c r="J49" s="34">
@@ -5021,7 +5016,7 @@
       <c r="H50" s="44">
         <v>200</v>
       </c>
-      <c r="I50" s="104" t="s">
+      <c r="I50" s="44" t="s">
         <v>128</v>
       </c>
       <c r="M50" s="44" t="s">
@@ -5050,7 +5045,7 @@
       <c r="H51" s="34">
         <v>200</v>
       </c>
-      <c r="I51" s="103" t="s">
+      <c r="I51" s="34" t="s">
         <v>131</v>
       </c>
       <c r="J51" s="34">
@@ -5082,7 +5077,7 @@
       <c r="H52" s="34">
         <v>200</v>
       </c>
-      <c r="I52" s="103" t="s">
+      <c r="I52" s="34" t="s">
         <v>132</v>
       </c>
       <c r="J52" s="34">
@@ -5114,7 +5109,7 @@
       <c r="H53" s="34">
         <v>200</v>
       </c>
-      <c r="I53" s="103" t="s">
+      <c r="I53" s="34" t="s">
         <v>128</v>
       </c>
       <c r="J53" s="34">
@@ -5146,7 +5141,7 @@
       <c r="H54" s="34">
         <v>200</v>
       </c>
-      <c r="I54" s="103" t="s">
+      <c r="I54" s="34" t="s">
         <v>131</v>
       </c>
       <c r="J54" s="34">
@@ -5178,7 +5173,7 @@
       <c r="H55" s="34">
         <v>200</v>
       </c>
-      <c r="I55" s="103" t="s">
+      <c r="I55" s="34" t="s">
         <v>128</v>
       </c>
       <c r="J55" s="34">
@@ -5210,7 +5205,7 @@
       <c r="H56" s="34">
         <v>200</v>
       </c>
-      <c r="I56" s="103" t="s">
+      <c r="I56" s="34" t="s">
         <v>131</v>
       </c>
       <c r="J56" s="34">
@@ -5242,7 +5237,7 @@
       <c r="H57" s="34">
         <v>200</v>
       </c>
-      <c r="I57" s="103" t="s">
+      <c r="I57" s="34" t="s">
         <v>128</v>
       </c>
       <c r="J57" s="34">
@@ -5274,7 +5269,7 @@
       <c r="H58" s="34">
         <v>200</v>
       </c>
-      <c r="I58" s="103" t="s">
+      <c r="I58" s="34" t="s">
         <v>147</v>
       </c>
       <c r="J58" s="34">
@@ -5306,7 +5301,7 @@
       <c r="H59" s="44">
         <v>200</v>
       </c>
-      <c r="I59" s="104" t="s">
+      <c r="I59" s="44" t="s">
         <v>148</v>
       </c>
       <c r="M59" s="44" t="s">
@@ -5335,7 +5330,7 @@
       <c r="H60" s="44">
         <v>200</v>
       </c>
-      <c r="I60" s="104" t="s">
+      <c r="I60" s="44" t="s">
         <v>148</v>
       </c>
       <c r="M60" s="44" t="s">
@@ -5364,7 +5359,7 @@
       <c r="H61" s="34">
         <v>200</v>
       </c>
-      <c r="I61" s="103" t="s">
+      <c r="I61" s="34" t="s">
         <v>147</v>
       </c>
       <c r="J61" s="34">
@@ -5396,7 +5391,7 @@
       <c r="H62" s="44">
         <v>200</v>
       </c>
-      <c r="I62" s="104" t="s">
+      <c r="I62" s="44" t="s">
         <v>148</v>
       </c>
       <c r="M62" s="44" t="s">
@@ -5425,7 +5420,7 @@
       <c r="H63" s="44">
         <v>200</v>
       </c>
-      <c r="I63" s="104" t="s">
+      <c r="I63" s="44" t="s">
         <v>148</v>
       </c>
       <c r="M63" s="44" t="s">
@@ -5454,7 +5449,7 @@
       <c r="H64" s="44">
         <v>200</v>
       </c>
-      <c r="I64" s="104" t="s">
+      <c r="I64" s="44" t="s">
         <v>131</v>
       </c>
       <c r="M64" s="44" t="s">
@@ -5483,7 +5478,7 @@
       <c r="H65" s="44">
         <v>200</v>
       </c>
-      <c r="I65" s="104" t="s">
+      <c r="I65" s="44" t="s">
         <v>131</v>
       </c>
       <c r="M65" s="44" t="s">
@@ -5512,7 +5507,7 @@
       <c r="H66" s="9">
         <v>200</v>
       </c>
-      <c r="I66" s="100" t="s">
+      <c r="I66" s="9" t="s">
         <v>166</v>
       </c>
       <c r="J66" s="9">
@@ -5544,7 +5539,7 @@
       <c r="H67" s="9">
         <v>200</v>
       </c>
-      <c r="I67" s="100" t="s">
+      <c r="I67" s="9" t="s">
         <v>166</v>
       </c>
       <c r="M67" s="9" t="s">
@@ -5573,7 +5568,7 @@
       <c r="H68" s="9">
         <v>200</v>
       </c>
-      <c r="I68" s="100" t="s">
+      <c r="I68" s="9" t="s">
         <v>167</v>
       </c>
       <c r="J68" s="9">
@@ -5605,7 +5600,7 @@
       <c r="H69" s="9">
         <v>200</v>
       </c>
-      <c r="I69" s="100" t="s">
+      <c r="I69" s="9" t="s">
         <v>167</v>
       </c>
     </row>
@@ -5631,7 +5626,7 @@
       <c r="H70" s="9">
         <v>200</v>
       </c>
-      <c r="I70" s="100" t="s">
+      <c r="I70" s="9" t="s">
         <v>169</v>
       </c>
       <c r="J70" s="9"/>
@@ -5683,7 +5678,7 @@
       <c r="H71" s="9">
         <v>200</v>
       </c>
-      <c r="I71" s="100" t="s">
+      <c r="I71" s="9" t="s">
         <v>170</v>
       </c>
       <c r="J71" s="9"/>
@@ -5735,7 +5730,7 @@
       <c r="H72" s="9">
         <v>200</v>
       </c>
-      <c r="I72" s="100" t="s">
+      <c r="I72" s="9" t="s">
         <v>171</v>
       </c>
       <c r="J72" s="9"/>
@@ -5787,7 +5782,7 @@
       <c r="H73" s="9">
         <v>200</v>
       </c>
-      <c r="I73" s="100" t="s">
+      <c r="I73" s="9" t="s">
         <v>172</v>
       </c>
       <c r="J73" s="9"/>
@@ -5839,7 +5834,7 @@
       <c r="H74" s="9">
         <v>200</v>
       </c>
-      <c r="I74" s="100" t="s">
+      <c r="I74" s="9" t="s">
         <v>173</v>
       </c>
       <c r="J74" s="9"/>
@@ -5891,7 +5886,7 @@
       <c r="H75" s="16">
         <v>200</v>
       </c>
-      <c r="I75" s="105" t="s">
+      <c r="I75" s="16" t="s">
         <v>174</v>
       </c>
       <c r="J75" s="9"/>
@@ -5943,7 +5938,7 @@
       <c r="H76" s="9">
         <v>50</v>
       </c>
-      <c r="I76" s="100" t="s">
+      <c r="I76" s="9" t="s">
         <v>181</v>
       </c>
     </row>
@@ -5969,7 +5964,7 @@
       <c r="H77" s="9">
         <v>50</v>
       </c>
-      <c r="I77" s="100" t="s">
+      <c r="I77" s="9" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5995,7 +5990,7 @@
       <c r="H78" s="9">
         <v>50</v>
       </c>
-      <c r="I78" s="100" t="s">
+      <c r="I78" s="9" t="s">
         <v>183</v>
       </c>
     </row>
@@ -6021,7 +6016,7 @@
       <c r="H79" s="9">
         <v>50</v>
       </c>
-      <c r="I79" s="100" t="s">
+      <c r="I79" s="9" t="s">
         <v>184</v>
       </c>
     </row>
@@ -6047,7 +6042,7 @@
       <c r="H80" s="9">
         <v>50</v>
       </c>
-      <c r="I80" s="100" t="s">
+      <c r="I80" s="9" t="s">
         <v>185</v>
       </c>
     </row>
@@ -6073,7 +6068,7 @@
       <c r="H81" s="89">
         <v>50</v>
       </c>
-      <c r="I81" s="106" t="s">
+      <c r="I81" s="89" t="s">
         <v>192</v>
       </c>
     </row>
@@ -6099,7 +6094,7 @@
       <c r="H82" s="89">
         <v>50</v>
       </c>
-      <c r="I82" s="106" t="s">
+      <c r="I82" s="89" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6125,7 +6120,7 @@
       <c r="H83" s="89">
         <v>50</v>
       </c>
-      <c r="I83" s="106" t="s">
+      <c r="I83" s="89" t="s">
         <v>194</v>
       </c>
     </row>
@@ -6151,7 +6146,7 @@
       <c r="H84" s="89">
         <v>50</v>
       </c>
-      <c r="I84" s="106" t="s">
+      <c r="I84" s="89" t="s">
         <v>192</v>
       </c>
     </row>
@@ -6177,7 +6172,7 @@
       <c r="H85" s="89">
         <v>50</v>
       </c>
-      <c r="I85" s="106" t="s">
+      <c r="I85" s="89" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6203,7 +6198,7 @@
       <c r="H86" s="89">
         <v>50</v>
       </c>
-      <c r="I86" s="106" t="s">
+      <c r="I86" s="89" t="s">
         <v>194</v>
       </c>
     </row>
@@ -6232,7 +6227,7 @@
       <c r="H87" s="34">
         <v>50</v>
       </c>
-      <c r="I87" s="103" t="s">
+      <c r="I87" s="34" t="s">
         <v>206</v>
       </c>
       <c r="J87" s="34">
@@ -6267,7 +6262,7 @@
       <c r="H88" s="44">
         <v>50</v>
       </c>
-      <c r="I88" s="104" t="s">
+      <c r="I88" s="44" t="s">
         <v>207</v>
       </c>
       <c r="L88" s="44" t="s">
@@ -6302,7 +6297,7 @@
       <c r="H89" s="44">
         <v>50</v>
       </c>
-      <c r="I89" s="104" t="s">
+      <c r="I89" s="44" t="s">
         <v>206</v>
       </c>
       <c r="L89" s="44" t="s">
@@ -6337,7 +6332,7 @@
       <c r="H90" s="44">
         <v>50</v>
       </c>
-      <c r="I90" s="104" t="s">
+      <c r="I90" s="44" t="s">
         <v>206</v>
       </c>
       <c r="L90" s="44" t="s">
@@ -6372,7 +6367,7 @@
       <c r="H91" s="44">
         <v>50</v>
       </c>
-      <c r="I91" s="104" t="s">
+      <c r="I91" s="44" t="s">
         <v>207</v>
       </c>
       <c r="L91" s="44" t="s">
@@ -6407,7 +6402,7 @@
       <c r="H92" s="44">
         <v>50</v>
       </c>
-      <c r="I92" s="104" t="s">
+      <c r="I92" s="44" t="s">
         <v>206</v>
       </c>
       <c r="J92" s="44">
@@ -6442,7 +6437,7 @@
       <c r="H93" s="44">
         <v>50</v>
       </c>
-      <c r="I93" s="104" t="s">
+      <c r="I93" s="44" t="s">
         <v>206</v>
       </c>
       <c r="J93" s="44">
@@ -6477,7 +6472,7 @@
       <c r="H94" s="44">
         <v>50</v>
       </c>
-      <c r="I94" s="104" t="s">
+      <c r="I94" s="44" t="s">
         <v>214</v>
       </c>
       <c r="J94" s="44">
@@ -6512,7 +6507,7 @@
       <c r="H95" s="44">
         <v>50</v>
       </c>
-      <c r="I95" s="104" t="s">
+      <c r="I95" s="44" t="s">
         <v>214</v>
       </c>
       <c r="J95" s="44">
@@ -6547,7 +6542,7 @@
       <c r="H96" s="34">
         <v>50</v>
       </c>
-      <c r="I96" s="103" t="s">
+      <c r="I96" s="34" t="s">
         <v>214</v>
       </c>
       <c r="J96" s="34">
@@ -6561,6 +6556,9 @@
       </c>
     </row>
     <row r="97" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="87">
+        <v>9088638</v>
+      </c>
       <c r="B97" s="90">
         <v>44609</v>
       </c>
@@ -6582,16 +6580,22 @@
       <c r="H97" s="34">
         <v>50</v>
       </c>
-      <c r="I97" s="103" t="s">
-        <v>214</v>
+      <c r="I97" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="J97" s="34">
+        <v>7</v>
+      </c>
+      <c r="K97" s="47">
+        <v>0.59799999999999998</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="87">
-        <v>9088638</v>
+      <c r="A98" s="34">
+        <v>9095133</v>
       </c>
       <c r="B98" s="90">
-        <v>44609</v>
+        <v>44613</v>
       </c>
       <c r="C98" s="34" t="s">
         <v>195</v>
@@ -6611,25 +6615,25 @@
       <c r="H98" s="34">
         <v>50</v>
       </c>
-      <c r="I98" s="103" t="s">
-        <v>221</v>
+      <c r="I98" s="34" t="s">
+        <v>227</v>
       </c>
       <c r="J98" s="34">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="K98" s="47">
-        <v>0.59799999999999998</v>
+        <v>0.64570000000000005</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="34">
-        <v>9095133</v>
+        <v>9095156</v>
       </c>
       <c r="B99" s="90">
         <v>44613</v>
       </c>
       <c r="C99" s="34" t="s">
-        <v>195</v>
+        <v>228</v>
       </c>
       <c r="D99" s="87">
         <v>2.9999999999999997E-4</v>
@@ -6646,37 +6650,14 @@
       <c r="H99" s="34">
         <v>50</v>
       </c>
-      <c r="I99" s="103" t="s">
+      <c r="I99" s="34" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>9095156</v>
-      </c>
-      <c r="B100" s="90">
-        <v>44613</v>
-      </c>
-      <c r="C100" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="D100" s="87">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E100" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="F100" s="87">
-        <v>128</v>
-      </c>
-      <c r="G100" s="34">
-        <v>1</v>
-      </c>
-      <c r="H100" s="34">
-        <v>50</v>
-      </c>
-      <c r="I100" s="103" t="s">
-        <v>227</v>
+      <c r="J99" s="34">
+        <v>37</v>
+      </c>
+      <c r="K99" s="47">
+        <v>0.64529999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -8244,10 +8225,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI62"/>
+  <dimension ref="A1:AI63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="156" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:G63"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9312,9 +9293,7 @@
       <c r="F39" s="39">
         <v>128</v>
       </c>
-      <c r="G39" s="39">
-        <v>1</v>
-      </c>
+      <c r="G39" s="39"/>
       <c r="H39" s="39">
         <v>100</v>
       </c>
@@ -9340,9 +9319,7 @@
       <c r="F40" s="39">
         <v>128</v>
       </c>
-      <c r="G40" s="39">
-        <v>1</v>
-      </c>
+      <c r="G40" s="39"/>
       <c r="H40" s="39">
         <v>300</v>
       </c>
@@ -9366,9 +9343,7 @@
       <c r="F41" s="39">
         <v>128</v>
       </c>
-      <c r="G41" s="39">
-        <v>1</v>
-      </c>
+      <c r="G41" s="39"/>
       <c r="H41" s="39"/>
       <c r="J41" s="85"/>
       <c r="K41" s="39"/>
@@ -9390,9 +9365,7 @@
       <c r="F42" s="39">
         <v>128</v>
       </c>
-      <c r="G42" s="39">
-        <v>1</v>
-      </c>
+      <c r="G42" s="39"/>
       <c r="H42" s="39"/>
       <c r="J42" s="85"/>
       <c r="K42" s="39"/>
@@ -9414,9 +9387,7 @@
       <c r="F43" s="39">
         <v>128</v>
       </c>
-      <c r="G43" s="39">
-        <v>1</v>
-      </c>
+      <c r="G43" s="39"/>
       <c r="H43" s="39">
         <v>300</v>
       </c>
@@ -9440,9 +9411,7 @@
       <c r="F44" s="39">
         <v>128</v>
       </c>
-      <c r="G44" s="39">
-        <v>1</v>
-      </c>
+      <c r="G44" s="39"/>
       <c r="H44" s="39"/>
       <c r="J44" s="85" t="s">
         <v>164</v>
@@ -9466,9 +9435,7 @@
       <c r="F45" s="39">
         <v>128</v>
       </c>
-      <c r="G45" s="39">
-        <v>1</v>
-      </c>
+      <c r="G45" s="39"/>
       <c r="H45" s="39"/>
       <c r="J45" s="85"/>
       <c r="K45" s="39"/>
@@ -9490,9 +9457,7 @@
       <c r="F46" s="39">
         <v>128</v>
       </c>
-      <c r="G46" s="39">
-        <v>1</v>
-      </c>
+      <c r="G46" s="39"/>
       <c r="H46" s="39"/>
       <c r="J46" s="85" t="s">
         <v>190</v>
@@ -9516,9 +9481,7 @@
       <c r="F47" s="79">
         <v>128</v>
       </c>
-      <c r="G47" s="79">
-        <v>1</v>
-      </c>
+      <c r="G47" s="79"/>
       <c r="H47" s="79"/>
       <c r="J47" s="86" t="s">
         <v>188</v>
@@ -9542,9 +9505,7 @@
       <c r="F48" s="39">
         <v>128</v>
       </c>
-      <c r="G48" s="39">
-        <v>1</v>
-      </c>
+      <c r="G48" s="39"/>
       <c r="H48" s="39"/>
       <c r="J48" s="85" t="s">
         <v>191</v>
@@ -9568,9 +9529,7 @@
       <c r="F49" s="79">
         <v>128</v>
       </c>
-      <c r="G49" s="79">
-        <v>1</v>
-      </c>
+      <c r="G49" s="79"/>
       <c r="H49" s="79"/>
       <c r="J49" s="86" t="s">
         <v>189</v>
@@ -9597,9 +9556,7 @@
       <c r="F50" s="39">
         <v>128</v>
       </c>
-      <c r="G50" s="39">
-        <v>1</v>
-      </c>
+      <c r="G50" s="39"/>
       <c r="H50" s="39"/>
       <c r="J50" s="85"/>
       <c r="K50" s="39"/>
@@ -9624,9 +9581,7 @@
       <c r="F51" s="39">
         <v>128</v>
       </c>
-      <c r="G51" s="39">
-        <v>1</v>
-      </c>
+      <c r="G51" s="39"/>
       <c r="J51" s="85" t="s">
         <v>199</v>
       </c>
@@ -9652,9 +9607,7 @@
       <c r="F52" s="39">
         <v>128</v>
       </c>
-      <c r="G52" s="39">
-        <v>1</v>
-      </c>
+      <c r="G52" s="39"/>
       <c r="J52" s="85" t="s">
         <v>198</v>
       </c>
@@ -9680,9 +9633,7 @@
       <c r="F53" s="39">
         <v>128</v>
       </c>
-      <c r="G53" s="39">
-        <v>1</v>
-      </c>
+      <c r="G53" s="39"/>
       <c r="J53" s="85" t="s">
         <v>201</v>
       </c>
@@ -9708,9 +9659,7 @@
       <c r="F54" s="39">
         <v>128</v>
       </c>
-      <c r="G54" s="39">
-        <v>1</v>
-      </c>
+      <c r="G54" s="39"/>
       <c r="J54" s="85" t="s">
         <v>197</v>
       </c>
@@ -9736,9 +9685,7 @@
       <c r="F55" s="39">
         <v>128</v>
       </c>
-      <c r="G55" s="39">
-        <v>1</v>
-      </c>
+      <c r="G55" s="39"/>
       <c r="J55" s="85"/>
       <c r="K55" s="39"/>
       <c r="L55" s="39"/>
@@ -9762,9 +9709,7 @@
       <c r="F56" s="39">
         <v>128</v>
       </c>
-      <c r="G56" s="39">
-        <v>1</v>
-      </c>
+      <c r="G56" s="39"/>
       <c r="J56" s="85"/>
       <c r="K56" s="39"/>
       <c r="L56" s="39"/>
@@ -9788,9 +9733,7 @@
       <c r="F57" s="39">
         <v>128</v>
       </c>
-      <c r="G57" s="39">
-        <v>1</v>
-      </c>
+      <c r="G57" s="39"/>
       <c r="J57" s="85"/>
       <c r="K57" s="39"/>
       <c r="L57" s="39"/>
@@ -9814,9 +9757,7 @@
       <c r="F58" s="39">
         <v>128</v>
       </c>
-      <c r="G58" s="39">
-        <v>1</v>
-      </c>
+      <c r="G58" s="39"/>
       <c r="J58" s="85" t="s">
         <v>223</v>
       </c>
@@ -9842,9 +9783,7 @@
       <c r="F59" s="39">
         <v>128</v>
       </c>
-      <c r="G59" s="39">
-        <v>1</v>
-      </c>
+      <c r="G59" s="39"/>
       <c r="H59" s="39">
         <v>319</v>
       </c>
@@ -9868,9 +9807,7 @@
       <c r="F60" s="39">
         <v>128</v>
       </c>
-      <c r="G60" s="39">
-        <v>1</v>
-      </c>
+      <c r="G60" s="39"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
@@ -9891,9 +9828,7 @@
       <c r="F61" s="39">
         <v>128</v>
       </c>
-      <c r="G61" s="39">
-        <v>1</v>
-      </c>
+      <c r="G61" s="39"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
@@ -9914,8 +9849,26 @@
       <c r="F62" s="39">
         <v>128</v>
       </c>
-      <c r="G62" s="39">
-        <v>1</v>
+      <c r="G62" s="39"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>9097788</v>
+      </c>
+      <c r="B63" s="81">
+        <v>44978</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D63" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F63" s="6">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standardized output from multitaskencoder loss
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F95F26CF-FDE0-244C-B97A-EA5AD110717C}"/>
+  <xr:revisionPtr revIDLastSave="296" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41F6BF3B-1182-7E40-AB7F-5BB4B2A91B13}"/>
   <bookViews>
     <workbookView xWindow="9160" yWindow="3000" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -8228,7 +8228,7 @@
   <dimension ref="A1:AI63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9853,7 +9853,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
-        <v>9097788</v>
+        <v>9097843</v>
       </c>
       <c r="B63" s="81">
         <v>44978</v>

</xml_diff>

<commit_message>
store losses for all tasks for multitask encoder
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41F6BF3B-1182-7E40-AB7F-5BB4B2A91B13}"/>
+  <xr:revisionPtr revIDLastSave="305" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E306789-2104-6049-BBE7-0EBD9AC8C5DB}"/>
   <bookViews>
     <workbookView xWindow="9160" yWindow="3000" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="231">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -724,16 +724,19 @@
     <t>OrdMoCo (projector, inc high-low stress dist, alpha=3)</t>
   </si>
   <si>
-    <t>OrdMoCo (projector, inc high-low stress dist, alpha=2, start from 9069293_300)</t>
-  </si>
-  <si>
     <t>9088855_319</t>
   </si>
   <si>
     <t>OrdMoCoClfV3 (no frozen)</t>
   </si>
   <si>
-    <t>Multitask (uniform weight, all features)</t>
+    <t>OrdMoCo (projector, alpha=2, start from 9069293_300)</t>
+  </si>
+  <si>
+    <t>Multitask (0.01 + uniform weight, all features)</t>
+  </si>
+  <si>
+    <t>Multitask (0.1 + uniform weight, all features)</t>
   </si>
 </sst>
 </file>
@@ -6616,7 +6619,7 @@
         <v>50</v>
       </c>
       <c r="I98" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J98" s="34">
         <v>37</v>
@@ -6633,7 +6636,7 @@
         <v>44613</v>
       </c>
       <c r="C99" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D99" s="87">
         <v>2.9999999999999997E-4</v>
@@ -6651,7 +6654,7 @@
         <v>50</v>
       </c>
       <c r="I99" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J99" s="34">
         <v>37</v>
@@ -8225,10 +8228,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI63"/>
+  <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="156" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9838,7 +9841,7 @@
         <v>44977</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D62" s="39">
         <v>30</v>
@@ -9850,6 +9853,9 @@
         <v>128</v>
       </c>
       <c r="G62" s="39"/>
+      <c r="H62">
+        <v>339</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
@@ -9868,6 +9874,26 @@
         <v>5</v>
       </c>
       <c r="F63" s="6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>9099853</v>
+      </c>
+      <c r="B64" s="81">
+        <v>44979</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D64" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F64" s="6">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solve the re-start issue for MultitaskEnc_train
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E306789-2104-6049-BBE7-0EBD9AC8C5DB}"/>
+  <xr:revisionPtr revIDLastSave="372" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0FDB10-2A55-5143-90C9-109FD903CD00}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="3000" windowWidth="30680" windowHeight="21920" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="15720" yWindow="9640" windowWidth="30240" windowHeight="17440" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="242">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -733,10 +733,43 @@
     <t>OrdMoCo (projector, alpha=2, start from 9069293_300)</t>
   </si>
   <si>
-    <t>Multitask (0.01 + uniform weight, all features)</t>
-  </si>
-  <si>
-    <t>Multitask (0.1 + uniform weight, all features)</t>
+    <t>seems to be dominated by the prediction losses</t>
+  </si>
+  <si>
+    <t>accideintly terminated because of some bugs at iteration 59, restart below</t>
+  </si>
+  <si>
+    <t>MultitaskClfV3</t>
+  </si>
+  <si>
+    <t>9089403_269</t>
+  </si>
+  <si>
+    <t>hasn't converged, restart below</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist, alpha=1, restart from 9089404_399)</t>
+  </si>
+  <si>
+    <t>9089404_399</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, alpha=2, inc high-low stress dict, add no grad to inc)</t>
+  </si>
+  <si>
+    <t>val loss inc very quickly</t>
+  </si>
+  <si>
+    <t>Multitask (SupMoCo + pred, all features)</t>
+  </si>
+  <si>
+    <t>Multitask (0.1 SupMoCo + pred, all features)</t>
+  </si>
+  <si>
+    <t>Multitask (0.01 SupMoCo + pred, all features)</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size)</t>
   </si>
 </sst>
 </file>
@@ -918,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1142,6 +1175,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,8 +1492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AG43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="174" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A18" zoomScale="174" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3422,10 +3456,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI99"/>
+  <dimension ref="A1:AI102"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView topLeftCell="A14" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6663,6 +6697,99 @@
         <v>0.64529999999999998</v>
       </c>
     </row>
+    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="87">
+        <v>9100982</v>
+      </c>
+      <c r="B100" s="90">
+        <v>44980</v>
+      </c>
+      <c r="C100" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="D100" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E100" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F100" s="87">
+        <v>128</v>
+      </c>
+      <c r="G100" s="34">
+        <v>1</v>
+      </c>
+      <c r="H100" s="34">
+        <v>50</v>
+      </c>
+      <c r="I100" s="87" t="s">
+        <v>232</v>
+      </c>
+      <c r="J100" s="34">
+        <v>23</v>
+      </c>
+      <c r="K100" s="47">
+        <v>0.63890000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="87">
+        <v>9113646</v>
+      </c>
+      <c r="B101" s="99">
+        <v>44982</v>
+      </c>
+      <c r="C101" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D101" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E101" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="87">
+        <v>128</v>
+      </c>
+      <c r="G101" s="34">
+        <v>1</v>
+      </c>
+      <c r="H101" s="34">
+        <v>50</v>
+      </c>
+      <c r="I101" s="87" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A102" s="87">
+        <v>9113695</v>
+      </c>
+      <c r="B102" s="99">
+        <v>44982</v>
+      </c>
+      <c r="C102" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="D102" s="87">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E102" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="F102" s="87">
+        <v>128</v>
+      </c>
+      <c r="G102" s="34">
+        <v>1</v>
+      </c>
+      <c r="H102" s="34">
+        <v>50</v>
+      </c>
+      <c r="I102" s="87" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -8228,10 +8355,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI64"/>
+  <dimension ref="A1:AI69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9811,6 +9938,9 @@
         <v>128</v>
       </c>
       <c r="G60" s="39"/>
+      <c r="J60" s="11" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
@@ -9832,6 +9962,9 @@
         <v>128</v>
       </c>
       <c r="G61" s="39"/>
+      <c r="H61">
+        <v>269</v>
+      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
@@ -9865,7 +9998,7 @@
         <v>44978</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D63" s="6">
         <v>0.3</v>
@@ -9875,6 +10008,9 @@
       </c>
       <c r="F63" s="6">
         <v>128</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -9885,7 +10021,7 @@
         <v>44979</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D64" s="6">
         <v>0.3</v>
@@ -9896,6 +10032,108 @@
       <c r="F64" s="6">
         <v>128</v>
       </c>
+      <c r="J64" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>9113636</v>
+      </c>
+      <c r="B65" s="81">
+        <v>44980</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D65" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F65" s="6">
+        <v>128</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>9113632</v>
+      </c>
+      <c r="B66" s="81">
+        <v>44981</v>
+      </c>
+      <c r="C66" s="85" t="s">
+        <v>234</v>
+      </c>
+      <c r="D66" s="39">
+        <v>30</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" s="39">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>9114442</v>
+      </c>
+      <c r="B67" s="81">
+        <v>44982</v>
+      </c>
+      <c r="C67" s="85" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" s="39">
+        <v>30</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="39">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>9116743</v>
+      </c>
+      <c r="B68" s="81">
+        <v>44983</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="D68" s="6">
+        <v>30</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" s="6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B69" s="92">
+        <v>44983</v>
+      </c>
+      <c r="C69" s="85" t="s">
+        <v>241</v>
+      </c>
+      <c r="D69" s="39">
+        <v>30</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
normalize vali loss for res50
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="372" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0FDB10-2A55-5143-90C9-109FD903CD00}"/>
+  <xr:revisionPtr revIDLastSave="462" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C060C0B-F640-DA47-AB30-622A2E2B64A0}"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="9640" windowWidth="30240" windowHeight="17440" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-28860" yWindow="11140" windowWidth="30680" windowHeight="11460" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="254">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -770,6 +770,42 @@
   </si>
   <si>
     <t>SupMoCo (projector, double queue size)</t>
+  </si>
+  <si>
+    <t>terminated due to vector cluster shutdown, restart below from 559</t>
+  </si>
+  <si>
+    <t>terminated due to vector cluster shutdown, restart below from 109</t>
+  </si>
+  <si>
+    <t>terminated due to vector cluster shutdown, restart below from 19</t>
+  </si>
+  <si>
+    <t>terminated due to vector cluster shutdown, restart below from 39</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size, from 9116803_39)</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, alpha=2, inc high-low stress dict, add no grad to inc, start from 9114442_109)</t>
+  </si>
+  <si>
+    <t>Multitask (SupMoCo + pred, all features, start from 9116743_19)</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, inc high-low stress dist, alpha=1, restart from 9113632_559)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, york)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, scarborough)</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, etobicoke)</t>
+  </si>
+  <si>
+    <t>the vali loss seems always much lower than the training loss, not sure why tho</t>
   </si>
 </sst>
 </file>
@@ -951,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1176,6 +1212,34 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3458,8 +3522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI102"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView topLeftCell="A73" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6798,10 +6862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="214" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="F1" zoomScale="214" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7281,6 +7345,75 @@
       </c>
       <c r="M14" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="28">
+        <v>9130500</v>
+      </c>
+      <c r="B15" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="71">
+        <v>128</v>
+      </c>
+      <c r="F15" s="54">
+        <v>11</v>
+      </c>
+      <c r="L15" s="31">
+        <v>0.65610000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="28">
+        <v>9130498</v>
+      </c>
+      <c r="B16" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="71">
+        <v>128</v>
+      </c>
+      <c r="F16" s="108">
+        <v>6</v>
+      </c>
+      <c r="L16" s="31">
+        <v>0.57350000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="28">
+        <v>9130484</v>
+      </c>
+      <c r="B17" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="71">
+        <v>128</v>
+      </c>
+      <c r="F17" s="108">
+        <v>9</v>
+      </c>
+      <c r="L17" s="31">
+        <v>0.59519999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -7468,10 +7601,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD73061-4BAF-F54E-8EFF-64837B56220A}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView zoomScale="255" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A2" zoomScale="255" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7618,6 +7751,57 @@
       </c>
       <c r="L4" s="12">
         <v>0.95299999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>9141632</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="71">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>9141629</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="71">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>9141611</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="71">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -7835,10 +8019,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E99EA194-F5BA-0349-B29E-B82D48F8A802}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView zoomScale="230" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="119" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8159,6 +8343,75 @@
         <v>175</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>9137170</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="71">
+        <v>128</v>
+      </c>
+      <c r="F10" s="8">
+        <v>7</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0.90339999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>9137179</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="C11" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D11" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="71">
+        <v>128</v>
+      </c>
+      <c r="F11" s="109">
+        <v>8</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0.84530000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>9137181</v>
+      </c>
+      <c r="B12" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="71">
+        <v>128</v>
+      </c>
+      <c r="F12" s="109">
+        <v>9</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0.89429999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8166,10 +8419,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5B8BFC-BD6E-0747-8364-88A4C94E808C}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScale="231" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A2" zoomScale="231" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8348,6 +8601,87 @@
         <v>0.88129999999999997</v>
       </c>
     </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>9121817</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="71">
+        <v>128</v>
+      </c>
+      <c r="F6" s="107">
+        <v>10</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0.91010000000000002</v>
+      </c>
+      <c r="M6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>9121825</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="71">
+        <v>128</v>
+      </c>
+      <c r="F7" s="107">
+        <v>12</v>
+      </c>
+      <c r="M7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>9121826</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="C8" s="70">
+        <v>1E-4</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="71">
+        <v>128</v>
+      </c>
+      <c r="F8" s="107">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8355,10 +8689,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AI69"/>
+  <dimension ref="A1:AH73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="141" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8367,16 +8701,15 @@
     <col min="2" max="2" width="11.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="37" style="11" customWidth="1"/>
     <col min="4" max="5" width="8.33203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="6" style="6" customWidth="1"/>
-    <col min="8" max="8" width="5.5" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19" style="11" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" style="6" customWidth="1"/>
-    <col min="12" max="12" width="17.5" style="6" customWidth="1"/>
+    <col min="6" max="6" width="6" style="6" customWidth="1"/>
+    <col min="7" max="7" width="5.5" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" style="11" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8392,17 +8725,15 @@
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="29"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="29"/>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -8425,9 +8756,8 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-    </row>
-    <row r="2" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>8544579</v>
       </c>
@@ -8444,19 +8774,16 @@
         <v>64</v>
       </c>
       <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8">
         <v>50</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="8"/>
       <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>8548727</v>
       </c>
@@ -8473,16 +8800,13 @@
         <v>64</v>
       </c>
       <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
         <v>50</v>
       </c>
-      <c r="J3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>8618521</v>
       </c>
@@ -8499,19 +8823,16 @@
         <v>128</v>
       </c>
       <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8">
         <v>50</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:35" s="36" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:34" s="36" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35">
         <v>8630046</v>
       </c>
@@ -8528,19 +8849,16 @@
         <v>128</v>
       </c>
       <c r="F5" s="35">
-        <v>1</v>
-      </c>
-      <c r="G5" s="35">
         <v>100</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="G5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="35"/>
       <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>8643007</v>
       </c>
@@ -8557,16 +8875,13 @@
         <v>128</v>
       </c>
       <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
         <v>100</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>8643330</v>
       </c>
@@ -8583,13 +8898,10 @@
         <v>128</v>
       </c>
       <c r="F7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>8704485</v>
       </c>
@@ -8606,16 +8918,13 @@
         <v>128</v>
       </c>
       <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
         <v>100</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8704666</v>
       </c>
@@ -8632,13 +8941,10 @@
         <v>128</v>
       </c>
       <c r="F9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>8714665</v>
       </c>
@@ -8655,22 +8961,19 @@
         <v>128</v>
       </c>
       <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8">
         <v>100</v>
       </c>
+      <c r="G10" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="H10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>8714947</v>
       </c>
@@ -8687,16 +8990,13 @@
         <v>128</v>
       </c>
       <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8">
         <v>100</v>
       </c>
-      <c r="J11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>8715114</v>
       </c>
@@ -8713,13 +9013,10 @@
         <v>128</v>
       </c>
       <c r="F12" s="6">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>8719970</v>
       </c>
@@ -8736,13 +9033,10 @@
         <v>128</v>
       </c>
       <c r="F13" s="6">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>8725293</v>
       </c>
@@ -8759,19 +9053,16 @@
         <v>128</v>
       </c>
       <c r="F14" s="6">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6">
         <v>100</v>
       </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
       <c r="H14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>8727149</v>
       </c>
@@ -8788,16 +9079,13 @@
         <v>128</v>
       </c>
       <c r="F15" s="6">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6">
         <v>100</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>8733913</v>
       </c>
@@ -8814,19 +9102,16 @@
         <v>128</v>
       </c>
       <c r="F16" s="6">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6">
         <v>100</v>
       </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
       <c r="H16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>8735495</v>
       </c>
@@ -8843,16 +9128,13 @@
         <v>128</v>
       </c>
       <c r="F17" s="6">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6">
         <v>100</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>8736656</v>
       </c>
@@ -8869,16 +9151,13 @@
         <v>128</v>
       </c>
       <c r="F18" s="6">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6">
         <v>100</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>8741212</v>
       </c>
@@ -8895,19 +9174,16 @@
         <v>128</v>
       </c>
       <c r="F19" s="6">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6">
         <v>300</v>
       </c>
+      <c r="G19" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
         <v>32</v>
       </c>
@@ -8921,19 +9197,16 @@
         <v>128</v>
       </c>
       <c r="F20" s="6">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6">
         <v>300</v>
       </c>
+      <c r="G20" t="s">
+        <v>45</v>
+      </c>
       <c r="H20" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>8751286</v>
       </c>
@@ -8950,22 +9223,19 @@
         <v>128</v>
       </c>
       <c r="F21" s="6">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6">
         <v>300</v>
       </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
       <c r="H21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>8760687</v>
       </c>
@@ -8982,19 +9252,16 @@
         <v>128</v>
       </c>
       <c r="F22" s="6">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6">
         <v>300</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s">
         <v>53</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="H22" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>8761020</v>
       </c>
@@ -9011,19 +9278,16 @@
         <v>128</v>
       </c>
       <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6">
         <v>300</v>
       </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
       <c r="H23" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="37">
         <v>8763825</v>
       </c>
@@ -9040,19 +9304,16 @@
         <v>128</v>
       </c>
       <c r="F24" s="37">
-        <v>1</v>
-      </c>
-      <c r="G24" s="37">
         <v>300</v>
       </c>
-      <c r="H24" s="38" t="s">
+      <c r="G24" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="84"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>8763833</v>
       </c>
@@ -9069,16 +9330,13 @@
         <v>128</v>
       </c>
       <c r="F25" s="6">
-        <v>1</v>
-      </c>
-      <c r="G25" s="6">
         <v>300</v>
       </c>
-      <c r="H25" t="s">
+      <c r="G25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>8763845</v>
       </c>
@@ -9095,16 +9353,13 @@
         <v>128</v>
       </c>
       <c r="F26" s="6">
-        <v>1</v>
-      </c>
-      <c r="G26" s="6">
         <v>300</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>8764388</v>
       </c>
@@ -9121,16 +9376,13 @@
         <v>128</v>
       </c>
       <c r="F27" s="6">
-        <v>1</v>
-      </c>
-      <c r="G27" s="6">
         <v>300</v>
       </c>
-      <c r="H27" t="s">
+      <c r="G27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>8775747</v>
       </c>
@@ -9147,19 +9399,16 @@
         <v>128</v>
       </c>
       <c r="F28" s="6">
-        <v>1</v>
-      </c>
-      <c r="G28" s="6">
         <v>480</v>
       </c>
+      <c r="G28" t="s">
+        <v>70</v>
+      </c>
       <c r="H28" t="s">
-        <v>70</v>
-      </c>
-      <c r="I28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>8776341</v>
       </c>
@@ -9176,16 +9425,13 @@
         <v>128</v>
       </c>
       <c r="F29" s="6">
-        <v>1</v>
-      </c>
-      <c r="G29" s="6">
         <v>500</v>
       </c>
-      <c r="H29" t="s">
+      <c r="G29" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>8782858</v>
       </c>
@@ -9202,16 +9448,13 @@
         <v>128</v>
       </c>
       <c r="F30" s="6">
-        <v>1</v>
-      </c>
-      <c r="G30" s="6">
         <v>500</v>
       </c>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>8783455</v>
       </c>
@@ -9228,16 +9471,13 @@
         <v>128</v>
       </c>
       <c r="F31" s="6">
-        <v>1</v>
-      </c>
-      <c r="G31" s="6">
         <v>500</v>
       </c>
-      <c r="H31" t="s">
+      <c r="G31" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>8786623</v>
       </c>
@@ -9254,16 +9494,13 @@
         <v>128</v>
       </c>
       <c r="F32" s="6">
-        <v>1</v>
-      </c>
-      <c r="G32" s="6">
         <v>500</v>
       </c>
-      <c r="H32" t="s">
+      <c r="G32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>8850812</v>
       </c>
@@ -9280,16 +9517,13 @@
         <v>128</v>
       </c>
       <c r="F33" s="6">
-        <v>1</v>
-      </c>
-      <c r="G33" s="6">
         <v>500</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G33" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>8850814</v>
       </c>
@@ -9306,16 +9540,13 @@
         <v>128</v>
       </c>
       <c r="F34" s="6">
-        <v>1</v>
-      </c>
-      <c r="G34" s="6">
         <v>500</v>
       </c>
-      <c r="H34" t="s">
+      <c r="G34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>8852324</v>
       </c>
@@ -9332,13 +9563,10 @@
         <v>128</v>
       </c>
       <c r="F35" s="6">
-        <v>1</v>
-      </c>
-      <c r="G35" s="6">
         <v>500</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>8852325</v>
       </c>
@@ -9352,16 +9580,13 @@
         <v>5</v>
       </c>
       <c r="F36" s="6">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="G36" s="6">
-        <v>1</v>
-      </c>
-      <c r="H36" s="6">
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>8852525</v>
       </c>
@@ -9375,16 +9600,13 @@
         <v>5</v>
       </c>
       <c r="F37" s="6">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="G37" s="6">
-        <v>1</v>
-      </c>
-      <c r="H37" s="6">
         <v>500</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>8858578</v>
       </c>
@@ -9398,16 +9620,13 @@
         <v>5</v>
       </c>
       <c r="F38" s="6">
-        <v>128</v>
+        <v>1</v>
       </c>
       <c r="G38" s="6">
-        <v>1</v>
-      </c>
-      <c r="H38" s="6">
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="32">
         <v>8878103</v>
       </c>
@@ -9420,20 +9639,17 @@
       <c r="E39" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="39">
-        <v>128</v>
-      </c>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39">
+      <c r="F39" s="39"/>
+      <c r="G39" s="39">
         <v>100</v>
       </c>
-      <c r="J39" s="85" t="s">
+      <c r="I39" s="85" t="s">
         <v>122</v>
       </c>
+      <c r="J39" s="39"/>
       <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-    </row>
-    <row r="40" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="32">
         <v>8878104</v>
       </c>
@@ -9446,18 +9662,15 @@
       <c r="E40" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="39">
-        <v>128</v>
-      </c>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39">
+      <c r="F40" s="39"/>
+      <c r="G40" s="39">
         <v>300</v>
       </c>
-      <c r="J40" s="85"/>
+      <c r="I40" s="85"/>
+      <c r="J40" s="39"/>
       <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-    </row>
-    <row r="41" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="39">
         <v>8893496</v>
       </c>
@@ -9470,16 +9683,13 @@
       <c r="E41" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="39">
-        <v>128</v>
-      </c>
+      <c r="F41" s="39"/>
       <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="J41" s="85"/>
+      <c r="I41" s="85"/>
+      <c r="J41" s="39"/>
       <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
-    </row>
-    <row r="42" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="39">
         <v>8893498</v>
       </c>
@@ -9492,16 +9702,13 @@
       <c r="E42" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="39">
-        <v>128</v>
-      </c>
+      <c r="F42" s="39"/>
       <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="J42" s="85"/>
+      <c r="I42" s="85"/>
+      <c r="J42" s="39"/>
       <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-    </row>
-    <row r="43" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="39">
         <v>8897030</v>
       </c>
@@ -9514,18 +9721,15 @@
       <c r="E43" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F43" s="39">
-        <v>128</v>
-      </c>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39">
+      <c r="F43" s="39"/>
+      <c r="G43" s="39">
         <v>300</v>
       </c>
-      <c r="J43" s="85"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="39"/>
       <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-    </row>
-    <row r="44" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="39">
         <v>8899242</v>
       </c>
@@ -9538,18 +9742,15 @@
       <c r="E44" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="39">
-        <v>128</v>
-      </c>
+      <c r="F44" s="39"/>
       <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="J44" s="85" t="s">
+      <c r="I44" s="85" t="s">
         <v>164</v>
       </c>
+      <c r="J44" s="39"/>
       <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-    </row>
-    <row r="45" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39">
         <v>8905233</v>
       </c>
@@ -9562,16 +9763,13 @@
       <c r="E45" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="39">
-        <v>128</v>
-      </c>
+      <c r="F45" s="39"/>
       <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="J45" s="85"/>
+      <c r="I45" s="85"/>
+      <c r="J45" s="39"/>
       <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-    </row>
-    <row r="46" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39">
         <v>9031422</v>
       </c>
@@ -9584,18 +9782,15 @@
       <c r="E46" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="39">
-        <v>128</v>
-      </c>
+      <c r="F46" s="39"/>
       <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="J46" s="85" t="s">
+      <c r="I46" s="85" t="s">
         <v>190</v>
       </c>
+      <c r="J46" s="39"/>
       <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-    </row>
-    <row r="47" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:11" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="79">
         <v>9031424</v>
       </c>
@@ -9608,18 +9803,15 @@
       <c r="E47" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="79">
-        <v>128</v>
-      </c>
+      <c r="F47" s="79"/>
       <c r="G47" s="79"/>
-      <c r="H47" s="79"/>
-      <c r="J47" s="86" t="s">
+      <c r="I47" s="86" t="s">
         <v>188</v>
       </c>
+      <c r="J47" s="79"/>
       <c r="K47" s="79"/>
-      <c r="L47" s="79"/>
-    </row>
-    <row r="48" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="39">
         <v>9031633</v>
       </c>
@@ -9632,18 +9824,15 @@
       <c r="E48" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="39">
-        <v>128</v>
-      </c>
+      <c r="F48" s="39"/>
       <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="J48" s="85" t="s">
+      <c r="I48" s="85" t="s">
         <v>191</v>
       </c>
+      <c r="J48" s="39"/>
       <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-    </row>
-    <row r="49" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:11" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="79">
         <v>9031630</v>
       </c>
@@ -9656,18 +9845,15 @@
       <c r="E49" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="79">
-        <v>128</v>
-      </c>
+      <c r="F49" s="79"/>
       <c r="G49" s="79"/>
-      <c r="H49" s="79"/>
-      <c r="J49" s="86" t="s">
+      <c r="I49" s="86" t="s">
         <v>189</v>
       </c>
+      <c r="J49" s="79"/>
       <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-    </row>
-    <row r="50" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="39">
         <v>9052126</v>
       </c>
@@ -9683,16 +9869,13 @@
       <c r="E50" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="39">
-        <v>128</v>
-      </c>
+      <c r="F50" s="39"/>
       <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="J50" s="85"/>
+      <c r="I50" s="85"/>
+      <c r="J50" s="39"/>
       <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-    </row>
-    <row r="51" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="39">
         <v>9062591</v>
       </c>
@@ -9708,17 +9891,14 @@
       <c r="E51" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F51" s="39">
-        <v>128</v>
-      </c>
-      <c r="G51" s="39"/>
-      <c r="J51" s="85" t="s">
+      <c r="F51" s="39"/>
+      <c r="I51" s="85" t="s">
         <v>199</v>
       </c>
+      <c r="J51" s="39"/>
       <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
-    </row>
-    <row r="52" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="39">
         <v>9062616</v>
       </c>
@@ -9734,17 +9914,14 @@
       <c r="E52" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="39">
-        <v>128</v>
-      </c>
-      <c r="G52" s="39"/>
-      <c r="J52" s="85" t="s">
+      <c r="F52" s="39"/>
+      <c r="I52" s="85" t="s">
         <v>198</v>
       </c>
+      <c r="J52" s="39"/>
       <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-    </row>
-    <row r="53" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="39">
         <v>9063219</v>
       </c>
@@ -9760,17 +9937,14 @@
       <c r="E53" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="39">
-        <v>128</v>
-      </c>
-      <c r="G53" s="39"/>
-      <c r="J53" s="85" t="s">
+      <c r="F53" s="39"/>
+      <c r="I53" s="85" t="s">
         <v>201</v>
       </c>
+      <c r="J53" s="39"/>
       <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
-    </row>
-    <row r="54" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="39">
         <v>9067187</v>
       </c>
@@ -9786,17 +9960,14 @@
       <c r="E54" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="39">
-        <v>128</v>
-      </c>
-      <c r="G54" s="39"/>
-      <c r="J54" s="85" t="s">
+      <c r="F54" s="39"/>
+      <c r="I54" s="85" t="s">
         <v>197</v>
       </c>
+      <c r="J54" s="39"/>
       <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-    </row>
-    <row r="55" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="39">
         <v>9069292</v>
       </c>
@@ -9812,15 +9983,12 @@
       <c r="E55" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="39">
-        <v>128</v>
-      </c>
-      <c r="G55" s="39"/>
-      <c r="J55" s="85"/>
+      <c r="F55" s="39"/>
+      <c r="I55" s="85"/>
+      <c r="J55" s="39"/>
       <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-    </row>
-    <row r="56" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="39">
         <v>9069293</v>
       </c>
@@ -9836,15 +10004,12 @@
       <c r="E56" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="39">
-        <v>128</v>
-      </c>
-      <c r="G56" s="39"/>
-      <c r="J56" s="85"/>
+      <c r="F56" s="39"/>
+      <c r="I56" s="85"/>
+      <c r="J56" s="39"/>
       <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-    </row>
-    <row r="57" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="39">
         <v>9075022</v>
       </c>
@@ -9860,15 +10025,12 @@
       <c r="E57" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="39">
-        <v>128</v>
-      </c>
-      <c r="G57" s="39"/>
-      <c r="J57" s="85"/>
+      <c r="F57" s="39"/>
+      <c r="I57" s="85"/>
+      <c r="J57" s="39"/>
       <c r="K57" s="39"/>
-      <c r="L57" s="39"/>
-    </row>
-    <row r="58" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="39">
         <v>9081486</v>
       </c>
@@ -9884,17 +10046,14 @@
       <c r="E58" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F58" s="39">
-        <v>128</v>
-      </c>
-      <c r="G58" s="39"/>
-      <c r="J58" s="85" t="s">
+      <c r="F58" s="39"/>
+      <c r="I58" s="85" t="s">
         <v>223</v>
       </c>
+      <c r="J58" s="39"/>
       <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>9088855</v>
       </c>
@@ -9910,15 +10069,12 @@
       <c r="E59" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F59" s="39">
-        <v>128</v>
-      </c>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39">
+      <c r="F59" s="39"/>
+      <c r="G59" s="39">
         <v>319</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>9089404</v>
       </c>
@@ -9934,15 +10090,12 @@
       <c r="E60" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="39">
-        <v>128</v>
-      </c>
-      <c r="G60" s="39"/>
-      <c r="J60" s="11" t="s">
+      <c r="F60" s="39"/>
+      <c r="I60" s="11" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>9089403</v>
       </c>
@@ -9958,15 +10111,12 @@
       <c r="E61" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="39">
-        <v>128</v>
-      </c>
-      <c r="G61" s="39"/>
-      <c r="H61">
+      <c r="F61" s="39"/>
+      <c r="G61">
         <v>269</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>9095151</v>
       </c>
@@ -9982,15 +10132,12 @@
       <c r="E62" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="39">
-        <v>128</v>
-      </c>
-      <c r="G62" s="39"/>
-      <c r="H62">
+      <c r="F62" s="39"/>
+      <c r="G62">
         <v>339</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>9097843</v>
       </c>
@@ -10006,14 +10153,11 @@
       <c r="E63" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F63" s="6">
-        <v>128</v>
-      </c>
-      <c r="J63" s="11" t="s">
+      <c r="I63" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>9099853</v>
       </c>
@@ -10029,14 +10173,11 @@
       <c r="E64" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="6">
-        <v>128</v>
-      </c>
-      <c r="J64" s="11" t="s">
+      <c r="I64" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>9113636</v>
       </c>
@@ -10052,88 +10193,184 @@
       <c r="E65" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="6">
-        <v>128</v>
-      </c>
-      <c r="J65" s="11" t="s">
+      <c r="I65" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" s="6">
+    <row r="66" spans="1:11" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="100">
         <v>9113632</v>
       </c>
-      <c r="B66" s="81">
+      <c r="B66" s="101">
         <v>44981</v>
       </c>
-      <c r="C66" s="85" t="s">
+      <c r="C66" s="102" t="s">
         <v>234</v>
       </c>
-      <c r="D66" s="39">
+      <c r="D66" s="100">
         <v>30</v>
       </c>
-      <c r="E66" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F66" s="39">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="6">
+      <c r="E66" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="F66" s="100"/>
+      <c r="I66" s="102" t="s">
+        <v>242</v>
+      </c>
+      <c r="J66" s="100"/>
+      <c r="K66" s="100"/>
+    </row>
+    <row r="67" spans="1:11" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="100">
         <v>9114442</v>
       </c>
-      <c r="B67" s="81">
+      <c r="B67" s="101">
         <v>44982</v>
       </c>
-      <c r="C67" s="85" t="s">
+      <c r="C67" s="102" t="s">
         <v>236</v>
       </c>
-      <c r="D67" s="39">
+      <c r="D67" s="100">
         <v>30</v>
       </c>
-      <c r="E67" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F67" s="39">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" s="6">
+      <c r="E67" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="F67" s="100"/>
+      <c r="I67" s="102" t="s">
+        <v>243</v>
+      </c>
+      <c r="J67" s="100"/>
+      <c r="K67" s="100"/>
+    </row>
+    <row r="68" spans="1:11" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="100">
         <v>9116743</v>
       </c>
-      <c r="B68" s="81">
+      <c r="B68" s="101">
         <v>44983</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="102" t="s">
         <v>238</v>
       </c>
-      <c r="D68" s="6">
+      <c r="D68" s="100">
         <v>30</v>
       </c>
-      <c r="E68" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F68" s="6">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="92">
+      <c r="E68" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="F68" s="100"/>
+      <c r="I68" s="102" t="s">
+        <v>244</v>
+      </c>
+      <c r="J68" s="100"/>
+      <c r="K68" s="100"/>
+    </row>
+    <row r="69" spans="1:11" s="89" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="100">
+        <v>9116803</v>
+      </c>
+      <c r="B69" s="101">
         <v>44983</v>
       </c>
-      <c r="C69" s="85" t="s">
+      <c r="C69" s="102" t="s">
         <v>241</v>
       </c>
-      <c r="D69" s="39">
+      <c r="D69" s="100">
         <v>30</v>
       </c>
-      <c r="E69" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" s="39"/>
-      <c r="G69" s="39"/>
+      <c r="E69" s="100" t="s">
+        <v>5</v>
+      </c>
+      <c r="F69" s="100"/>
+      <c r="I69" s="102" t="s">
+        <v>245</v>
+      </c>
+      <c r="J69" s="100"/>
+      <c r="K69" s="100"/>
+    </row>
+    <row r="70" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="8">
+        <v>9121884</v>
+      </c>
+      <c r="B70" s="103">
+        <v>44985</v>
+      </c>
+      <c r="C70" s="82" t="s">
+        <v>246</v>
+      </c>
+      <c r="D70" s="8">
+        <v>30</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F70" s="8"/>
+      <c r="G70" s="9">
+        <v>99</v>
+      </c>
+      <c r="I70" s="82"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+    </row>
+    <row r="71" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="8">
+        <v>9121929</v>
+      </c>
+      <c r="B71" s="103">
+        <v>44985</v>
+      </c>
+      <c r="C71" s="82" t="s">
+        <v>247</v>
+      </c>
+      <c r="D71" s="8">
+        <v>30</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="8"/>
+      <c r="I71" s="82"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+    </row>
+    <row r="72" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="8">
+        <v>9121931</v>
+      </c>
+      <c r="B72" s="103">
+        <v>44985</v>
+      </c>
+      <c r="C72" s="82" t="s">
+        <v>248</v>
+      </c>
+      <c r="D72" s="8">
+        <v>30</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="8"/>
+      <c r="I72" s="82"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+    </row>
+    <row r="73" spans="1:11" s="106" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="104"/>
+      <c r="B73" s="104"/>
+      <c r="C73" s="105" t="s">
+        <v>249</v>
+      </c>
+      <c r="D73" s="104">
+        <v>30</v>
+      </c>
+      <c r="E73" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" s="104"/>
+      <c r="I73" s="105"/>
+      <c r="J73" s="104"/>
+      <c r="K73" s="104"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update gen_emb so that we only save the projected embedding (2d). This is to save disc space.
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C060C0B-F640-DA47-AB30-622A2E2B64A0}"/>
+  <xr:revisionPtr revIDLastSave="463" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66D825DC-35A0-C744-AEE4-B9A32B97614F}"/>
   <bookViews>
-    <workbookView xWindow="-28860" yWindow="11140" windowWidth="30680" windowHeight="11460" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-29020" yWindow="15720" windowWidth="30680" windowHeight="11460" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -3522,8 +3522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI102"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A93" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8691,8 +8691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AH73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="141" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="141" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10351,6 +10351,9 @@
         <v>5</v>
       </c>
       <c r="F72" s="8"/>
+      <c r="G72" s="9">
+        <v>69</v>
+      </c>
       <c r="I72" s="82"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>

</xml_diff>

<commit_message>
add evaluation code to the codebase
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="623" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3EF08D7-D895-9540-AA65-ED1C08DDD214}"/>
+  <xr:revisionPtr revIDLastSave="782" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5565FE3-884E-3C40-A49C-44605E37BFA0}"/>
   <bookViews>
-    <workbookView xWindow="-25240" yWindow="7780" windowWidth="33140" windowHeight="16060" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-36700" yWindow="6680" windowWidth="33140" windowHeight="16060" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="276">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -842,6 +842,36 @@
   </si>
   <si>
     <t>Res50 (onehot, scarborough)  + sce2</t>
+  </si>
+  <si>
+    <t>Res50 (onehot, scarborough, biased)</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3 + sce3</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + sce3</t>
+  </si>
+  <si>
+    <t>Havn't converge yet, warm start below</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3 + sce3 (start from 9163516_49)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + sce3 (start from 9163515_48)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + sce2</t>
+  </si>
+  <si>
+    <t>OrdMoCoClfV3 + sce2</t>
+  </si>
+  <si>
+    <t>9121929_219</t>
+  </si>
+  <si>
+    <t>very unstable</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1284,6 +1314,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1600,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
   <dimension ref="A1:AG52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="119" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="A23" zoomScale="165" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3762,10 +3809,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI105"/>
+  <dimension ref="A1:AI120"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="C107" zoomScale="183" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6739,7 +6786,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="81">
         <v>9088638</v>
       </c>
@@ -6774,7 +6821,7 @@
         <v>0.59799999999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="29">
         <v>9095133</v>
       </c>
@@ -6809,7 +6856,7 @@
         <v>0.64570000000000005</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="29">
         <v>9095156</v>
       </c>
@@ -6844,7 +6891,7 @@
         <v>0.64529999999999998</v>
       </c>
     </row>
-    <row r="100" spans="1:11" s="105" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" s="105" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="103">
         <v>9100982</v>
       </c>
@@ -6879,7 +6926,7 @@
         <v>0.63890000000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="81">
         <v>9113646</v>
       </c>
@@ -6911,7 +6958,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="102" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="81">
         <v>9113695</v>
       </c>
@@ -6943,7 +6990,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="1:11" s="105" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" s="105" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="105">
         <v>9145823</v>
       </c>
@@ -6978,7 +7025,7 @@
         <v>0.6472</v>
       </c>
     </row>
-    <row r="104" spans="1:11" s="105" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" s="105" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="105">
         <v>9145859</v>
       </c>
@@ -7010,7 +7057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" s="83" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" s="83" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="83">
         <v>9145892</v>
       </c>
@@ -7044,6 +7091,529 @@
       <c r="K105" s="108">
         <v>0.63939999999999997</v>
       </c>
+    </row>
+    <row r="106" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="29">
+        <v>9163516</v>
+      </c>
+      <c r="B106" s="84">
+        <v>44991</v>
+      </c>
+      <c r="C106" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="D106" s="81">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E106" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F106" s="81">
+        <v>128</v>
+      </c>
+      <c r="G106" s="29">
+        <v>1</v>
+      </c>
+      <c r="H106" s="29">
+        <v>50</v>
+      </c>
+      <c r="I106" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="J106" s="29">
+        <v>49</v>
+      </c>
+      <c r="P106" s="29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="83">
+        <v>9163515</v>
+      </c>
+      <c r="B107" s="107">
+        <v>44991</v>
+      </c>
+      <c r="C107" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D107" s="82">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E107" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F107" s="82">
+        <v>128</v>
+      </c>
+      <c r="G107" s="83">
+        <v>1</v>
+      </c>
+      <c r="H107" s="83">
+        <v>50</v>
+      </c>
+      <c r="I107" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="J107" s="83">
+        <v>48</v>
+      </c>
+      <c r="P107" s="29" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="29">
+        <v>9165365</v>
+      </c>
+      <c r="B108" s="84">
+        <v>44991</v>
+      </c>
+      <c r="C108" s="29" t="s">
+        <v>270</v>
+      </c>
+      <c r="D108" s="81">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E108" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F108" s="81">
+        <v>128</v>
+      </c>
+      <c r="G108" s="29">
+        <v>1</v>
+      </c>
+      <c r="H108" s="29">
+        <v>50</v>
+      </c>
+      <c r="I108" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="J108" s="29">
+        <v>92</v>
+      </c>
+      <c r="K108" s="42">
+        <v>0.81069999999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="83">
+        <v>9165800</v>
+      </c>
+      <c r="B109" s="107">
+        <v>44991</v>
+      </c>
+      <c r="C109" s="83" t="s">
+        <v>271</v>
+      </c>
+      <c r="D109" s="82">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E109" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F109" s="82">
+        <v>128</v>
+      </c>
+      <c r="G109" s="83">
+        <v>1</v>
+      </c>
+      <c r="H109" s="83">
+        <v>50</v>
+      </c>
+      <c r="I109" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="J109" s="83">
+        <v>99</v>
+      </c>
+      <c r="K109" s="108">
+        <v>0.81489999999999996</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="83">
+        <v>9167059</v>
+      </c>
+      <c r="B110" s="107">
+        <v>44991</v>
+      </c>
+      <c r="C110" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="D110" s="82">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E110" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F110" s="82">
+        <v>128</v>
+      </c>
+      <c r="G110" s="83">
+        <v>1</v>
+      </c>
+      <c r="H110" s="83">
+        <v>50</v>
+      </c>
+      <c r="I110" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="J110" s="83">
+        <v>98</v>
+      </c>
+      <c r="K110" s="108">
+        <v>0.68530000000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="29">
+        <v>9167127</v>
+      </c>
+      <c r="B111" s="84">
+        <v>44991</v>
+      </c>
+      <c r="C111" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D111" s="81">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E111" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F111" s="81">
+        <v>128</v>
+      </c>
+      <c r="G111" s="29">
+        <v>1</v>
+      </c>
+      <c r="H111" s="29">
+        <v>50</v>
+      </c>
+      <c r="I111" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="J111" s="29">
+        <v>97</v>
+      </c>
+      <c r="K111" s="42">
+        <v>0.67359999999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="29">
+        <v>9170111</v>
+      </c>
+      <c r="B112" s="84">
+        <v>44992</v>
+      </c>
+      <c r="C112" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="D112" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="E112" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F112" s="81">
+        <v>128</v>
+      </c>
+      <c r="G112" s="29">
+        <v>1</v>
+      </c>
+      <c r="H112" s="29">
+        <v>50</v>
+      </c>
+      <c r="I112" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="J112" s="29">
+        <v>98</v>
+      </c>
+      <c r="K112" s="42">
+        <v>0.81469999999999998</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="83">
+        <v>9170112</v>
+      </c>
+      <c r="B113" s="107">
+        <v>44992</v>
+      </c>
+      <c r="C113" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D113" s="82">
+        <v>1E-3</v>
+      </c>
+      <c r="E113" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F113" s="82">
+        <v>128</v>
+      </c>
+      <c r="G113" s="83">
+        <v>1</v>
+      </c>
+      <c r="H113" s="83">
+        <v>50</v>
+      </c>
+      <c r="I113" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="J113" s="83">
+        <v>97</v>
+      </c>
+      <c r="K113" s="108">
+        <v>0.81879999999999997</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="83">
+        <v>9175239</v>
+      </c>
+      <c r="B114" s="107">
+        <v>44992</v>
+      </c>
+      <c r="C114" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="D114" s="82">
+        <v>1E-3</v>
+      </c>
+      <c r="E114" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F114" s="82">
+        <v>128</v>
+      </c>
+      <c r="G114" s="83">
+        <v>1</v>
+      </c>
+      <c r="H114" s="83">
+        <v>50</v>
+      </c>
+      <c r="I114" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="J114" s="83">
+        <v>92</v>
+      </c>
+      <c r="K114" s="108">
+        <v>0.68759999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="29">
+        <v>9175240</v>
+      </c>
+      <c r="B115" s="84">
+        <v>44992</v>
+      </c>
+      <c r="C115" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D115" s="81">
+        <v>1E-3</v>
+      </c>
+      <c r="E115" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F115" s="81">
+        <v>128</v>
+      </c>
+      <c r="G115" s="29">
+        <v>1</v>
+      </c>
+      <c r="H115" s="29">
+        <v>50</v>
+      </c>
+      <c r="I115" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="J115" s="29">
+        <v>92</v>
+      </c>
+      <c r="K115" s="42">
+        <v>0.67679999999999996</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="29">
+        <v>9176938</v>
+      </c>
+      <c r="B116" s="84">
+        <v>44993</v>
+      </c>
+      <c r="C116" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="D116" s="81">
+        <v>0.01</v>
+      </c>
+      <c r="E116" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" s="81">
+        <v>128</v>
+      </c>
+      <c r="G116" s="29">
+        <v>1</v>
+      </c>
+      <c r="H116" s="29">
+        <v>50</v>
+      </c>
+      <c r="I116" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="J116" s="29">
+        <v>77</v>
+      </c>
+      <c r="K116" s="42">
+        <v>0.81759999999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" s="119" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="119">
+        <v>9176940</v>
+      </c>
+      <c r="B117" s="120">
+        <v>44993</v>
+      </c>
+      <c r="C117" s="119" t="s">
+        <v>268</v>
+      </c>
+      <c r="D117" s="121">
+        <v>0.01</v>
+      </c>
+      <c r="E117" s="121" t="s">
+        <v>5</v>
+      </c>
+      <c r="F117" s="121">
+        <v>128</v>
+      </c>
+      <c r="G117" s="119">
+        <v>1</v>
+      </c>
+      <c r="H117" s="119">
+        <v>50</v>
+      </c>
+      <c r="I117" s="119" t="s">
+        <v>206</v>
+      </c>
+      <c r="J117" s="119">
+        <v>79</v>
+      </c>
+      <c r="K117" s="122">
+        <v>0.82210000000000005</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="29">
+        <v>9182629</v>
+      </c>
+      <c r="B118" s="84">
+        <v>44993</v>
+      </c>
+      <c r="C118" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="D118" s="81">
+        <v>0.01</v>
+      </c>
+      <c r="E118" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="F118" s="81">
+        <v>128</v>
+      </c>
+      <c r="G118" s="29">
+        <v>1</v>
+      </c>
+      <c r="H118" s="29">
+        <v>50</v>
+      </c>
+      <c r="I118" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="J118" s="29">
+        <v>91</v>
+      </c>
+      <c r="K118" s="42">
+        <v>0.81200000000000006</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="83">
+        <v>9185746</v>
+      </c>
+      <c r="B119" s="107">
+        <v>44993</v>
+      </c>
+      <c r="C119" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="D119" s="82">
+        <v>0.01</v>
+      </c>
+      <c r="E119" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F119" s="82">
+        <v>128</v>
+      </c>
+      <c r="G119" s="83">
+        <v>1</v>
+      </c>
+      <c r="H119" s="83">
+        <v>50</v>
+      </c>
+      <c r="I119" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="J119" s="83">
+        <v>74</v>
+      </c>
+      <c r="K119" s="108">
+        <v>0.68210000000000004</v>
+      </c>
+      <c r="L119" s="83" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" s="83" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="83">
+        <v>9192127</v>
+      </c>
+      <c r="B120" s="107">
+        <v>44995</v>
+      </c>
+      <c r="C120" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="D120" s="82">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E120" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="F120" s="82">
+        <v>128</v>
+      </c>
+      <c r="G120" s="83">
+        <v>1</v>
+      </c>
+      <c r="H120" s="83">
+        <v>50</v>
+      </c>
+      <c r="I120" s="83" t="s">
+        <v>206</v>
+      </c>
+      <c r="K120" s="108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7055,8 +7625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA9A435-0915-1440-8C06-1D46D6292DDC}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="114" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7549,7 +8119,7 @@
         <v>249</v>
       </c>
       <c r="C15" s="65">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D15" s="66" t="s">
         <v>5</v>
@@ -7572,7 +8142,7 @@
         <v>250</v>
       </c>
       <c r="C16" s="65">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D16" s="66" t="s">
         <v>5</v>
@@ -7595,7 +8165,7 @@
         <v>251</v>
       </c>
       <c r="C17" s="65">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D17" s="66" t="s">
         <v>5</v>
@@ -7618,7 +8188,7 @@
         <v>250</v>
       </c>
       <c r="C18" s="65">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D18" s="66" t="s">
         <v>5</v>
@@ -7635,13 +8205,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="23">
-        <v>9153954</v>
+        <v>9161726</v>
       </c>
       <c r="B19" s="64" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C19" s="65">
-        <v>1E-4</v>
+        <v>3.0000000000000001E-6</v>
       </c>
       <c r="D19" s="66" t="s">
         <v>5</v>
@@ -7649,7 +8219,12 @@
       <c r="E19" s="66">
         <v>128</v>
       </c>
-      <c r="F19" s="101"/>
+      <c r="F19" s="101">
+        <v>34</v>
+      </c>
+      <c r="L19" s="26">
+        <v>0.57469999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8870,10 +9445,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C5B8BFC-BD6E-0747-8364-88A4C94E808C}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9156,6 +9731,29 @@
         <v>0.84499999999999997</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9159257</v>
+      </c>
+      <c r="B10" s="64" t="s">
+        <v>266</v>
+      </c>
+      <c r="C10" s="65">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="D10" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="66">
+        <v>128</v>
+      </c>
+      <c r="F10" s="100">
+        <v>11</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.8548</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9165,15 +9763,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AH73"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="141" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A52" zoomScale="141" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="6" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="37" style="10" customWidth="1"/>
+    <col min="3" max="3" width="87.6640625" style="10" customWidth="1"/>
     <col min="4" max="5" width="8.33203125" style="6" customWidth="1"/>
     <col min="6" max="6" width="6" style="6" customWidth="1"/>
     <col min="7" max="7" width="5.5" customWidth="1"/>
@@ -10372,28 +10970,28 @@
       <c r="J51" s="34"/>
       <c r="K51" s="34"/>
     </row>
-    <row r="52" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="34">
+    <row r="52" spans="1:11" s="117" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="114">
         <v>9062616</v>
       </c>
-      <c r="B52" s="86">
+      <c r="B52" s="115">
         <v>44969</v>
       </c>
-      <c r="C52" s="79" t="s">
+      <c r="C52" s="116" t="s">
         <v>202</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52" s="114">
         <v>30</v>
       </c>
-      <c r="E52" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="34"/>
-      <c r="I52" s="79" t="s">
+      <c r="E52" s="114" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="114"/>
+      <c r="I52" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="J52" s="34"/>
-      <c r="K52" s="34"/>
+      <c r="J52" s="114"/>
+      <c r="K52" s="114"/>
     </row>
     <row r="53" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34">
@@ -10527,26 +11125,29 @@
       <c r="J58" s="34"/>
       <c r="K58" s="34"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="6">
+    <row r="59" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="32">
         <v>9088855</v>
       </c>
-      <c r="B59" s="75">
+      <c r="B59" s="118">
         <v>44976</v>
       </c>
-      <c r="C59" s="79" t="s">
+      <c r="C59" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="D59" s="34">
+      <c r="D59" s="114">
         <v>30</v>
       </c>
-      <c r="E59" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34">
+      <c r="E59" s="114" t="s">
+        <v>5</v>
+      </c>
+      <c r="F59" s="114"/>
+      <c r="G59" s="114">
         <v>319</v>
       </c>
+      <c r="I59" s="78"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="6">

</xml_diff>

<commit_message>
update loss agg method. Change from sum to mean to avoid numerical issues.
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="926" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E769A5F7-5245-634A-8B17-E90CC2C5D94A}"/>
+  <xr:revisionPtr revIDLastSave="1097" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43B73A6B-8EDF-FE42-9CBB-6EFA330C683A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-33680" yWindow="4360" windowWidth="24860" windowHeight="20100" firstSheet="1" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="301">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -898,20 +898,62 @@
     <t>9194674_149</t>
   </si>
   <si>
-    <t>SupMoCo (projector, double queue size, lts wo volume, tao=0.1)</t>
-  </si>
-  <si>
-    <t>SupMoCo (projector, double queue size, lts wo volume, tao=0.08)</t>
-  </si>
-  <si>
     <t>worse than end to end</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + sce2 (start from 9216112_96)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 + sce3 (start from 9216111_94)</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size, lts wo volume, tau=0.1, start from 9206361_199)</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size, lts wo volume, tau=0.08)</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size, lts wo volume, tau=0.1)</t>
+  </si>
+  <si>
+    <t>9206370_169</t>
+  </si>
+  <si>
+    <t>-------</t>
+  </si>
+  <si>
+    <t>9224733_249</t>
+  </si>
+  <si>
+    <t>TwoStep + sce3</t>
+  </si>
+  <si>
+    <t>------</t>
+  </si>
+  <si>
+    <t>Not worth considering anymore because tau=0.08 is better</t>
+  </si>
+  <si>
+    <t>OrdMoCo (projector, alpha=100, tau=0.08, inc high-low stress dict, add no grad to inc)</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size, lts wo volume, tau=0.09)</t>
+  </si>
+  <si>
+    <t>Sup tau=0.07</t>
+  </si>
+  <si>
+    <t>Sup tau=0.08</t>
+  </si>
+  <si>
+    <t>Sup tau=0.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -933,8 +975,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1025,6 +1073,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1086,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1389,6 +1443,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4202,10 +4265,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI126"/>
+  <dimension ref="A1:AI133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4219,6 +4282,7 @@
     <col min="7" max="7" width="7.1640625" customWidth="1"/>
     <col min="8" max="8" width="14" style="10" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -7871,37 +7935,37 @@
       </c>
     </row>
     <row r="117" spans="1:12" s="102" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="102">
+      <c r="A117" s="137">
         <v>9176940</v>
       </c>
-      <c r="B117" s="103">
+      <c r="B117" s="138">
         <v>44993</v>
       </c>
-      <c r="C117" s="102" t="s">
+      <c r="C117" s="137" t="s">
         <v>268</v>
       </c>
-      <c r="D117" s="104">
+      <c r="D117" s="139">
         <v>0.01</v>
       </c>
-      <c r="E117" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="F117" s="104">
-        <v>128</v>
-      </c>
-      <c r="G117" s="102">
-        <v>1</v>
-      </c>
-      <c r="H117" s="102">
+      <c r="E117" s="139" t="s">
+        <v>5</v>
+      </c>
+      <c r="F117" s="139">
+        <v>128</v>
+      </c>
+      <c r="G117" s="137">
+        <v>1</v>
+      </c>
+      <c r="H117" s="137">
         <v>50</v>
       </c>
-      <c r="I117" s="102" t="s">
+      <c r="I117" s="137" t="s">
         <v>206</v>
       </c>
-      <c r="J117" s="102">
+      <c r="J117" s="137">
         <v>79</v>
       </c>
-      <c r="K117" s="105">
+      <c r="K117" s="140">
         <v>0.82210000000000005</v>
       </c>
     </row>
@@ -8041,8 +8105,14 @@
       <c r="I121" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="K121" s="39" t="s">
-        <v>286</v>
+      <c r="J121" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="K121" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="L121" s="39" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="122" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.2">
@@ -8073,8 +8143,14 @@
       <c r="I122" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="K122" s="39" t="s">
-        <v>286</v>
+      <c r="J122" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="K122" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="L122" s="39" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="123" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.2">
@@ -8105,8 +8181,14 @@
       <c r="I123" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="K123" s="39" t="s">
-        <v>286</v>
+      <c r="J123" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="K123" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="L123" s="39" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="124" spans="1:12" s="39" customFormat="1" x14ac:dyDescent="0.2">
@@ -8137,8 +8219,14 @@
       <c r="I124" s="39" t="s">
         <v>226</v>
       </c>
-      <c r="K124" s="39" t="s">
-        <v>286</v>
+      <c r="J124" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="K124" s="135" t="s">
+        <v>294</v>
+      </c>
+      <c r="L124" s="39" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="125" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
@@ -8180,32 +8268,307 @@
       </c>
     </row>
     <row r="126" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="80">
+      <c r="A126" s="102">
+        <v>9216112</v>
+      </c>
+      <c r="B126" s="103">
+        <v>44999</v>
+      </c>
+      <c r="C126" s="102" t="s">
+        <v>272</v>
+      </c>
+      <c r="D126" s="104">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E126" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="F126" s="104">
+        <v>128</v>
+      </c>
+      <c r="G126" s="102">
+        <v>1</v>
+      </c>
+      <c r="H126" s="102">
+        <v>50</v>
+      </c>
+      <c r="I126" s="102" t="s">
+        <v>283</v>
+      </c>
+      <c r="J126" s="102">
+        <v>94</v>
+      </c>
+      <c r="K126" s="105">
+        <v>0.74890000000000001</v>
+      </c>
+      <c r="L126" s="136" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="80">
+        <v>9216111</v>
+      </c>
+      <c r="B127" s="97">
+        <v>44999</v>
+      </c>
+      <c r="C127" s="80" t="s">
+        <v>268</v>
+      </c>
+      <c r="D127" s="118">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E127" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F127" s="118">
+        <v>128</v>
+      </c>
+      <c r="G127" s="80">
+        <v>1</v>
+      </c>
+      <c r="H127" s="80">
+        <v>50</v>
+      </c>
+      <c r="I127" s="80" t="s">
+        <v>283</v>
+      </c>
+      <c r="J127" s="80">
+        <v>96</v>
+      </c>
+      <c r="K127" s="98">
+        <v>0.90910000000000002</v>
+      </c>
+      <c r="L127" s="80" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="80">
+        <v>9222429</v>
+      </c>
+      <c r="B128" s="97">
+        <v>45000</v>
+      </c>
+      <c r="C128" s="80" t="s">
+        <v>285</v>
+      </c>
+      <c r="D128" s="118">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E128" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F128" s="118">
+        <v>128</v>
+      </c>
+      <c r="G128" s="80">
+        <v>1</v>
+      </c>
+      <c r="H128" s="80">
+        <v>50</v>
+      </c>
+      <c r="I128" s="80" t="s">
+        <v>283</v>
+      </c>
+      <c r="J128" s="80">
+        <v>199</v>
+      </c>
+      <c r="K128" s="98">
+        <v>0.74770000000000003</v>
+      </c>
+      <c r="L128" s="80" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="102">
+        <v>9222428</v>
+      </c>
+      <c r="B129" s="103">
+        <v>45000</v>
+      </c>
+      <c r="C129" s="102" t="s">
+        <v>286</v>
+      </c>
+      <c r="D129" s="104">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E129" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129" s="104">
+        <v>128</v>
+      </c>
+      <c r="G129" s="102">
+        <v>1</v>
+      </c>
+      <c r="H129" s="102">
+        <v>50</v>
+      </c>
+      <c r="I129" s="102" t="s">
+        <v>283</v>
+      </c>
+      <c r="J129" s="102">
+        <v>192</v>
+      </c>
+      <c r="K129" s="105">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="L129" s="80" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="80">
+        <v>9236373</v>
+      </c>
+      <c r="B130" s="97">
+        <v>45001</v>
+      </c>
+      <c r="C130" s="80" t="s">
+        <v>293</v>
+      </c>
+      <c r="D130" s="118">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E130" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F130" s="118">
+        <v>128</v>
+      </c>
+      <c r="G130" s="80">
+        <v>1</v>
+      </c>
+      <c r="H130" s="80">
+        <v>50</v>
+      </c>
+      <c r="I130" s="80" t="s">
+        <v>283</v>
+      </c>
+      <c r="J130" s="132" t="s">
+        <v>294</v>
+      </c>
+      <c r="K130" s="132" t="s">
+        <v>294</v>
+      </c>
+      <c r="L130" s="80" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" s="134" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="137">
         <v>9209702</v>
       </c>
-      <c r="B126" s="97">
+      <c r="B131" s="138">
         <v>44998</v>
       </c>
-      <c r="C126" s="80" t="s">
+      <c r="C131" s="137" t="s">
         <v>205</v>
       </c>
-      <c r="D126" s="118">
+      <c r="D131" s="139">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E126" s="118" t="s">
-        <v>5</v>
-      </c>
-      <c r="F126" s="118">
-        <v>128</v>
-      </c>
-      <c r="G126" s="80">
-        <v>1</v>
-      </c>
-      <c r="H126" s="80">
+      <c r="E131" s="139" t="s">
+        <v>5</v>
+      </c>
+      <c r="F131" s="139">
+        <v>128</v>
+      </c>
+      <c r="G131" s="137">
+        <v>1</v>
+      </c>
+      <c r="H131" s="137">
         <v>50</v>
       </c>
-      <c r="I126" s="80" t="s">
+      <c r="I131" s="137" t="s">
         <v>283</v>
+      </c>
+      <c r="J131" s="137">
+        <v>45</v>
+      </c>
+      <c r="K131" s="140">
+        <v>0.70750000000000002</v>
+      </c>
+      <c r="L131" s="136" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="102">
+        <v>9236457</v>
+      </c>
+      <c r="B132" s="103">
+        <v>45001</v>
+      </c>
+      <c r="C132" s="102" t="s">
+        <v>205</v>
+      </c>
+      <c r="D132" s="104">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E132" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="104">
+        <v>128</v>
+      </c>
+      <c r="G132" s="102">
+        <v>1</v>
+      </c>
+      <c r="H132" s="102">
+        <v>50</v>
+      </c>
+      <c r="I132" s="102" t="s">
+        <v>290</v>
+      </c>
+      <c r="J132" s="102">
+        <v>25</v>
+      </c>
+      <c r="K132" s="105">
+        <v>0.7117</v>
+      </c>
+      <c r="L132" s="80" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="80">
+        <v>9236461</v>
+      </c>
+      <c r="B133" s="97">
+        <v>45001</v>
+      </c>
+      <c r="C133" s="80" t="s">
+        <v>205</v>
+      </c>
+      <c r="D133" s="118">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E133" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133" s="118">
+        <v>128</v>
+      </c>
+      <c r="G133" s="80">
+        <v>1</v>
+      </c>
+      <c r="H133" s="80">
+        <v>50</v>
+      </c>
+      <c r="I133" s="80" t="s">
+        <v>292</v>
+      </c>
+      <c r="J133" s="80">
+        <v>37</v>
+      </c>
+      <c r="K133" s="98">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="L133" s="80" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -10354,10 +10717,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AH76"/>
+  <dimension ref="A1:AH79"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="141" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView topLeftCell="C53" zoomScale="141" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12108,6 +12471,9 @@
         <v>5</v>
       </c>
       <c r="F74" s="34"/>
+      <c r="G74" s="133" t="s">
+        <v>291</v>
+      </c>
       <c r="I74" s="77"/>
       <c r="J74" s="34"/>
       <c r="K74" s="34"/>
@@ -12120,7 +12486,7 @@
         <v>44997</v>
       </c>
       <c r="C75" s="92" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="D75" s="90">
         <v>30</v>
@@ -12129,11 +12495,14 @@
         <v>5</v>
       </c>
       <c r="F75" s="90"/>
+      <c r="G75" s="132" t="s">
+        <v>291</v>
+      </c>
       <c r="I75" s="92"/>
       <c r="J75" s="90"/>
       <c r="K75" s="90"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="80" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="90">
         <v>9206370</v>
       </c>
@@ -12141,7 +12510,7 @@
         <v>44997</v>
       </c>
       <c r="C76" s="92" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D76" s="90">
         <v>30</v>
@@ -12149,6 +12518,79 @@
       <c r="E76" s="90" t="s">
         <v>5</v>
       </c>
+      <c r="F76" s="90"/>
+      <c r="G76" s="80">
+        <v>169</v>
+      </c>
+      <c r="I76" s="92"/>
+      <c r="J76" s="90"/>
+      <c r="K76" s="90"/>
+    </row>
+    <row r="77" spans="1:11" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="90">
+        <v>9237545</v>
+      </c>
+      <c r="B77" s="91">
+        <v>45001</v>
+      </c>
+      <c r="C77" s="92" t="s">
+        <v>297</v>
+      </c>
+      <c r="D77" s="90">
+        <v>30</v>
+      </c>
+      <c r="E77" s="90" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="90"/>
+      <c r="I77" s="92"/>
+      <c r="J77" s="90"/>
+      <c r="K77" s="90"/>
+    </row>
+    <row r="78" spans="1:11" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="90">
+        <v>9224733</v>
+      </c>
+      <c r="B78" s="91">
+        <v>45000</v>
+      </c>
+      <c r="C78" s="92" t="s">
+        <v>287</v>
+      </c>
+      <c r="D78" s="90">
+        <v>30</v>
+      </c>
+      <c r="E78" s="90" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" s="90"/>
+      <c r="G78" s="80">
+        <v>249</v>
+      </c>
+      <c r="I78" s="92"/>
+      <c r="J78" s="90"/>
+      <c r="K78" s="90"/>
+    </row>
+    <row r="79" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="34">
+        <v>9237485</v>
+      </c>
+      <c r="B79" s="83">
+        <v>45001</v>
+      </c>
+      <c r="C79" s="77" t="s">
+        <v>296</v>
+      </c>
+      <c r="D79" s="34">
+        <v>30</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F79" s="34"/>
+      <c r="I79" s="77"/>
+      <c r="J79" s="34"/>
+      <c r="K79" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change default loss for supervised contrastive loss from inner to outer
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1097" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43B73A6B-8EDF-FE42-9CBB-6EFA330C683A}"/>
+  <xr:revisionPtr revIDLastSave="1104" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ACC7F76-2C44-DA4C-9FAA-9C0717BF8FF6}"/>
   <bookViews>
-    <workbookView xWindow="-33680" yWindow="4360" windowWidth="24860" windowHeight="20100" firstSheet="1" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-33680" yWindow="4360" windowWidth="24860" windowHeight="20100" firstSheet="1" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="302">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -947,6 +947,9 @@
   </si>
   <si>
     <t>Sup tau=0.10</t>
+  </si>
+  <si>
+    <t>SupMoCo (projector, double queue size, lts wo volume, tau=0.08, outer)</t>
   </si>
 </sst>
 </file>
@@ -4267,8 +4270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView topLeftCell="A114" zoomScale="132" workbookViewId="0">
+      <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10717,10 +10720,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AH79"/>
+  <dimension ref="A1:AH80"/>
   <sheetViews>
-    <sheetView topLeftCell="C53" zoomScale="141" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12573,7 +12576,7 @@
     </row>
     <row r="79" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="34">
-        <v>9237485</v>
+        <v>9241982</v>
       </c>
       <c r="B79" s="83">
         <v>45001</v>
@@ -12591,6 +12594,27 @@
       <c r="I79" s="77"/>
       <c r="J79" s="34"/>
       <c r="K79" s="34"/>
+    </row>
+    <row r="80" spans="1:11" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="90">
+        <v>9241981</v>
+      </c>
+      <c r="B80" s="91">
+        <v>45002</v>
+      </c>
+      <c r="C80" s="92" t="s">
+        <v>301</v>
+      </c>
+      <c r="D80" s="90">
+        <v>30</v>
+      </c>
+      <c r="E80" s="90" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="90"/>
+      <c r="I80" s="92"/>
+      <c r="J80" s="90"/>
+      <c r="K80" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correct parameters for two step cart
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1913" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10A56344-8A97-DF4A-BFD2-5BB0EF7F3003}"/>
+  <xr:revisionPtr revIDLastSave="1926" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B548129-5193-D945-AEBF-1CC83A8243C2}"/>
   <bookViews>
     <workbookView xWindow="-39700" yWindow="10680" windowWidth="39700" windowHeight="14740" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="393">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -1217,6 +1217,12 @@
   </si>
   <si>
     <t>HieMoCo (york, projector, tau=0.08, lambd=0.95)</t>
+  </si>
+  <si>
+    <t>HieMoCo (etobicoke, projector, tau=0.08, lambd=0.95)</t>
+  </si>
+  <si>
+    <t>HieMoCo (scarborough, projector, tau=0.08, lambd=0.95)</t>
   </si>
 </sst>
 </file>
@@ -1410,7 +1416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1800,16 +1806,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4625,8 +4621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
   <dimension ref="A1:AI164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="137" workbookViewId="0">
-      <selection activeCell="K162" sqref="K162"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="137" workbookViewId="0">
+      <selection activeCell="K164" sqref="K164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10044,6 +10040,9 @@
       <c r="J162" s="39">
         <v>77</v>
       </c>
+      <c r="K162" s="153">
+        <v>0.73409999999999997</v>
+      </c>
     </row>
     <row r="163" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="53">
@@ -10072,6 +10071,12 @@
       </c>
       <c r="I163" s="172" t="s">
         <v>367</v>
+      </c>
+      <c r="J163" s="39">
+        <v>114</v>
+      </c>
+      <c r="K163" s="153">
+        <v>0.75880000000000003</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
@@ -12271,10 +12276,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
-  <dimension ref="A1:AH1048576"/>
+  <dimension ref="A1:AH1048575"/>
   <sheetViews>
     <sheetView topLeftCell="A99" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14810,39 +14815,39 @@
       <c r="J110" s="54"/>
       <c r="K110" s="54"/>
     </row>
-    <row r="111" spans="1:11" s="175" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="173">
-        <v>9485149</v>
-      </c>
-      <c r="B111" s="176">
-        <v>45034</v>
-      </c>
-      <c r="C111" s="174" t="s">
-        <v>12</v>
-      </c>
-      <c r="D111" s="173">
+    <row r="111" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="54">
+        <v>9485138</v>
+      </c>
+      <c r="B111" s="143">
+        <v>45035</v>
+      </c>
+      <c r="C111" s="99" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" s="54">
         <v>30</v>
       </c>
-      <c r="E111" s="173" t="s">
-        <v>5</v>
-      </c>
-      <c r="F111" s="173"/>
-      <c r="G111" s="175">
+      <c r="E111" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F111" s="54"/>
+      <c r="G111" s="39">
         <v>49</v>
       </c>
-      <c r="I111" s="174"/>
-      <c r="J111" s="173"/>
-      <c r="K111" s="173"/>
-    </row>
-    <row r="112" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="54">
-        <v>9485138</v>
+      <c r="I111" s="99"/>
+      <c r="J111" s="54"/>
+      <c r="K111" s="54"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A112" s="6">
+        <v>9487306</v>
       </c>
       <c r="B112" s="143">
         <v>45035</v>
       </c>
       <c r="C112" s="99" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D112" s="54">
         <v>30</v>
@@ -14854,15 +14859,33 @@
       <c r="G112" s="39">
         <v>49</v>
       </c>
-      <c r="I112" s="99"/>
-      <c r="J112" s="54"/>
-      <c r="K112" s="54"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="6">
+        <v>9487307</v>
+      </c>
+      <c r="B113" s="143">
+        <v>45035</v>
+      </c>
+      <c r="C113" s="99" t="s">
+        <v>392</v>
+      </c>
+      <c r="D113" s="54">
+        <v>30</v>
+      </c>
+      <c r="E113" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F113" s="54"/>
+      <c r="G113" s="39">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1048574" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1048574" s="73"/>
     </row>
     <row r="1048575" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1048575" s="73"/>
-    </row>
-    <row r="1048576" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B1048576" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
convert eval scripts to cmd line styles
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1926" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B548129-5193-D945-AEBF-1CC83A8243C2}"/>
+  <xr:revisionPtr revIDLastSave="1935" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{795245B3-A282-0440-8B77-BA3F2BE48589}"/>
   <bookViews>
-    <workbookView xWindow="-39700" yWindow="10680" windowWidth="39700" windowHeight="14740" activeTab="9" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-39700" yWindow="10680" windowWidth="39700" windowHeight="14740" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="393">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -4619,10 +4619,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI164"/>
+  <dimension ref="A1:AI165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="137" workbookViewId="0">
-      <selection activeCell="K164" sqref="K164"/>
+    <sheetView topLeftCell="A98" zoomScale="137" workbookViewId="0">
+      <selection activeCell="J159" sqref="J159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10105,6 +10105,41 @@
         <v>50</v>
       </c>
       <c r="I164" s="172" t="s">
+        <v>367</v>
+      </c>
+      <c r="J164" s="39">
+        <v>160</v>
+      </c>
+      <c r="K164" s="11">
+        <v>0.91720000000000002</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="53">
+        <v>9488194</v>
+      </c>
+      <c r="B165" s="82">
+        <v>45035</v>
+      </c>
+      <c r="C165" s="170" t="s">
+        <v>389</v>
+      </c>
+      <c r="D165" s="170">
+        <v>1E-4</v>
+      </c>
+      <c r="E165" s="170" t="s">
+        <v>5</v>
+      </c>
+      <c r="F165" s="170">
+        <v>128</v>
+      </c>
+      <c r="G165" s="170">
+        <v>1</v>
+      </c>
+      <c r="H165" s="171">
+        <v>50</v>
+      </c>
+      <c r="I165" s="172" t="s">
         <v>367</v>
       </c>
     </row>
@@ -12278,8 +12313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AH1048575"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14833,7 +14868,7 @@
       </c>
       <c r="F111" s="54"/>
       <c r="G111" s="39">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="I111" s="99"/>
       <c r="J111" s="54"/>
@@ -14856,9 +14891,7 @@
         <v>5</v>
       </c>
       <c r="F112" s="54"/>
-      <c r="G112" s="39">
-        <v>49</v>
-      </c>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="6">
@@ -14877,9 +14910,7 @@
         <v>5</v>
       </c>
       <c r="F113" s="54"/>
-      <c r="G113" s="39">
-        <v>49</v>
-      </c>
+      <c r="G113" s="39"/>
     </row>
     <row r="1048574" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1048574" s="73"/>

</xml_diff>

<commit_message>
update MoCo so that we train it on the full dataset
</commit_message>
<xml_diff>
--- a/res/exp_records.xlsx
+++ b/res/exp_records.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/imbo_lin_mail_utoronto_ca/Documents/AutoLTS/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1935" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{795245B3-A282-0440-8B77-BA3F2BE48589}"/>
+  <xr:revisionPtr revIDLastSave="2227" documentId="8_{B8B76244-D9D0-5747-BC88-AC1B9C2A16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A509CC5F-5DAD-6948-8CAC-30746D867E23}"/>
   <bookViews>
-    <workbookView xWindow="-39700" yWindow="10680" windowWidth="39700" windowHeight="14740" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
+    <workbookView xWindow="-23960" yWindow="2680" windowWidth="39700" windowHeight="14740" activeTab="8" xr2:uid="{A7230C82-A41D-5F45-B501-631FA4A16867}"/>
   </bookViews>
   <sheets>
     <sheet name="Res50FC" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1388" uniqueCount="433">
   <si>
     <t>slurm_job_id</t>
   </si>
@@ -1223,6 +1223,126 @@
   </si>
   <si>
     <t>HieMoCo (scarborough, projector, tau=0.08, lambd=0.95)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (york, sce1 prob)</t>
+  </si>
+  <si>
+    <t>9485138_34</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (york, sce2 prob)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (york, sce3 prob)</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (york, LTS wo volume)</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (york, LTS wo volume) + sce2</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (york, LTS wo volume) + sce3</t>
+  </si>
+  <si>
+    <t>SupMoCo (york)</t>
+  </si>
+  <si>
+    <t>SupMoCo (etobicoke)</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (etobicoke, LTS wo volume)</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (etobicoke, LTS wo volume) + sce2</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (etobicoke, LTS wo volume) + sce3</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (scarborough, LTS wo volume)</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (scarborough, LTS wo volume) + sce2</t>
+  </si>
+  <si>
+    <t>Res50-noFC-100-4 (scarborough, LTS wo volume) + sce3</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (etobicoke, sce1 prob)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (etobicoke, sce2 prob)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (etobicoke, sce3 prob)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (scarborough, sce1 prob)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (scarborough, sce2 prob)</t>
+  </si>
+  <si>
+    <t>HieMoCoClfV3 (scarborough, sce3 prob)</t>
+  </si>
+  <si>
+    <t>9487306_39</t>
+  </si>
+  <si>
+    <t>9487307_44</t>
+  </si>
+  <si>
+    <t>SupMoCo (scarborough)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (scarborough, sce1 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (scarborough, sce2 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (scarborough, sce3 prob)</t>
+  </si>
+  <si>
+    <t>9494479_19</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (york, sce1 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (york, sce2 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (york, sce3 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (etobicoke, sce1 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (etobicoke, sce2 prob)</t>
+  </si>
+  <si>
+    <t>SupMoCoClfV3 (etobicoke, sce3 prob)</t>
+  </si>
+  <si>
+    <t>9494478_9</t>
+  </si>
+  <si>
+    <t>9494453_9</t>
+  </si>
+  <si>
+    <t>AutoLTS - SupCon -sce1</t>
+  </si>
+  <si>
+    <t>AutoLTS - SupCon -sce2</t>
+  </si>
+  <si>
+    <t>AutoLTS - SupCon -sce3</t>
+  </si>
+  <si>
+    <t>MoCo (city)</t>
   </si>
 </sst>
 </file>
@@ -1416,7 +1536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1772,16 +1892,6 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1799,13 +1909,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2120,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01ECC99D-8CA5-C548-AE53-24D83CC0DB06}">
-  <dimension ref="A1:AG58"/>
+  <dimension ref="A1:AG67"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="165" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A51" zoomScale="165" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4611,6 +4722,363 @@
       <c r="AF58" s="87"/>
       <c r="AG58" s="87"/>
     </row>
+    <row r="59" spans="1:33" s="88" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="84">
+        <v>9494361</v>
+      </c>
+      <c r="B59" s="85" t="s">
+        <v>397</v>
+      </c>
+      <c r="C59" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D59" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="84">
+        <v>128</v>
+      </c>
+      <c r="F59" s="84">
+        <v>6</v>
+      </c>
+      <c r="G59" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" s="86">
+        <v>0.60970000000000002</v>
+      </c>
+      <c r="K59" s="87"/>
+      <c r="L59" s="87"/>
+      <c r="M59" s="87"/>
+      <c r="N59" s="87"/>
+      <c r="O59" s="87"/>
+      <c r="P59" s="87"/>
+      <c r="Q59" s="87"/>
+      <c r="R59" s="87"/>
+      <c r="S59" s="87"/>
+      <c r="T59" s="87"/>
+      <c r="U59" s="87"/>
+      <c r="V59" s="87"/>
+      <c r="W59" s="87"/>
+      <c r="X59" s="87"/>
+      <c r="Y59" s="87"/>
+      <c r="Z59" s="87"/>
+      <c r="AA59" s="87"/>
+      <c r="AB59" s="87"/>
+      <c r="AC59" s="87"/>
+      <c r="AD59" s="87"/>
+      <c r="AE59" s="87"/>
+      <c r="AF59" s="87"/>
+      <c r="AG59" s="87"/>
+    </row>
+    <row r="60" spans="1:33" s="88" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="84">
+        <v>9495014</v>
+      </c>
+      <c r="B60" s="85" t="s">
+        <v>398</v>
+      </c>
+      <c r="C60" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D60" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="84">
+        <v>128</v>
+      </c>
+      <c r="F60" s="84">
+        <v>6</v>
+      </c>
+      <c r="G60" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" s="86">
+        <v>0.63370000000000004</v>
+      </c>
+      <c r="K60" s="87"/>
+      <c r="L60" s="87"/>
+      <c r="M60" s="87"/>
+      <c r="N60" s="87"/>
+      <c r="O60" s="87"/>
+      <c r="P60" s="87"/>
+      <c r="Q60" s="87"/>
+      <c r="R60" s="87"/>
+      <c r="S60" s="87"/>
+      <c r="T60" s="87"/>
+      <c r="U60" s="87"/>
+      <c r="V60" s="87"/>
+      <c r="W60" s="87"/>
+      <c r="X60" s="87"/>
+      <c r="Y60" s="87"/>
+      <c r="Z60" s="87"/>
+      <c r="AA60" s="87"/>
+      <c r="AB60" s="87"/>
+      <c r="AC60" s="87"/>
+      <c r="AD60" s="87"/>
+      <c r="AE60" s="87"/>
+      <c r="AF60" s="87"/>
+      <c r="AG60" s="87"/>
+    </row>
+    <row r="61" spans="1:33" s="88" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="84">
+        <v>9495013</v>
+      </c>
+      <c r="B61" s="85" t="s">
+        <v>399</v>
+      </c>
+      <c r="C61" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D61" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="84">
+        <v>128</v>
+      </c>
+      <c r="F61" s="84">
+        <v>6</v>
+      </c>
+      <c r="G61" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" s="86">
+        <v>0.89229999999999998</v>
+      </c>
+      <c r="K61" s="87"/>
+      <c r="L61" s="87"/>
+      <c r="M61" s="87"/>
+      <c r="N61" s="87"/>
+      <c r="O61" s="87"/>
+      <c r="P61" s="87"/>
+      <c r="Q61" s="87"/>
+      <c r="R61" s="87"/>
+      <c r="S61" s="87"/>
+      <c r="T61" s="87"/>
+      <c r="U61" s="87"/>
+      <c r="V61" s="87"/>
+      <c r="W61" s="87"/>
+      <c r="X61" s="87"/>
+      <c r="Y61" s="87"/>
+      <c r="Z61" s="87"/>
+      <c r="AA61" s="87"/>
+      <c r="AB61" s="87"/>
+      <c r="AC61" s="87"/>
+      <c r="AD61" s="87"/>
+      <c r="AE61" s="87"/>
+      <c r="AF61" s="87"/>
+      <c r="AG61" s="87"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>9495206</v>
+      </c>
+      <c r="B62" s="85" t="s">
+        <v>402</v>
+      </c>
+      <c r="C62" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D62" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="84">
+        <v>128</v>
+      </c>
+      <c r="F62" s="84">
+        <v>11</v>
+      </c>
+      <c r="G62" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J62" s="4">
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>9495201</v>
+      </c>
+      <c r="B63" s="85" t="s">
+        <v>403</v>
+      </c>
+      <c r="C63" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D63" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="84">
+        <v>128</v>
+      </c>
+      <c r="F63" s="84">
+        <v>7</v>
+      </c>
+      <c r="G63" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" s="4">
+        <v>0.66210000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>9495204</v>
+      </c>
+      <c r="B64" s="85" t="s">
+        <v>404</v>
+      </c>
+      <c r="C64" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D64" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="84">
+        <v>128</v>
+      </c>
+      <c r="F64" s="84">
+        <v>11</v>
+      </c>
+      <c r="G64" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H64" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I64" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
+        <v>0.81010000000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>9496447</v>
+      </c>
+      <c r="B65" s="85" t="s">
+        <v>405</v>
+      </c>
+      <c r="C65" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D65" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="84">
+        <v>128</v>
+      </c>
+      <c r="F65" s="3">
+        <v>8</v>
+      </c>
+      <c r="G65" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J65" s="4">
+        <v>0.64280000000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>9496458</v>
+      </c>
+      <c r="B66" s="85" t="s">
+        <v>406</v>
+      </c>
+      <c r="C66" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D66" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="84">
+        <v>128</v>
+      </c>
+      <c r="F66" s="3">
+        <v>2</v>
+      </c>
+      <c r="G66" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I66" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J66" s="4">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>9496456</v>
+      </c>
+      <c r="B67" s="85" t="s">
+        <v>407</v>
+      </c>
+      <c r="C67" s="84">
+        <v>1E-4</v>
+      </c>
+      <c r="D67" s="84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="84">
+        <v>128</v>
+      </c>
+      <c r="F67" s="3">
+        <v>13</v>
+      </c>
+      <c r="G67" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="84" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="84" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" s="4">
+        <v>0.91449999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4619,10 +5087,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109032B-B2DB-8445-873A-289912732FBA}">
-  <dimension ref="A1:AI165"/>
+  <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" zoomScale="137" workbookViewId="0">
-      <selection activeCell="J159" sqref="J159"/>
+    <sheetView topLeftCell="A164" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8849,41 +9317,41 @@
         <v>298</v>
       </c>
     </row>
-    <row r="132" spans="1:14" s="157" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="155">
+    <row r="132" spans="1:14" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="150">
         <v>9236457</v>
       </c>
-      <c r="B132" s="156">
+      <c r="B132" s="96">
         <v>45001</v>
       </c>
-      <c r="C132" s="157" t="s">
+      <c r="C132" s="80" t="s">
         <v>205</v>
       </c>
-      <c r="D132" s="158">
+      <c r="D132" s="117">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="E132" s="158" t="s">
-        <v>5</v>
-      </c>
-      <c r="F132" s="158">
-        <v>128</v>
-      </c>
-      <c r="G132" s="157">
-        <v>1</v>
-      </c>
-      <c r="H132" s="157">
+      <c r="E132" s="117" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="117">
+        <v>128</v>
+      </c>
+      <c r="G132" s="80">
+        <v>1</v>
+      </c>
+      <c r="H132" s="80">
         <v>50</v>
       </c>
-      <c r="I132" s="159" t="s">
+      <c r="I132" s="91" t="s">
         <v>290</v>
       </c>
-      <c r="J132" s="157">
+      <c r="J132" s="80">
         <v>25</v>
       </c>
-      <c r="K132" s="160">
+      <c r="K132" s="97">
         <v>0.7117</v>
       </c>
-      <c r="L132" s="157" t="s">
+      <c r="L132" s="80" t="s">
         <v>299</v>
       </c>
     </row>
@@ -8963,41 +9431,41 @@
         <v>303</v>
       </c>
     </row>
-    <row r="135" spans="1:14" s="157" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="155">
+    <row r="135" spans="1:14" s="80" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="150">
         <v>9263472</v>
       </c>
-      <c r="B135" s="156">
+      <c r="B135" s="96">
         <v>45004</v>
       </c>
-      <c r="C135" s="157" t="s">
+      <c r="C135" s="80" t="s">
         <v>205</v>
       </c>
-      <c r="D135" s="158">
+      <c r="D135" s="117">
         <v>1E-4</v>
       </c>
-      <c r="E135" s="158" t="s">
-        <v>5</v>
-      </c>
-      <c r="F135" s="158">
-        <v>128</v>
-      </c>
-      <c r="G135" s="157">
-        <v>1</v>
-      </c>
-      <c r="H135" s="157">
+      <c r="E135" s="117" t="s">
+        <v>5</v>
+      </c>
+      <c r="F135" s="117">
+        <v>128</v>
+      </c>
+      <c r="G135" s="80">
+        <v>1</v>
+      </c>
+      <c r="H135" s="80">
         <v>50</v>
       </c>
-      <c r="I135" s="159" t="s">
+      <c r="I135" s="91" t="s">
         <v>302</v>
       </c>
-      <c r="J135" s="157">
+      <c r="J135" s="80">
         <v>13</v>
       </c>
-      <c r="K135" s="160">
+      <c r="K135" s="97">
         <v>0.71260000000000001</v>
       </c>
-      <c r="L135" s="157" t="s">
+      <c r="L135" s="80" t="s">
         <v>303</v>
       </c>
     </row>
@@ -9512,44 +9980,44 @@
       </c>
       <c r="Q148" s="153"/>
     </row>
-    <row r="149" spans="1:17" s="163" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="161">
+    <row r="149" spans="1:17" s="157" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="155">
         <v>9408911</v>
       </c>
-      <c r="B149" s="162">
+      <c r="B149" s="156">
         <v>45025</v>
       </c>
-      <c r="C149" s="163" t="s">
+      <c r="C149" s="157" t="s">
         <v>349</v>
       </c>
-      <c r="D149" s="163">
+      <c r="D149" s="157">
         <v>1E-4</v>
       </c>
-      <c r="E149" s="163" t="s">
-        <v>5</v>
-      </c>
-      <c r="F149" s="163">
-        <v>128</v>
-      </c>
-      <c r="G149" s="163">
-        <v>1</v>
-      </c>
-      <c r="H149" s="161">
+      <c r="E149" s="157" t="s">
+        <v>5</v>
+      </c>
+      <c r="F149" s="157">
+        <v>128</v>
+      </c>
+      <c r="G149" s="157">
+        <v>1</v>
+      </c>
+      <c r="H149" s="155">
         <v>50</v>
       </c>
-      <c r="I149" s="164" t="s">
+      <c r="I149" s="158" t="s">
         <v>367</v>
       </c>
-      <c r="J149" s="163">
+      <c r="J149" s="157">
         <v>93</v>
       </c>
-      <c r="K149" s="165">
+      <c r="K149" s="159">
         <v>0.71109999999999995</v>
       </c>
-      <c r="L149" s="163" t="s">
+      <c r="L149" s="157" t="s">
         <v>371</v>
       </c>
-      <c r="Q149" s="165"/>
+      <c r="Q149" s="159"/>
     </row>
     <row r="150" spans="1:17" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="53">
@@ -9863,79 +10331,79 @@
       </c>
       <c r="Q157" s="153"/>
     </row>
-    <row r="158" spans="1:17" s="163" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="161">
+    <row r="158" spans="1:17" s="157" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="155">
         <v>9467660</v>
       </c>
-      <c r="B158" s="162">
+      <c r="B158" s="156">
         <v>45030</v>
       </c>
-      <c r="C158" s="163" t="s">
+      <c r="C158" s="157" t="s">
         <v>384</v>
       </c>
-      <c r="D158" s="163">
+      <c r="D158" s="157">
         <v>1E-4</v>
       </c>
-      <c r="E158" s="163" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="163">
-        <v>128</v>
-      </c>
-      <c r="G158" s="163">
-        <v>1</v>
-      </c>
-      <c r="H158" s="161">
+      <c r="E158" s="157" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" s="157">
+        <v>128</v>
+      </c>
+      <c r="G158" s="157">
+        <v>1</v>
+      </c>
+      <c r="H158" s="155">
         <v>50</v>
       </c>
-      <c r="I158" s="164" t="s">
+      <c r="I158" s="158" t="s">
         <v>367</v>
       </c>
-      <c r="J158" s="163">
+      <c r="J158" s="157">
         <v>234</v>
       </c>
-      <c r="K158" s="165">
+      <c r="K158" s="159">
         <v>0.90600000000000003</v>
       </c>
-      <c r="L158" s="163" t="s">
+      <c r="L158" s="157" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="159" spans="1:17" s="163" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="161">
+    <row r="159" spans="1:17" s="157" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="155">
         <v>9467662</v>
       </c>
-      <c r="B159" s="162">
+      <c r="B159" s="156">
         <v>45030</v>
       </c>
-      <c r="C159" s="166" t="s">
+      <c r="C159" s="160" t="s">
         <v>385</v>
       </c>
-      <c r="D159" s="163">
+      <c r="D159" s="157">
         <v>1E-4</v>
       </c>
-      <c r="E159" s="166" t="s">
-        <v>5</v>
-      </c>
-      <c r="F159" s="166">
-        <v>128</v>
-      </c>
-      <c r="G159" s="166">
-        <v>1</v>
-      </c>
-      <c r="H159" s="167">
+      <c r="E159" s="160" t="s">
+        <v>5</v>
+      </c>
+      <c r="F159" s="160">
+        <v>128</v>
+      </c>
+      <c r="G159" s="160">
+        <v>1</v>
+      </c>
+      <c r="H159" s="161">
         <v>50</v>
       </c>
-      <c r="I159" s="168" t="s">
+      <c r="I159" s="162" t="s">
         <v>367</v>
       </c>
-      <c r="J159" s="166">
+      <c r="J159" s="160">
         <v>167</v>
       </c>
-      <c r="K159" s="169">
+      <c r="K159" s="163">
         <v>0.74339999999999995</v>
       </c>
-      <c r="L159" s="166" t="s">
+      <c r="L159" s="160" t="s">
         <v>371</v>
       </c>
     </row>
@@ -9946,25 +10414,25 @@
       <c r="B160" s="82">
         <v>45034</v>
       </c>
-      <c r="C160" s="170" t="s">
+      <c r="C160" s="39" t="s">
         <v>386</v>
       </c>
-      <c r="D160" s="170">
+      <c r="D160" s="39">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="E160" s="170" t="s">
-        <v>5</v>
-      </c>
-      <c r="F160" s="170">
-        <v>128</v>
-      </c>
-      <c r="G160" s="170">
-        <v>1</v>
-      </c>
-      <c r="H160" s="171">
+      <c r="E160" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F160" s="39">
+        <v>128</v>
+      </c>
+      <c r="G160" s="39">
+        <v>1</v>
+      </c>
+      <c r="H160" s="53">
         <v>50</v>
       </c>
-      <c r="I160" s="172" t="s">
+      <c r="I160" s="99" t="s">
         <v>367</v>
       </c>
       <c r="J160" s="39">
@@ -9981,25 +10449,25 @@
       <c r="B161" s="82">
         <v>45034</v>
       </c>
-      <c r="C161" s="170" t="s">
+      <c r="C161" s="39" t="s">
         <v>386</v>
       </c>
-      <c r="D161" s="170">
+      <c r="D161" s="39">
         <v>1E-4</v>
       </c>
-      <c r="E161" s="170" t="s">
-        <v>5</v>
-      </c>
-      <c r="F161" s="170">
-        <v>128</v>
-      </c>
-      <c r="G161" s="170">
-        <v>1</v>
-      </c>
-      <c r="H161" s="171">
+      <c r="E161" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F161" s="39">
+        <v>128</v>
+      </c>
+      <c r="G161" s="39">
+        <v>1</v>
+      </c>
+      <c r="H161" s="53">
         <v>50</v>
       </c>
-      <c r="I161" s="172" t="s">
+      <c r="I161" s="99" t="s">
         <v>367</v>
       </c>
       <c r="J161" s="39">
@@ -10016,25 +10484,25 @@
       <c r="B162" s="82">
         <v>45035</v>
       </c>
-      <c r="C162" s="170" t="s">
+      <c r="C162" s="39" t="s">
         <v>387</v>
       </c>
-      <c r="D162" s="170">
+      <c r="D162" s="39">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="E162" s="170" t="s">
-        <v>5</v>
-      </c>
-      <c r="F162" s="170">
-        <v>128</v>
-      </c>
-      <c r="G162" s="170">
-        <v>1</v>
-      </c>
-      <c r="H162" s="171">
+      <c r="E162" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F162" s="39">
+        <v>128</v>
+      </c>
+      <c r="G162" s="39">
+        <v>1</v>
+      </c>
+      <c r="H162" s="53">
         <v>50</v>
       </c>
-      <c r="I162" s="172" t="s">
+      <c r="I162" s="99" t="s">
         <v>367</v>
       </c>
       <c r="J162" s="39">
@@ -10051,25 +10519,25 @@
       <c r="B163" s="82">
         <v>45035</v>
       </c>
-      <c r="C163" s="170" t="s">
+      <c r="C163" s="39" t="s">
         <v>388</v>
       </c>
-      <c r="D163" s="170">
+      <c r="D163" s="39">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="E163" s="170" t="s">
-        <v>5</v>
-      </c>
-      <c r="F163" s="170">
-        <v>128</v>
-      </c>
-      <c r="G163" s="170">
-        <v>1</v>
-      </c>
-      <c r="H163" s="171">
+      <c r="E163" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F163" s="39">
+        <v>128</v>
+      </c>
+      <c r="G163" s="39">
+        <v>1</v>
+      </c>
+      <c r="H163" s="53">
         <v>50</v>
       </c>
-      <c r="I163" s="172" t="s">
+      <c r="I163" s="99" t="s">
         <v>367</v>
       </c>
       <c r="J163" s="39">
@@ -10079,38 +10547,38 @@
         <v>0.75880000000000003</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="53">
         <v>9482705</v>
       </c>
       <c r="B164" s="82">
         <v>45035</v>
       </c>
-      <c r="C164" s="170" t="s">
+      <c r="C164" s="39" t="s">
         <v>389</v>
       </c>
-      <c r="D164" s="170">
+      <c r="D164" s="39">
         <v>3.0000000000000001E-5</v>
       </c>
-      <c r="E164" s="170" t="s">
-        <v>5</v>
-      </c>
-      <c r="F164" s="170">
-        <v>128</v>
-      </c>
-      <c r="G164" s="170">
-        <v>1</v>
-      </c>
-      <c r="H164" s="171">
+      <c r="E164" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F164" s="39">
+        <v>128</v>
+      </c>
+      <c r="G164" s="39">
+        <v>1</v>
+      </c>
+      <c r="H164" s="53">
         <v>50</v>
       </c>
-      <c r="I164" s="172" t="s">
+      <c r="I164" s="99" t="s">
         <v>367</v>
       </c>
       <c r="J164" s="39">
         <v>160</v>
       </c>
-      <c r="K164" s="11">
+      <c r="K164" s="153">
         <v>0.91720000000000002</v>
       </c>
     </row>
@@ -10121,27 +10589,720 @@
       <c r="B165" s="82">
         <v>45035</v>
       </c>
-      <c r="C165" s="170" t="s">
+      <c r="C165" s="39" t="s">
         <v>389</v>
       </c>
-      <c r="D165" s="170">
+      <c r="D165" s="39">
         <v>1E-4</v>
       </c>
-      <c r="E165" s="170" t="s">
-        <v>5</v>
-      </c>
-      <c r="F165" s="170">
-        <v>128</v>
-      </c>
-      <c r="G165" s="170">
-        <v>1</v>
-      </c>
-      <c r="H165" s="171">
+      <c r="E165" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F165" s="39">
+        <v>128</v>
+      </c>
+      <c r="G165" s="39">
+        <v>1</v>
+      </c>
+      <c r="H165" s="53">
         <v>50</v>
       </c>
-      <c r="I165" s="172" t="s">
+      <c r="I165" s="99" t="s">
         <v>367</v>
       </c>
+      <c r="J165" s="39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="53">
+        <v>9506545</v>
+      </c>
+      <c r="B166" s="82">
+        <v>45040</v>
+      </c>
+      <c r="C166" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="D166" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E166" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F166" s="39">
+        <v>128</v>
+      </c>
+      <c r="G166" s="39">
+        <v>1</v>
+      </c>
+      <c r="H166" s="53">
+        <v>50</v>
+      </c>
+      <c r="I166" s="99" t="s">
+        <v>394</v>
+      </c>
+      <c r="J166" s="39">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="53">
+        <v>9506546</v>
+      </c>
+      <c r="B167" s="82">
+        <v>45040</v>
+      </c>
+      <c r="C167" s="39" t="s">
+        <v>395</v>
+      </c>
+      <c r="D167" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E167" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F167" s="39">
+        <v>128</v>
+      </c>
+      <c r="G167" s="39">
+        <v>1</v>
+      </c>
+      <c r="H167" s="53">
+        <v>50</v>
+      </c>
+      <c r="I167" s="99" t="s">
+        <v>394</v>
+      </c>
+      <c r="J167" s="39">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="53">
+        <v>9506547</v>
+      </c>
+      <c r="B168" s="82">
+        <v>45040</v>
+      </c>
+      <c r="C168" s="39" t="s">
+        <v>396</v>
+      </c>
+      <c r="D168" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E168" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F168" s="39">
+        <v>128</v>
+      </c>
+      <c r="G168" s="39">
+        <v>1</v>
+      </c>
+      <c r="H168" s="53">
+        <v>50</v>
+      </c>
+      <c r="I168" s="99" t="s">
+        <v>394</v>
+      </c>
+      <c r="J168" s="39">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="53">
+        <v>9497709</v>
+      </c>
+      <c r="B169" s="82">
+        <v>45038</v>
+      </c>
+      <c r="C169" s="39" t="s">
+        <v>408</v>
+      </c>
+      <c r="D169" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E169" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F169" s="39">
+        <v>128</v>
+      </c>
+      <c r="G169" s="39">
+        <v>1</v>
+      </c>
+      <c r="H169" s="53">
+        <v>50</v>
+      </c>
+      <c r="I169" s="99" t="s">
+        <v>414</v>
+      </c>
+      <c r="J169" s="39">
+        <v>198</v>
+      </c>
+      <c r="K169" s="153">
+        <v>0.77910000000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="53">
+        <v>9497710</v>
+      </c>
+      <c r="B170" s="82">
+        <v>45038</v>
+      </c>
+      <c r="C170" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="D170" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E170" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F170" s="39">
+        <v>128</v>
+      </c>
+      <c r="G170" s="39">
+        <v>1</v>
+      </c>
+      <c r="H170" s="53">
+        <v>50</v>
+      </c>
+      <c r="I170" s="99" t="s">
+        <v>414</v>
+      </c>
+      <c r="J170" s="39">
+        <v>199</v>
+      </c>
+      <c r="K170" s="153">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="53">
+        <v>9497711</v>
+      </c>
+      <c r="B171" s="82">
+        <v>45038</v>
+      </c>
+      <c r="C171" s="39" t="s">
+        <v>410</v>
+      </c>
+      <c r="D171" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E171" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F171" s="39">
+        <v>128</v>
+      </c>
+      <c r="G171" s="39">
+        <v>1</v>
+      </c>
+      <c r="H171" s="53">
+        <v>50</v>
+      </c>
+      <c r="I171" s="99" t="s">
+        <v>414</v>
+      </c>
+      <c r="J171" s="39">
+        <v>199</v>
+      </c>
+      <c r="K171" s="153">
+        <v>0.92800000000000005</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="53">
+        <v>9497672</v>
+      </c>
+      <c r="B172" s="82">
+        <v>45038</v>
+      </c>
+      <c r="C172" s="39" t="s">
+        <v>411</v>
+      </c>
+      <c r="D172" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E172" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F172" s="39">
+        <v>128</v>
+      </c>
+      <c r="G172" s="39">
+        <v>1</v>
+      </c>
+      <c r="H172" s="53">
+        <v>50</v>
+      </c>
+      <c r="I172" s="99" t="s">
+        <v>415</v>
+      </c>
+      <c r="J172" s="39">
+        <v>197</v>
+      </c>
+      <c r="K172" s="153">
+        <v>0.79610000000000003</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="53">
+        <v>9497693</v>
+      </c>
+      <c r="B173" s="82">
+        <v>45038</v>
+      </c>
+      <c r="C173" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="D173" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E173" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F173" s="39">
+        <v>128</v>
+      </c>
+      <c r="G173" s="39">
+        <v>1</v>
+      </c>
+      <c r="H173" s="53">
+        <v>50</v>
+      </c>
+      <c r="I173" s="99" t="s">
+        <v>415</v>
+      </c>
+      <c r="J173" s="39">
+        <v>195</v>
+      </c>
+      <c r="K173" s="153">
+        <v>0.79710000000000003</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="53">
+        <v>9497694</v>
+      </c>
+      <c r="B174" s="82">
+        <v>45038</v>
+      </c>
+      <c r="C174" s="39" t="s">
+        <v>413</v>
+      </c>
+      <c r="D174" s="39">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="E174" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F174" s="39">
+        <v>128</v>
+      </c>
+      <c r="G174" s="39">
+        <v>1</v>
+      </c>
+      <c r="H174" s="53">
+        <v>50</v>
+      </c>
+      <c r="I174" s="99" t="s">
+        <v>415</v>
+      </c>
+      <c r="J174" s="39">
+        <v>188</v>
+      </c>
+      <c r="K174" s="153">
+        <v>0.96220000000000006</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="149">
+        <v>9509053</v>
+      </c>
+      <c r="B175" s="93">
+        <v>45038</v>
+      </c>
+      <c r="C175" s="94" t="s">
+        <v>421</v>
+      </c>
+      <c r="D175" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E175" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F175" s="94">
+        <v>128</v>
+      </c>
+      <c r="G175" s="94">
+        <v>1</v>
+      </c>
+      <c r="H175" s="149">
+        <v>50</v>
+      </c>
+      <c r="I175" s="120" t="s">
+        <v>428</v>
+      </c>
+      <c r="J175" s="94">
+        <v>66</v>
+      </c>
+      <c r="K175" s="95">
+        <v>0.61170000000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="149">
+        <v>9509051</v>
+      </c>
+      <c r="B176" s="93">
+        <v>45038</v>
+      </c>
+      <c r="C176" s="94" t="s">
+        <v>422</v>
+      </c>
+      <c r="D176" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E176" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F176" s="94">
+        <v>128</v>
+      </c>
+      <c r="G176" s="94">
+        <v>1</v>
+      </c>
+      <c r="H176" s="149">
+        <v>50</v>
+      </c>
+      <c r="I176" s="120" t="s">
+        <v>428</v>
+      </c>
+      <c r="J176" s="94">
+        <v>71</v>
+      </c>
+      <c r="K176" s="95">
+        <v>0.64129999999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="149">
+        <v>9509049</v>
+      </c>
+      <c r="B177" s="93">
+        <v>45038</v>
+      </c>
+      <c r="C177" s="94" t="s">
+        <v>423</v>
+      </c>
+      <c r="D177" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E177" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F177" s="94">
+        <v>128</v>
+      </c>
+      <c r="G177" s="94">
+        <v>1</v>
+      </c>
+      <c r="H177" s="149">
+        <v>50</v>
+      </c>
+      <c r="I177" s="120" t="s">
+        <v>428</v>
+      </c>
+      <c r="J177" s="94">
+        <v>72</v>
+      </c>
+      <c r="K177" s="95">
+        <v>0.87419999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="149">
+        <v>9509435</v>
+      </c>
+      <c r="B178" s="93">
+        <v>45042</v>
+      </c>
+      <c r="C178" s="94" t="s">
+        <v>424</v>
+      </c>
+      <c r="D178" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E178" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F178" s="94">
+        <v>128</v>
+      </c>
+      <c r="G178" s="94">
+        <v>1</v>
+      </c>
+      <c r="H178" s="149">
+        <v>50</v>
+      </c>
+      <c r="I178" s="120" t="s">
+        <v>427</v>
+      </c>
+      <c r="J178" s="94">
+        <v>60</v>
+      </c>
+      <c r="K178" s="95">
+        <v>0.64290000000000003</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="149">
+        <v>9509436</v>
+      </c>
+      <c r="B179" s="93">
+        <v>45042</v>
+      </c>
+      <c r="C179" s="94" t="s">
+        <v>425</v>
+      </c>
+      <c r="D179" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E179" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F179" s="94">
+        <v>128</v>
+      </c>
+      <c r="G179" s="94">
+        <v>1</v>
+      </c>
+      <c r="H179" s="149">
+        <v>50</v>
+      </c>
+      <c r="I179" s="120" t="s">
+        <v>427</v>
+      </c>
+      <c r="J179" s="94">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="149">
+        <v>9509437</v>
+      </c>
+      <c r="B180" s="93">
+        <v>45042</v>
+      </c>
+      <c r="C180" s="94" t="s">
+        <v>426</v>
+      </c>
+      <c r="D180" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E180" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F180" s="94">
+        <v>128</v>
+      </c>
+      <c r="G180" s="94">
+        <v>1</v>
+      </c>
+      <c r="H180" s="149">
+        <v>50</v>
+      </c>
+      <c r="I180" s="120" t="s">
+        <v>427</v>
+      </c>
+      <c r="J180" s="94">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="149">
+        <v>9510554</v>
+      </c>
+      <c r="B181" s="93">
+        <v>45042</v>
+      </c>
+      <c r="C181" s="94" t="s">
+        <v>417</v>
+      </c>
+      <c r="D181" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E181" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F181" s="94">
+        <v>128</v>
+      </c>
+      <c r="G181" s="94">
+        <v>1</v>
+      </c>
+      <c r="H181" s="149">
+        <v>50</v>
+      </c>
+      <c r="I181" s="120" t="s">
+        <v>420</v>
+      </c>
+      <c r="J181" s="94">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="149">
+        <v>9510555</v>
+      </c>
+      <c r="B182" s="93">
+        <v>45042</v>
+      </c>
+      <c r="C182" s="94" t="s">
+        <v>418</v>
+      </c>
+      <c r="D182" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E182" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F182" s="94">
+        <v>128</v>
+      </c>
+      <c r="G182" s="94">
+        <v>1</v>
+      </c>
+      <c r="H182" s="149">
+        <v>50</v>
+      </c>
+      <c r="I182" s="120" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="149">
+        <v>9510556</v>
+      </c>
+      <c r="B183" s="93">
+        <v>45042</v>
+      </c>
+      <c r="C183" s="94" t="s">
+        <v>419</v>
+      </c>
+      <c r="D183" s="94">
+        <v>1E-4</v>
+      </c>
+      <c r="E183" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="F183" s="94">
+        <v>128</v>
+      </c>
+      <c r="G183" s="94">
+        <v>1</v>
+      </c>
+      <c r="H183" s="149">
+        <v>50</v>
+      </c>
+      <c r="I183" s="120" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" s="164" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="165">
+        <v>9512321</v>
+      </c>
+      <c r="B184" s="167">
+        <v>45043</v>
+      </c>
+      <c r="C184" s="164" t="s">
+        <v>429</v>
+      </c>
+      <c r="D184" s="164">
+        <v>1E-4</v>
+      </c>
+      <c r="E184" s="164" t="s">
+        <v>5</v>
+      </c>
+      <c r="F184" s="164">
+        <v>128</v>
+      </c>
+      <c r="G184" s="164">
+        <v>1</v>
+      </c>
+      <c r="H184" s="165">
+        <v>50</v>
+      </c>
+      <c r="I184" s="166" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" s="164" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="165">
+        <v>9512322</v>
+      </c>
+      <c r="B185" s="167">
+        <v>45043</v>
+      </c>
+      <c r="C185" s="164" t="s">
+        <v>430</v>
+      </c>
+      <c r="D185" s="164">
+        <v>1E-4</v>
+      </c>
+      <c r="E185" s="164" t="s">
+        <v>5</v>
+      </c>
+      <c r="F185" s="164">
+        <v>128</v>
+      </c>
+      <c r="G185" s="164">
+        <v>1</v>
+      </c>
+      <c r="H185" s="165">
+        <v>50</v>
+      </c>
+      <c r="I185" s="166" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" s="164" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="165">
+        <v>9512323</v>
+      </c>
+      <c r="B186" s="167">
+        <v>45043</v>
+      </c>
+      <c r="C186" s="164" t="s">
+        <v>431</v>
+      </c>
+      <c r="D186" s="164">
+        <v>1E-4</v>
+      </c>
+      <c r="E186" s="164" t="s">
+        <v>5</v>
+      </c>
+      <c r="F186" s="164">
+        <v>128</v>
+      </c>
+      <c r="G186" s="164">
+        <v>1</v>
+      </c>
+      <c r="H186" s="165">
+        <v>50</v>
+      </c>
+      <c r="I186" s="166" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="1048576" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B1048576" s="167"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12313,8 +13474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ED3A1D-2BE0-0249-BD3E-EFC2CB07D0F3}">
   <dimension ref="A1:AH1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14874,8 +16035,8 @@
       <c r="J111" s="54"/>
       <c r="K111" s="54"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A112" s="6">
+    <row r="112" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="54">
         <v>9487306</v>
       </c>
       <c r="B112" s="143">
@@ -14891,10 +16052,15 @@
         <v>5</v>
       </c>
       <c r="F112" s="54"/>
-      <c r="G112" s="39"/>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="6">
+      <c r="G112" s="39">
+        <v>39</v>
+      </c>
+      <c r="I112" s="99"/>
+      <c r="J112" s="54"/>
+      <c r="K112" s="54"/>
+    </row>
+    <row r="113" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="54">
         <v>9487307</v>
       </c>
       <c r="B113" s="143">
@@ -14910,7 +16076,101 @@
         <v>5</v>
       </c>
       <c r="F113" s="54"/>
-      <c r="G113" s="39"/>
+      <c r="G113" s="39">
+        <v>44</v>
+      </c>
+      <c r="I113" s="99"/>
+      <c r="J113" s="54"/>
+      <c r="K113" s="54"/>
+    </row>
+    <row r="114" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="118">
+        <v>9494453</v>
+      </c>
+      <c r="B114" s="119">
+        <v>45037</v>
+      </c>
+      <c r="C114" s="120" t="s">
+        <v>400</v>
+      </c>
+      <c r="D114" s="118">
+        <v>30</v>
+      </c>
+      <c r="E114" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F114" s="118"/>
+      <c r="G114" s="94">
+        <v>9</v>
+      </c>
+      <c r="I114" s="120"/>
+      <c r="J114" s="118"/>
+      <c r="K114" s="118"/>
+    </row>
+    <row r="115" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="118">
+        <v>9494478</v>
+      </c>
+      <c r="B115" s="119">
+        <v>45037</v>
+      </c>
+      <c r="C115" s="120" t="s">
+        <v>401</v>
+      </c>
+      <c r="D115" s="118">
+        <v>30</v>
+      </c>
+      <c r="E115" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F115" s="118"/>
+      <c r="G115" s="94">
+        <v>9</v>
+      </c>
+      <c r="I115" s="120"/>
+      <c r="J115" s="118"/>
+      <c r="K115" s="118"/>
+    </row>
+    <row r="116" spans="1:11" s="94" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="118">
+        <v>9494479</v>
+      </c>
+      <c r="B116" s="119">
+        <v>45037</v>
+      </c>
+      <c r="C116" s="120" t="s">
+        <v>416</v>
+      </c>
+      <c r="D116" s="118">
+        <v>30</v>
+      </c>
+      <c r="E116" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" s="118"/>
+      <c r="G116" s="94">
+        <v>19</v>
+      </c>
+      <c r="I116" s="120"/>
+      <c r="J116" s="118"/>
+      <c r="K116" s="118"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A117" s="6">
+        <v>9512344</v>
+      </c>
+      <c r="B117" s="73">
+        <v>45043</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="D117" s="6">
+        <v>30</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="1048574" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1048574" s="73"/>

</xml_diff>